<commit_message>
changing clock for it to stop
</commit_message>
<xml_diff>
--- a/data/Power_plants.xlsx
+++ b/data/Power_plants.xlsx
@@ -8,25 +8,38 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isanchezjimene\Documents\TraderesCode\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA813F88-DA01-428E-98D1-888B88B244E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36589534-77A8-432B-9C2B-691C23ADBC5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
     <sheet name="backup" sheetId="1" r:id="rId2"/>
     <sheet name="powerplants" sheetId="3" r:id="rId3"/>
-    <sheet name="dummy" sheetId="2" r:id="rId4"/>
+    <sheet name="germany2019" sheetId="5" r:id="rId4"/>
+    <sheet name="dummy" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId5"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="37">
   <si>
     <t>Technology</t>
   </si>
@@ -105,6 +118,39 @@
   <si>
     <t>Average of Age</t>
   </si>
+  <si>
+    <t>other res</t>
+  </si>
+  <si>
+    <t>opex</t>
+  </si>
+  <si>
+    <t>biogas</t>
+  </si>
+  <si>
+    <t>river</t>
+  </si>
+  <si>
+    <t>comments</t>
+  </si>
+  <si>
+    <t>fit</t>
+  </si>
+  <si>
+    <t># oil, other fossil fuels, mixed fossil fuels</t>
+  </si>
+  <si>
+    <t>natural gas</t>
+  </si>
+  <si>
+    <t>gasTurbine</t>
+  </si>
+  <si>
+    <t>#gasCC</t>
+  </si>
+  <si>
+    <t>HARD_COAL</t>
+  </si>
 </sst>
 </file>
 
@@ -113,7 +159,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +179,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF6897BB"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF629755"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF6A8759"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -142,7 +208,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -165,11 +231,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -181,6 +256,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2967,7 +3057,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2F2A88F4-60AA-4E67-A537-DC2C51174147}" name="PivotTable1" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{2F2A88F4-60AA-4E67-A537-DC2C51174147}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:D15" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField axis="axisRow" showAll="0">
@@ -3362,7 +3452,7 @@
       <selection activeCell="D14" sqref="A4:D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="28.1796875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.26953125" bestFit="1" customWidth="1"/>
@@ -3370,7 +3460,7 @@
     <col min="4" max="4" width="13.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -3384,7 +3474,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
@@ -3398,7 +3488,7 @@
         <v>20.333333333333332</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
         <v>10</v>
       </c>
@@ -3412,7 +3502,7 @@
         <v>28.205882352941178</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
@@ -3426,7 +3516,7 @@
         <v>31.09375</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4">
       <c r="A7" s="3" t="s">
         <v>18</v>
       </c>
@@ -3440,7 +3530,7 @@
         <v>36.705882352941174</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -3454,7 +3544,7 @@
         <v>56.971428571428568</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4">
       <c r="A9" s="3" t="s">
         <v>17</v>
       </c>
@@ -3468,7 +3558,7 @@
         <v>38.666666666666664</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4">
       <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
@@ -3482,7 +3572,7 @@
         <v>35.6</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -3496,7 +3586,7 @@
         <v>28.828571428571429</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4">
       <c r="A12" s="3" t="s">
         <v>16</v>
       </c>
@@ -3510,7 +3600,7 @@
         <v>10.5</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4">
       <c r="A13" s="3" t="s">
         <v>15</v>
       </c>
@@ -3524,7 +3614,7 @@
         <v>6.4545454545454541</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4">
       <c r="A14" s="3" t="s">
         <v>14</v>
       </c>
@@ -3538,7 +3628,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
@@ -3565,12 +3655,12 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="14.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3596,7 +3686,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -3625,7 +3715,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -3654,7 +3744,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -3683,7 +3773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3712,7 +3802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -3741,7 +3831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -3770,7 +3860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -3799,7 +3889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -3828,7 +3918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -3857,7 +3947,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -3886,7 +3976,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -3915,7 +4005,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -3944,7 +4034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -3973,7 +4063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -4002,7 +4092,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -4031,7 +4121,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -4060,7 +4150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -4089,7 +4179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -4118,7 +4208,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -4147,7 +4237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -4176,7 +4266,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -4205,7 +4295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -4234,7 +4324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -4263,7 +4353,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -4292,7 +4382,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -4321,7 +4411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -4350,7 +4440,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -4379,7 +4469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -4408,7 +4498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -4437,7 +4527,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -4466,7 +4556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -4495,7 +4585,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -4524,7 +4614,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -4553,7 +4643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -4582,7 +4672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -4611,7 +4701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -4640,7 +4730,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -4669,7 +4759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -4698,7 +4788,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -4727,7 +4817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -4756,7 +4846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -4785,7 +4875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -4814,7 +4904,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -4843,7 +4933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -4872,7 +4962,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -4901,7 +4991,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -4930,7 +5020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -4959,7 +5049,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -4988,7 +5078,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -5017,7 +5107,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -5046,7 +5136,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -5075,7 +5165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -5104,7 +5194,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -5133,7 +5223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -5162,7 +5252,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -5191,7 +5281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -5220,7 +5310,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -5249,7 +5339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -5278,7 +5368,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -5307,7 +5397,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -5336,7 +5426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -5365,7 +5455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -5394,7 +5484,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -5423,7 +5513,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -5452,7 +5542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -5481,7 +5571,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -5510,7 +5600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -5539,7 +5629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -5568,7 +5658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -5597,7 +5687,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -5626,7 +5716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -5655,7 +5745,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -5684,7 +5774,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -5713,7 +5803,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -5742,7 +5832,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -5771,7 +5861,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -5800,7 +5890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -5829,7 +5919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -5858,7 +5948,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -5887,7 +5977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -5916,7 +6006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -5945,7 +6035,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -5974,7 +6064,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -6003,7 +6093,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -6032,7 +6122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -6061,7 +6151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -6090,7 +6180,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -6119,7 +6209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -6148,7 +6238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -6177,7 +6267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -6206,7 +6296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:9">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -6235,7 +6325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -6264,7 +6354,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -6293,7 +6383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -6322,7 +6412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -6351,7 +6441,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -6380,7 +6470,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -6409,7 +6499,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -6438,7 +6528,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -6467,7 +6557,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -6496,7 +6586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:9">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -6525,7 +6615,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:9">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -6554,7 +6644,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -6583,7 +6673,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -6612,7 +6702,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -6641,7 +6731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -6670,7 +6760,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:9">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -6699,7 +6789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:9">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -6728,7 +6818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -6757,7 +6847,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:9">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -6786,7 +6876,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:9">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -6815,7 +6905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:9">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -6844,7 +6934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -6873,7 +6963,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:9">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -6902,7 +6992,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -6931,7 +7021,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -6960,7 +7050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -6989,7 +7079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:9">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -7018,7 +7108,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -7047,7 +7137,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -7076,7 +7166,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -7105,7 +7195,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:9">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -7134,7 +7224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:9">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -7163,7 +7253,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:9">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -7192,7 +7282,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:9">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -7221,7 +7311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:9">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -7250,7 +7340,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:9">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -7279,7 +7369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:9">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -7308,7 +7398,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:9">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -7337,7 +7427,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:9">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -7366,7 +7456,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:9">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -7395,7 +7485,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:9">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -7424,7 +7514,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:9">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -7453,7 +7543,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:9">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -7482,7 +7572,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:9">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -7511,7 +7601,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:9">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -7540,7 +7630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:9">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -7569,7 +7659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:9">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -7598,7 +7688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:9">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -7627,7 +7717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:9">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -7656,7 +7746,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:9">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -7685,7 +7775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:9">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -7714,7 +7804,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:9">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -7743,7 +7833,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:9">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -7772,7 +7862,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:9">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -7801,7 +7891,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:9">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -7830,7 +7920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:9">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -7859,7 +7949,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:9">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -7888,7 +7978,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:9">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -7917,7 +8007,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:9">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -7946,7 +8036,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:9">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -7975,7 +8065,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:9">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -8004,7 +8094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:9">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -8033,7 +8123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:9">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -8062,7 +8152,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:9">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -8091,7 +8181,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:9">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -8120,7 +8210,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:9">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -8149,7 +8239,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:9">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -8178,7 +8268,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:9">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -8207,7 +8297,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:9">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -8236,7 +8326,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:9">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -8265,7 +8355,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:9">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -8294,7 +8384,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:9">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -8323,7 +8413,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:9">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -8352,7 +8442,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:9">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -8381,7 +8471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:9">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -8410,7 +8500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:9">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -8439,7 +8529,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:9">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -8468,7 +8558,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:9">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -8497,7 +8587,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:9">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -8526,7 +8616,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:9">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -8555,7 +8645,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:9">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -8584,7 +8674,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:9">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -8613,7 +8703,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:9">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -8642,7 +8732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:9">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -8671,7 +8761,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:9">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -8700,7 +8790,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:9">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -8729,7 +8819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:9">
       <c r="A179" s="1">
         <v>177</v>
       </c>
@@ -8758,7 +8848,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:9">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -8787,7 +8877,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:9">
       <c r="A181" s="1">
         <v>179</v>
       </c>
@@ -8816,7 +8906,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:9">
       <c r="A182" s="1">
         <v>180</v>
       </c>
@@ -8845,7 +8935,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:9">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -8874,7 +8964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:9">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -8903,7 +8993,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:9">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -8932,7 +9022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:9">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -8961,7 +9051,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:9">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -8990,7 +9080,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:9">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -9019,7 +9109,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:9">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -9048,7 +9138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:9">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -9077,7 +9167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:9">
       <c r="A191" s="1">
         <v>189</v>
       </c>
@@ -9106,7 +9196,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:9">
       <c r="A192" s="1">
         <v>190</v>
       </c>
@@ -9135,7 +9225,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:9">
       <c r="A193" s="1">
         <v>191</v>
       </c>
@@ -9164,7 +9254,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:9">
       <c r="A194" s="1">
         <v>192</v>
       </c>
@@ -9193,7 +9283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="195" spans="1:9">
       <c r="A195" s="1">
         <v>193</v>
       </c>
@@ -9222,7 +9312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="196" spans="1:9">
       <c r="A196" s="1">
         <v>194</v>
       </c>
@@ -9251,7 +9341,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="197" spans="1:9">
       <c r="A197" s="1">
         <v>195</v>
       </c>
@@ -9280,7 +9370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="198" spans="1:9">
       <c r="A198" s="1">
         <v>196</v>
       </c>
@@ -9309,7 +9399,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="199" spans="1:9">
       <c r="A199" s="1">
         <v>197</v>
       </c>
@@ -9338,7 +9428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="200" spans="1:9">
       <c r="A200" s="1">
         <v>198</v>
       </c>
@@ -9367,7 +9457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="201" spans="1:9">
       <c r="A201" s="1">
         <v>199</v>
       </c>
@@ -9396,7 +9486,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="202" spans="1:9">
       <c r="A202" s="1">
         <v>200</v>
       </c>
@@ -9425,7 +9515,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="203" spans="1:9">
       <c r="A203" s="1">
         <v>201</v>
       </c>
@@ -9454,7 +9544,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="204" spans="1:9">
       <c r="A204" s="1">
         <v>202</v>
       </c>
@@ -9483,7 +9573,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="205" spans="1:9">
       <c r="A205" s="1">
         <v>203</v>
       </c>
@@ -9512,7 +9602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="206" spans="1:9">
       <c r="A206" s="1">
         <v>204</v>
       </c>
@@ -9541,7 +9631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="207" spans="1:9">
       <c r="A207" s="1">
         <v>205</v>
       </c>
@@ -9570,7 +9660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="208" spans="1:9">
       <c r="A208" s="1">
         <v>206</v>
       </c>
@@ -9599,7 +9689,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="209" spans="1:9">
       <c r="A209" s="1">
         <v>207</v>
       </c>
@@ -9628,7 +9718,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="210" spans="1:9">
       <c r="A210" s="1">
         <v>208</v>
       </c>
@@ -9657,7 +9747,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="211" spans="1:9">
       <c r="A211" s="1">
         <v>209</v>
       </c>
@@ -9686,7 +9776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="212" spans="1:9">
       <c r="A212" s="1">
         <v>210</v>
       </c>
@@ -9715,7 +9805,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="213" spans="1:9">
       <c r="A213" s="1">
         <v>211</v>
       </c>
@@ -9744,7 +9834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="214" spans="1:9">
       <c r="A214" s="1">
         <v>212</v>
       </c>
@@ -9773,7 +9863,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="215" spans="1:9">
       <c r="A215" s="1">
         <v>213</v>
       </c>
@@ -9802,7 +9892,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="216" spans="1:9">
       <c r="A216" s="1">
         <v>214</v>
       </c>
@@ -9831,7 +9921,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="217" spans="1:9">
       <c r="A217" s="1">
         <v>215</v>
       </c>
@@ -9860,7 +9950,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="218" spans="1:9">
       <c r="A218" s="1">
         <v>216</v>
       </c>
@@ -9889,7 +9979,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="219" spans="1:9">
       <c r="A219" s="1">
         <v>217</v>
       </c>
@@ -9918,7 +10008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:9">
       <c r="A220" s="1">
         <v>218</v>
       </c>
@@ -9947,7 +10037,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:9">
       <c r="A221" s="1">
         <v>219</v>
       </c>
@@ -9976,7 +10066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:9">
       <c r="A222" s="1">
         <v>220</v>
       </c>
@@ -10005,7 +10095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:9">
       <c r="A223" s="1">
         <v>221</v>
       </c>
@@ -10034,7 +10124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:9">
       <c r="A224" s="1">
         <v>222</v>
       </c>
@@ -10063,7 +10153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:9">
       <c r="A225" s="1">
         <v>223</v>
       </c>
@@ -10092,7 +10182,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:9">
       <c r="A226" s="1">
         <v>224</v>
       </c>
@@ -10121,7 +10211,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:9">
       <c r="A227" s="1">
         <v>225</v>
       </c>
@@ -10150,7 +10240,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:9">
       <c r="A228" s="1">
         <v>226</v>
       </c>
@@ -10179,7 +10269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:9">
       <c r="A229" s="1">
         <v>227</v>
       </c>
@@ -10208,7 +10298,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:9">
       <c r="A230" s="1">
         <v>228</v>
       </c>
@@ -10237,7 +10327,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:9">
       <c r="A231" s="1">
         <v>229</v>
       </c>
@@ -10266,7 +10356,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:9">
       <c r="A232" s="1">
         <v>230</v>
       </c>
@@ -10295,7 +10385,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:9">
       <c r="A233" s="1">
         <v>231</v>
       </c>
@@ -10324,7 +10414,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:9">
       <c r="A234" s="1">
         <v>232</v>
       </c>
@@ -10353,7 +10443,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:9">
       <c r="A235" s="1">
         <v>233</v>
       </c>
@@ -10382,7 +10472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:9">
       <c r="A236" s="1">
         <v>234</v>
       </c>
@@ -10411,7 +10501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:9">
       <c r="A237" s="1">
         <v>235</v>
       </c>
@@ -10440,7 +10530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:9">
       <c r="A238" s="1">
         <v>236</v>
       </c>
@@ -10469,7 +10559,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:9">
       <c r="A239" s="1">
         <v>237</v>
       </c>
@@ -10498,7 +10588,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:9">
       <c r="A240" s="1">
         <v>238</v>
       </c>
@@ -10527,7 +10617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:9">
       <c r="A241" s="1">
         <v>239</v>
       </c>
@@ -10556,7 +10646,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:9">
       <c r="A242" s="1">
         <v>240</v>
       </c>
@@ -10585,7 +10675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:9">
       <c r="A243" s="1">
         <v>241</v>
       </c>
@@ -10614,7 +10704,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:9">
       <c r="A244" s="1">
         <v>242</v>
       </c>
@@ -10643,7 +10733,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:9">
       <c r="A245" s="1">
         <v>243</v>
       </c>
@@ -10672,7 +10762,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:9">
       <c r="A246" s="1">
         <v>244</v>
       </c>
@@ -10701,7 +10791,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:9">
       <c r="A247" s="1">
         <v>245</v>
       </c>
@@ -10730,7 +10820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:9">
       <c r="A248" s="1">
         <v>246</v>
       </c>
@@ -10759,7 +10849,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:9">
       <c r="A249" s="1">
         <v>247</v>
       </c>
@@ -10788,7 +10878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:9">
       <c r="A250" s="1">
         <v>248</v>
       </c>
@@ -10817,7 +10907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:9">
       <c r="A251" s="1">
         <v>249</v>
       </c>
@@ -10846,7 +10936,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:9">
       <c r="A252" s="1">
         <v>250</v>
       </c>
@@ -10875,7 +10965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:9">
       <c r="A253" s="1">
         <v>251</v>
       </c>
@@ -10904,7 +10994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:9">
       <c r="A254" s="1">
         <v>252</v>
       </c>
@@ -10933,7 +11023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:9">
       <c r="A255" s="1">
         <v>253</v>
       </c>
@@ -10962,7 +11052,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:9">
       <c r="A256" s="1">
         <v>254</v>
       </c>
@@ -10991,7 +11081,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:9">
       <c r="A257" s="1">
         <v>255</v>
       </c>
@@ -11020,7 +11110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:9">
       <c r="A258" s="1">
         <v>256</v>
       </c>
@@ -11049,7 +11139,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:9">
       <c r="A259" s="1">
         <v>257</v>
       </c>
@@ -11078,7 +11168,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:9">
       <c r="A260" s="1">
         <v>258</v>
       </c>
@@ -11107,7 +11197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="261" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:9">
       <c r="A261" s="1">
         <v>259</v>
       </c>
@@ -11136,7 +11226,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="262" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:9">
       <c r="A262" s="1">
         <v>260</v>
       </c>
@@ -11165,7 +11255,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="263" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:9">
       <c r="A263" s="1">
         <v>261</v>
       </c>
@@ -11194,7 +11284,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="264" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:9">
       <c r="A264" s="1">
         <v>262</v>
       </c>
@@ -11223,7 +11313,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="265" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:9">
       <c r="A265" s="1">
         <v>263</v>
       </c>
@@ -11252,7 +11342,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="266" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:9">
       <c r="A266" s="1">
         <v>264</v>
       </c>
@@ -11281,7 +11371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="267" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:9">
       <c r="A267" s="1">
         <v>265</v>
       </c>
@@ -11310,7 +11400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="268" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:9">
       <c r="A268" s="1">
         <v>266</v>
       </c>
@@ -11339,7 +11429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="269" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:9">
       <c r="A269" s="1">
         <v>267</v>
       </c>
@@ -11368,7 +11458,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="270" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:9">
       <c r="A270" s="1">
         <v>268</v>
       </c>
@@ -11397,7 +11487,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="271" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:9">
       <c r="A271" s="1">
         <v>269</v>
       </c>
@@ -11426,7 +11516,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="272" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:9">
       <c r="A272" s="1">
         <v>270</v>
       </c>
@@ -11464,16 +11554,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88DF7B89-3137-4483-A2A9-559F907A912A}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10:H12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="A1:H12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="30.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11496,7 +11586,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -11522,7 +11612,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -11548,7 +11638,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -11574,7 +11664,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -11600,7 +11690,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -11626,7 +11716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -11652,7 +11742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -11678,7 +11768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -11704,7 +11794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -11730,7 +11820,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -11756,7 +11846,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -11789,6 +11879,452 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871B8469-CA4D-495B-9C72-1DE61BB7D586}">
+  <dimension ref="A1:P17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="2" width="30.08984375" customWidth="1"/>
+    <col min="8" max="8" width="16.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="6">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6">
+        <v>7908</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="O2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="6">
+        <v>8</v>
+      </c>
+      <c r="D3" s="6">
+        <v>22051</v>
+      </c>
+      <c r="E3" s="5"/>
+      <c r="F3" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="O3" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" s="1">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="6">
+        <v>8</v>
+      </c>
+      <c r="D4" s="6">
+        <v>3747</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="O4" s="10" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" s="1">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="6">
+        <v>8</v>
+      </c>
+      <c r="D5" s="6">
+        <v>8000</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6" s="1">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="6">
+        <v>8</v>
+      </c>
+      <c r="D6" s="6">
+        <v>18049</v>
+      </c>
+      <c r="E6" s="5"/>
+      <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7" s="1">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="6">
+        <v>8</v>
+      </c>
+      <c r="D7" s="7">
+        <v>9516</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="6">
+        <v>8</v>
+      </c>
+      <c r="D8" s="7">
+        <v>7820.6</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="O8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9" s="1">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="6">
+        <v>8</v>
+      </c>
+      <c r="D9" s="7">
+        <v>16062.2</v>
+      </c>
+      <c r="E9" s="5"/>
+      <c r="F9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="P9" s="10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10" s="1">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="6">
+        <v>8</v>
+      </c>
+      <c r="D10" s="6">
+        <f>197+806+1229 +4257 +8015</f>
+        <v>14504</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" t="s">
+        <v>8</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="P10" s="10" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="6">
+        <v>8</v>
+      </c>
+      <c r="D11" s="6">
+        <v>30932</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="O11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="6">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>471</v>
+      </c>
+      <c r="G12" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="6">
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <v>2328</v>
+      </c>
+      <c r="F13" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" t="s">
+        <v>8</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="6">
+        <v>8</v>
+      </c>
+      <c r="D14" s="6">
+        <f>12666 +14503 +13974 +5670 + 3804</f>
+        <v>50617</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" t="s">
+        <v>8</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="6">
+        <v>8</v>
+      </c>
+      <c r="D15" s="7">
+        <f>2108 + 79 +672</f>
+        <v>2859</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" t="s">
+        <v>8</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="6">
+        <v>8</v>
+      </c>
+      <c r="D16" s="7">
+        <v>4644</v>
+      </c>
+      <c r="E16" s="5"/>
+      <c r="F16" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" t="s">
+        <v>8</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="6">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>5317</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73D2471E-A65C-45D2-8906-9D7F22409E2C}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -11796,7 +12332,7 @@
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
prepared data for amiris example germany 2019
</commit_message>
<xml_diff>
--- a/data/Power_plants.xlsx
+++ b/data/Power_plants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isanchezjimene\Documents\TraderesCode\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE95D08-1F81-4320-82FA-D29563BF3B77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8595642-26F3-4515-84E6-0356A2B25925}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="4515" yWindow="-11535" windowWidth="19425" windowHeight="10425" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet4" sheetId="4" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="938" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="940" uniqueCount="37">
   <si>
     <t>Technology</t>
   </si>
@@ -128,9 +128,6 @@
     <t>biogas</t>
   </si>
   <si>
-    <t>river</t>
-  </si>
-  <si>
     <t>comments</t>
   </si>
   <si>
@@ -143,16 +140,16 @@
     <t>natural gas</t>
   </si>
   <si>
-    <t>gasTurbine</t>
-  </si>
-  <si>
-    <t>#gasCC</t>
-  </si>
-  <si>
     <t>HARD_COAL</t>
   </si>
   <si>
     <t>ProducerDE</t>
+  </si>
+  <si>
+    <t>Hydropower_ROR</t>
+  </si>
+  <si>
+    <t>Number</t>
   </si>
 </sst>
 </file>
@@ -185,13 +182,6 @@
     <font>
       <i/>
       <sz val="10"/>
-      <color rgb="FF6897BB"/>
-      <name val="JetBrains Mono"/>
-      <family val="3"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="10"/>
       <color rgb="FF629755"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
@@ -201,6 +191,12 @@
       <color rgb="FF6A8759"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -247,7 +243,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -259,21 +255,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3710,7 +3707,7 @@
         <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -3739,7 +3736,7 @@
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H3">
         <v>0</v>
@@ -3768,7 +3765,7 @@
         <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H4">
         <v>0</v>
@@ -3797,7 +3794,7 @@
         <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -3826,7 +3823,7 @@
         <v>7</v>
       </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -3855,7 +3852,7 @@
         <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -3884,7 +3881,7 @@
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -3913,7 +3910,7 @@
         <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -3942,7 +3939,7 @@
         <v>7</v>
       </c>
       <c r="G10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -3971,7 +3968,7 @@
         <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -4000,7 +3997,7 @@
         <v>7</v>
       </c>
       <c r="G12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H12">
         <v>0</v>
@@ -4029,7 +4026,7 @@
         <v>7</v>
       </c>
       <c r="G13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H13">
         <v>0</v>
@@ -4058,7 +4055,7 @@
         <v>7</v>
       </c>
       <c r="G14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -4087,7 +4084,7 @@
         <v>7</v>
       </c>
       <c r="G15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H15">
         <v>0</v>
@@ -4116,7 +4113,7 @@
         <v>7</v>
       </c>
       <c r="G16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -4145,7 +4142,7 @@
         <v>7</v>
       </c>
       <c r="G17" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H17">
         <v>0</v>
@@ -4174,7 +4171,7 @@
         <v>7</v>
       </c>
       <c r="G18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -4203,7 +4200,7 @@
         <v>7</v>
       </c>
       <c r="G19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -4232,7 +4229,7 @@
         <v>7</v>
       </c>
       <c r="G20" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -4261,7 +4258,7 @@
         <v>7</v>
       </c>
       <c r="G21" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H21">
         <v>0</v>
@@ -4290,7 +4287,7 @@
         <v>7</v>
       </c>
       <c r="G22" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H22">
         <v>0</v>
@@ -4319,7 +4316,7 @@
         <v>7</v>
       </c>
       <c r="G23" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -4348,7 +4345,7 @@
         <v>7</v>
       </c>
       <c r="G24" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -4377,7 +4374,7 @@
         <v>7</v>
       </c>
       <c r="G25" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H25">
         <v>0</v>
@@ -4406,7 +4403,7 @@
         <v>7</v>
       </c>
       <c r="G26" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -4435,7 +4432,7 @@
         <v>7</v>
       </c>
       <c r="G27" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -4464,7 +4461,7 @@
         <v>7</v>
       </c>
       <c r="G28" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H28">
         <v>0</v>
@@ -4493,7 +4490,7 @@
         <v>7</v>
       </c>
       <c r="G29" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H29">
         <v>0</v>
@@ -4522,7 +4519,7 @@
         <v>7</v>
       </c>
       <c r="G30" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H30">
         <v>0</v>
@@ -4551,7 +4548,7 @@
         <v>7</v>
       </c>
       <c r="G31" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -4580,7 +4577,7 @@
         <v>7</v>
       </c>
       <c r="G32" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H32">
         <v>0</v>
@@ -4609,7 +4606,7 @@
         <v>7</v>
       </c>
       <c r="G33" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H33">
         <v>0</v>
@@ -4638,7 +4635,7 @@
         <v>7</v>
       </c>
       <c r="G34" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H34">
         <v>0</v>
@@ -4667,7 +4664,7 @@
         <v>7</v>
       </c>
       <c r="G35" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -4696,7 +4693,7 @@
         <v>7</v>
       </c>
       <c r="G36" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -4725,7 +4722,7 @@
         <v>7</v>
       </c>
       <c r="G37" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H37">
         <v>0</v>
@@ -4754,7 +4751,7 @@
         <v>7</v>
       </c>
       <c r="G38" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H38">
         <v>0</v>
@@ -4783,7 +4780,7 @@
         <v>7</v>
       </c>
       <c r="G39" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H39">
         <v>0</v>
@@ -4812,7 +4809,7 @@
         <v>7</v>
       </c>
       <c r="G40" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H40">
         <v>0</v>
@@ -4841,7 +4838,7 @@
         <v>7</v>
       </c>
       <c r="G41" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -4870,7 +4867,7 @@
         <v>7</v>
       </c>
       <c r="G42" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H42">
         <v>0</v>
@@ -4899,7 +4896,7 @@
         <v>7</v>
       </c>
       <c r="G43" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -4928,7 +4925,7 @@
         <v>7</v>
       </c>
       <c r="G44" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H44">
         <v>0</v>
@@ -4957,7 +4954,7 @@
         <v>7</v>
       </c>
       <c r="G45" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H45">
         <v>0</v>
@@ -4986,7 +4983,7 @@
         <v>7</v>
       </c>
       <c r="G46" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H46">
         <v>0</v>
@@ -5015,7 +5012,7 @@
         <v>7</v>
       </c>
       <c r="G47" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H47">
         <v>0</v>
@@ -5044,7 +5041,7 @@
         <v>7</v>
       </c>
       <c r="G48" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H48">
         <v>0</v>
@@ -5073,7 +5070,7 @@
         <v>7</v>
       </c>
       <c r="G49" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H49">
         <v>0</v>
@@ -5102,7 +5099,7 @@
         <v>7</v>
       </c>
       <c r="G50" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H50">
         <v>0</v>
@@ -5131,7 +5128,7 @@
         <v>7</v>
       </c>
       <c r="G51" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H51">
         <v>0</v>
@@ -5160,7 +5157,7 @@
         <v>7</v>
       </c>
       <c r="G52" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H52">
         <v>0</v>
@@ -5189,7 +5186,7 @@
         <v>7</v>
       </c>
       <c r="G53" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H53">
         <v>0</v>
@@ -5218,7 +5215,7 @@
         <v>7</v>
       </c>
       <c r="G54" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H54">
         <v>0</v>
@@ -5247,7 +5244,7 @@
         <v>7</v>
       </c>
       <c r="G55" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H55">
         <v>0</v>
@@ -5276,7 +5273,7 @@
         <v>7</v>
       </c>
       <c r="G56" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H56">
         <v>0</v>
@@ -5305,7 +5302,7 @@
         <v>7</v>
       </c>
       <c r="G57" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H57">
         <v>0</v>
@@ -5334,7 +5331,7 @@
         <v>7</v>
       </c>
       <c r="G58" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H58">
         <v>0</v>
@@ -5363,7 +5360,7 @@
         <v>7</v>
       </c>
       <c r="G59" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H59">
         <v>0</v>
@@ -5392,7 +5389,7 @@
         <v>7</v>
       </c>
       <c r="G60" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H60">
         <v>0</v>
@@ -5421,7 +5418,7 @@
         <v>7</v>
       </c>
       <c r="G61" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H61">
         <v>0</v>
@@ -5450,7 +5447,7 @@
         <v>7</v>
       </c>
       <c r="G62" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H62">
         <v>0</v>
@@ -5479,7 +5476,7 @@
         <v>7</v>
       </c>
       <c r="G63" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H63">
         <v>0</v>
@@ -5508,7 +5505,7 @@
         <v>7</v>
       </c>
       <c r="G64" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H64">
         <v>0</v>
@@ -5537,7 +5534,7 @@
         <v>7</v>
       </c>
       <c r="G65" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H65">
         <v>0</v>
@@ -5566,7 +5563,7 @@
         <v>7</v>
       </c>
       <c r="G66" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H66">
         <v>0</v>
@@ -5595,7 +5592,7 @@
         <v>7</v>
       </c>
       <c r="G67" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H67">
         <v>0</v>
@@ -5624,7 +5621,7 @@
         <v>7</v>
       </c>
       <c r="G68" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H68">
         <v>0</v>
@@ -5653,7 +5650,7 @@
         <v>7</v>
       </c>
       <c r="G69" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H69">
         <v>0</v>
@@ -5682,7 +5679,7 @@
         <v>7</v>
       </c>
       <c r="G70" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H70">
         <v>0</v>
@@ -5711,7 +5708,7 @@
         <v>7</v>
       </c>
       <c r="G71" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H71">
         <v>0</v>
@@ -5740,7 +5737,7 @@
         <v>7</v>
       </c>
       <c r="G72" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H72">
         <v>0</v>
@@ -5769,7 +5766,7 @@
         <v>7</v>
       </c>
       <c r="G73" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H73">
         <v>0</v>
@@ -5798,7 +5795,7 @@
         <v>7</v>
       </c>
       <c r="G74" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H74">
         <v>0</v>
@@ -5827,7 +5824,7 @@
         <v>7</v>
       </c>
       <c r="G75" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H75">
         <v>0</v>
@@ -5856,7 +5853,7 @@
         <v>7</v>
       </c>
       <c r="G76" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H76">
         <v>0</v>
@@ -5885,7 +5882,7 @@
         <v>7</v>
       </c>
       <c r="G77" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H77">
         <v>0</v>
@@ -5914,7 +5911,7 @@
         <v>7</v>
       </c>
       <c r="G78" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H78">
         <v>0</v>
@@ -5943,7 +5940,7 @@
         <v>7</v>
       </c>
       <c r="G79" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H79">
         <v>0</v>
@@ -5972,7 +5969,7 @@
         <v>7</v>
       </c>
       <c r="G80" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H80">
         <v>0</v>
@@ -6001,7 +5998,7 @@
         <v>7</v>
       </c>
       <c r="G81" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H81">
         <v>0</v>
@@ -6030,7 +6027,7 @@
         <v>7</v>
       </c>
       <c r="G82" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H82">
         <v>0</v>
@@ -6059,7 +6056,7 @@
         <v>7</v>
       </c>
       <c r="G83" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H83">
         <v>0</v>
@@ -6088,7 +6085,7 @@
         <v>7</v>
       </c>
       <c r="G84" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H84">
         <v>0</v>
@@ -6117,7 +6114,7 @@
         <v>7</v>
       </c>
       <c r="G85" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H85">
         <v>0</v>
@@ -6146,7 +6143,7 @@
         <v>7</v>
       </c>
       <c r="G86" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H86">
         <v>0</v>
@@ -6175,7 +6172,7 @@
         <v>7</v>
       </c>
       <c r="G87" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H87">
         <v>0</v>
@@ -6204,7 +6201,7 @@
         <v>7</v>
       </c>
       <c r="G88" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H88">
         <v>0</v>
@@ -6233,7 +6230,7 @@
         <v>7</v>
       </c>
       <c r="G89" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H89">
         <v>0</v>
@@ -6262,7 +6259,7 @@
         <v>7</v>
       </c>
       <c r="G90" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H90">
         <v>0</v>
@@ -6291,7 +6288,7 @@
         <v>7</v>
       </c>
       <c r="G91" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H91">
         <v>0</v>
@@ -6320,7 +6317,7 @@
         <v>7</v>
       </c>
       <c r="G92" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H92">
         <v>0</v>
@@ -6349,7 +6346,7 @@
         <v>7</v>
       </c>
       <c r="G93" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H93">
         <v>0</v>
@@ -6378,7 +6375,7 @@
         <v>7</v>
       </c>
       <c r="G94" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H94">
         <v>0</v>
@@ -6407,7 +6404,7 @@
         <v>7</v>
       </c>
       <c r="G95" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H95">
         <v>0</v>
@@ -6436,7 +6433,7 @@
         <v>7</v>
       </c>
       <c r="G96" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H96">
         <v>0</v>
@@ -6465,7 +6462,7 @@
         <v>7</v>
       </c>
       <c r="G97" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H97">
         <v>0</v>
@@ -6494,7 +6491,7 @@
         <v>7</v>
       </c>
       <c r="G98" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H98">
         <v>0</v>
@@ -6523,7 +6520,7 @@
         <v>7</v>
       </c>
       <c r="G99" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H99">
         <v>0</v>
@@ -6552,7 +6549,7 @@
         <v>7</v>
       </c>
       <c r="G100" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H100">
         <v>0</v>
@@ -6581,7 +6578,7 @@
         <v>7</v>
       </c>
       <c r="G101" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H101">
         <v>0</v>
@@ -6610,7 +6607,7 @@
         <v>7</v>
       </c>
       <c r="G102" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H102">
         <v>0</v>
@@ -6639,7 +6636,7 @@
         <v>7</v>
       </c>
       <c r="G103" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H103">
         <v>0</v>
@@ -6668,7 +6665,7 @@
         <v>7</v>
       </c>
       <c r="G104" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H104">
         <v>0</v>
@@ -6697,7 +6694,7 @@
         <v>7</v>
       </c>
       <c r="G105" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H105">
         <v>0</v>
@@ -6726,7 +6723,7 @@
         <v>7</v>
       </c>
       <c r="G106" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H106">
         <v>0</v>
@@ -6755,7 +6752,7 @@
         <v>7</v>
       </c>
       <c r="G107" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H107">
         <v>0</v>
@@ -6784,7 +6781,7 @@
         <v>7</v>
       </c>
       <c r="G108" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H108">
         <v>0</v>
@@ -6813,7 +6810,7 @@
         <v>7</v>
       </c>
       <c r="G109" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H109">
         <v>0</v>
@@ -6842,7 +6839,7 @@
         <v>7</v>
       </c>
       <c r="G110" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H110">
         <v>0</v>
@@ -6871,7 +6868,7 @@
         <v>7</v>
       </c>
       <c r="G111" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H111">
         <v>0</v>
@@ -6900,7 +6897,7 @@
         <v>7</v>
       </c>
       <c r="G112" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H112">
         <v>0</v>
@@ -6929,7 +6926,7 @@
         <v>7</v>
       </c>
       <c r="G113" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H113">
         <v>0</v>
@@ -6958,7 +6955,7 @@
         <v>7</v>
       </c>
       <c r="G114" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H114">
         <v>0</v>
@@ -6987,7 +6984,7 @@
         <v>7</v>
       </c>
       <c r="G115" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H115">
         <v>0</v>
@@ -7016,7 +7013,7 @@
         <v>7</v>
       </c>
       <c r="G116" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H116">
         <v>0</v>
@@ -7045,7 +7042,7 @@
         <v>7</v>
       </c>
       <c r="G117" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H117">
         <v>0</v>
@@ -7074,7 +7071,7 @@
         <v>7</v>
       </c>
       <c r="G118" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H118">
         <v>0</v>
@@ -7103,7 +7100,7 @@
         <v>7</v>
       </c>
       <c r="G119" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H119">
         <v>0</v>
@@ -7132,7 +7129,7 @@
         <v>7</v>
       </c>
       <c r="G120" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H120">
         <v>0</v>
@@ -7161,7 +7158,7 @@
         <v>7</v>
       </c>
       <c r="G121" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H121">
         <v>0</v>
@@ -7190,7 +7187,7 @@
         <v>7</v>
       </c>
       <c r="G122" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H122">
         <v>0</v>
@@ -7219,7 +7216,7 @@
         <v>7</v>
       </c>
       <c r="G123" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H123">
         <v>0</v>
@@ -7248,7 +7245,7 @@
         <v>7</v>
       </c>
       <c r="G124" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H124">
         <v>0</v>
@@ -7277,7 +7274,7 @@
         <v>7</v>
       </c>
       <c r="G125" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H125">
         <v>0</v>
@@ -7306,7 +7303,7 @@
         <v>7</v>
       </c>
       <c r="G126" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H126">
         <v>0</v>
@@ -7335,7 +7332,7 @@
         <v>7</v>
       </c>
       <c r="G127" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H127">
         <v>0</v>
@@ -7364,7 +7361,7 @@
         <v>7</v>
       </c>
       <c r="G128" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H128">
         <v>0</v>
@@ -7393,7 +7390,7 @@
         <v>7</v>
       </c>
       <c r="G129" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H129">
         <v>0</v>
@@ -7422,7 +7419,7 @@
         <v>7</v>
       </c>
       <c r="G130" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H130">
         <v>0</v>
@@ -7451,7 +7448,7 @@
         <v>7</v>
       </c>
       <c r="G131" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H131">
         <v>0</v>
@@ -7480,7 +7477,7 @@
         <v>7</v>
       </c>
       <c r="G132" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H132">
         <v>0</v>
@@ -7509,7 +7506,7 @@
         <v>7</v>
       </c>
       <c r="G133" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H133">
         <v>0</v>
@@ -7538,7 +7535,7 @@
         <v>7</v>
       </c>
       <c r="G134" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H134">
         <v>0</v>
@@ -7567,7 +7564,7 @@
         <v>7</v>
       </c>
       <c r="G135" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H135">
         <v>0</v>
@@ -7596,7 +7593,7 @@
         <v>7</v>
       </c>
       <c r="G136" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H136">
         <v>0</v>
@@ -7625,7 +7622,7 @@
         <v>7</v>
       </c>
       <c r="G137" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H137">
         <v>0</v>
@@ -7654,7 +7651,7 @@
         <v>7</v>
       </c>
       <c r="G138" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H138">
         <v>0</v>
@@ -7683,7 +7680,7 @@
         <v>7</v>
       </c>
       <c r="G139" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H139">
         <v>0</v>
@@ -7712,7 +7709,7 @@
         <v>7</v>
       </c>
       <c r="G140" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H140">
         <v>0</v>
@@ -7741,7 +7738,7 @@
         <v>7</v>
       </c>
       <c r="G141" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H141">
         <v>0</v>
@@ -7770,7 +7767,7 @@
         <v>7</v>
       </c>
       <c r="G142" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H142">
         <v>0</v>
@@ -7799,7 +7796,7 @@
         <v>7</v>
       </c>
       <c r="G143" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H143">
         <v>0</v>
@@ -7828,7 +7825,7 @@
         <v>7</v>
       </c>
       <c r="G144" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H144">
         <v>0</v>
@@ -7857,7 +7854,7 @@
         <v>7</v>
       </c>
       <c r="G145" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H145">
         <v>0</v>
@@ -7886,7 +7883,7 @@
         <v>7</v>
       </c>
       <c r="G146" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H146">
         <v>0</v>
@@ -7915,7 +7912,7 @@
         <v>7</v>
       </c>
       <c r="G147" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H147">
         <v>0</v>
@@ -7944,7 +7941,7 @@
         <v>7</v>
       </c>
       <c r="G148" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H148">
         <v>0</v>
@@ -7973,7 +7970,7 @@
         <v>7</v>
       </c>
       <c r="G149" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H149">
         <v>0</v>
@@ -8002,7 +7999,7 @@
         <v>7</v>
       </c>
       <c r="G150" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H150">
         <v>0</v>
@@ -8031,7 +8028,7 @@
         <v>7</v>
       </c>
       <c r="G151" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H151">
         <v>0</v>
@@ -8060,7 +8057,7 @@
         <v>7</v>
       </c>
       <c r="G152" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H152">
         <v>0</v>
@@ -8089,7 +8086,7 @@
         <v>7</v>
       </c>
       <c r="G153" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H153">
         <v>0</v>
@@ -8118,7 +8115,7 @@
         <v>7</v>
       </c>
       <c r="G154" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H154">
         <v>0</v>
@@ -8147,7 +8144,7 @@
         <v>7</v>
       </c>
       <c r="G155" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H155">
         <v>0</v>
@@ -8176,7 +8173,7 @@
         <v>7</v>
       </c>
       <c r="G156" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H156">
         <v>0</v>
@@ -8205,7 +8202,7 @@
         <v>7</v>
       </c>
       <c r="G157" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H157">
         <v>0</v>
@@ -8234,7 +8231,7 @@
         <v>7</v>
       </c>
       <c r="G158" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H158">
         <v>0</v>
@@ -8263,7 +8260,7 @@
         <v>7</v>
       </c>
       <c r="G159" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H159">
         <v>0</v>
@@ -8292,7 +8289,7 @@
         <v>7</v>
       </c>
       <c r="G160" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H160">
         <v>0</v>
@@ -8321,7 +8318,7 @@
         <v>7</v>
       </c>
       <c r="G161" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H161">
         <v>0</v>
@@ -8350,7 +8347,7 @@
         <v>7</v>
       </c>
       <c r="G162" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H162">
         <v>0</v>
@@ -8379,7 +8376,7 @@
         <v>7</v>
       </c>
       <c r="G163" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H163">
         <v>0</v>
@@ -8408,7 +8405,7 @@
         <v>7</v>
       </c>
       <c r="G164" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H164">
         <v>0</v>
@@ -8437,7 +8434,7 @@
         <v>7</v>
       </c>
       <c r="G165" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H165">
         <v>0</v>
@@ -8466,7 +8463,7 @@
         <v>7</v>
       </c>
       <c r="G166" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H166">
         <v>0</v>
@@ -8495,7 +8492,7 @@
         <v>7</v>
       </c>
       <c r="G167" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H167">
         <v>0</v>
@@ -8524,7 +8521,7 @@
         <v>7</v>
       </c>
       <c r="G168" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H168">
         <v>0</v>
@@ -8553,7 +8550,7 @@
         <v>7</v>
       </c>
       <c r="G169" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H169">
         <v>0</v>
@@ -8582,7 +8579,7 @@
         <v>7</v>
       </c>
       <c r="G170" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H170">
         <v>0</v>
@@ -8611,7 +8608,7 @@
         <v>7</v>
       </c>
       <c r="G171" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H171">
         <v>0</v>
@@ -8640,7 +8637,7 @@
         <v>7</v>
       </c>
       <c r="G172" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H172">
         <v>0</v>
@@ -8669,7 +8666,7 @@
         <v>7</v>
       </c>
       <c r="G173" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H173">
         <v>0</v>
@@ -8698,7 +8695,7 @@
         <v>7</v>
       </c>
       <c r="G174" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H174">
         <v>0</v>
@@ -8727,7 +8724,7 @@
         <v>7</v>
       </c>
       <c r="G175" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H175">
         <v>0</v>
@@ -8756,7 +8753,7 @@
         <v>7</v>
       </c>
       <c r="G176" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H176">
         <v>0</v>
@@ -8785,7 +8782,7 @@
         <v>7</v>
       </c>
       <c r="G177" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H177">
         <v>0</v>
@@ -8814,7 +8811,7 @@
         <v>7</v>
       </c>
       <c r="G178" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H178">
         <v>0</v>
@@ -8843,7 +8840,7 @@
         <v>7</v>
       </c>
       <c r="G179" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H179">
         <v>0</v>
@@ -8872,7 +8869,7 @@
         <v>7</v>
       </c>
       <c r="G180" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H180">
         <v>0</v>
@@ -8901,7 +8898,7 @@
         <v>7</v>
       </c>
       <c r="G181" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H181">
         <v>0</v>
@@ -8930,7 +8927,7 @@
         <v>7</v>
       </c>
       <c r="G182" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H182">
         <v>0</v>
@@ -8959,7 +8956,7 @@
         <v>7</v>
       </c>
       <c r="G183" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H183">
         <v>0</v>
@@ -8988,7 +8985,7 @@
         <v>7</v>
       </c>
       <c r="G184" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H184">
         <v>0</v>
@@ -9017,7 +9014,7 @@
         <v>7</v>
       </c>
       <c r="G185" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H185">
         <v>0</v>
@@ -9046,7 +9043,7 @@
         <v>7</v>
       </c>
       <c r="G186" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H186">
         <v>0</v>
@@ -9075,7 +9072,7 @@
         <v>7</v>
       </c>
       <c r="G187" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H187">
         <v>0</v>
@@ -9104,7 +9101,7 @@
         <v>7</v>
       </c>
       <c r="G188" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H188">
         <v>0</v>
@@ -9133,7 +9130,7 @@
         <v>7</v>
       </c>
       <c r="G189" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H189">
         <v>0</v>
@@ -9162,7 +9159,7 @@
         <v>7</v>
       </c>
       <c r="G190" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H190">
         <v>0</v>
@@ -9191,7 +9188,7 @@
         <v>7</v>
       </c>
       <c r="G191" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H191">
         <v>0</v>
@@ -9220,7 +9217,7 @@
         <v>7</v>
       </c>
       <c r="G192" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H192">
         <v>0</v>
@@ -9249,7 +9246,7 @@
         <v>7</v>
       </c>
       <c r="G193" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H193">
         <v>0</v>
@@ -9278,7 +9275,7 @@
         <v>7</v>
       </c>
       <c r="G194" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H194">
         <v>0</v>
@@ -9307,7 +9304,7 @@
         <v>7</v>
       </c>
       <c r="G195" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H195">
         <v>0</v>
@@ -9336,7 +9333,7 @@
         <v>7</v>
       </c>
       <c r="G196" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H196">
         <v>0</v>
@@ -9365,7 +9362,7 @@
         <v>7</v>
       </c>
       <c r="G197" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H197">
         <v>0</v>
@@ -9394,7 +9391,7 @@
         <v>7</v>
       </c>
       <c r="G198" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H198">
         <v>0</v>
@@ -9423,7 +9420,7 @@
         <v>7</v>
       </c>
       <c r="G199" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H199">
         <v>0</v>
@@ -9452,7 +9449,7 @@
         <v>7</v>
       </c>
       <c r="G200" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H200">
         <v>0</v>
@@ -9481,7 +9478,7 @@
         <v>7</v>
       </c>
       <c r="G201" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H201">
         <v>0</v>
@@ -9510,7 +9507,7 @@
         <v>7</v>
       </c>
       <c r="G202" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H202">
         <v>0</v>
@@ -9539,7 +9536,7 @@
         <v>7</v>
       </c>
       <c r="G203" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H203">
         <v>0</v>
@@ -9568,7 +9565,7 @@
         <v>7</v>
       </c>
       <c r="G204" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H204">
         <v>0</v>
@@ -9597,7 +9594,7 @@
         <v>7</v>
       </c>
       <c r="G205" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H205">
         <v>0</v>
@@ -9626,7 +9623,7 @@
         <v>7</v>
       </c>
       <c r="G206" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H206">
         <v>0</v>
@@ -9655,7 +9652,7 @@
         <v>7</v>
       </c>
       <c r="G207" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H207">
         <v>0</v>
@@ -9684,7 +9681,7 @@
         <v>7</v>
       </c>
       <c r="G208" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H208">
         <v>0</v>
@@ -9713,7 +9710,7 @@
         <v>7</v>
       </c>
       <c r="G209" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H209">
         <v>0</v>
@@ -9742,7 +9739,7 @@
         <v>7</v>
       </c>
       <c r="G210" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H210">
         <v>0</v>
@@ -9771,7 +9768,7 @@
         <v>7</v>
       </c>
       <c r="G211" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H211">
         <v>0</v>
@@ -9800,7 +9797,7 @@
         <v>7</v>
       </c>
       <c r="G212" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H212">
         <v>0</v>
@@ -9829,7 +9826,7 @@
         <v>7</v>
       </c>
       <c r="G213" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H213">
         <v>0</v>
@@ -9858,7 +9855,7 @@
         <v>7</v>
       </c>
       <c r="G214" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H214">
         <v>0</v>
@@ -9887,7 +9884,7 @@
         <v>7</v>
       </c>
       <c r="G215" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H215">
         <v>0</v>
@@ -9916,7 +9913,7 @@
         <v>7</v>
       </c>
       <c r="G216" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H216">
         <v>0</v>
@@ -9945,7 +9942,7 @@
         <v>7</v>
       </c>
       <c r="G217" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H217">
         <v>0</v>
@@ -9974,7 +9971,7 @@
         <v>7</v>
       </c>
       <c r="G218" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H218">
         <v>0</v>
@@ -10003,7 +10000,7 @@
         <v>7</v>
       </c>
       <c r="G219" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H219">
         <v>0</v>
@@ -10032,7 +10029,7 @@
         <v>7</v>
       </c>
       <c r="G220" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H220">
         <v>0</v>
@@ -10061,7 +10058,7 @@
         <v>7</v>
       </c>
       <c r="G221" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H221">
         <v>0</v>
@@ -10090,7 +10087,7 @@
         <v>7</v>
       </c>
       <c r="G222" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H222">
         <v>0</v>
@@ -10119,7 +10116,7 @@
         <v>7</v>
       </c>
       <c r="G223" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H223">
         <v>0</v>
@@ -10148,7 +10145,7 @@
         <v>7</v>
       </c>
       <c r="G224" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H224">
         <v>0</v>
@@ -10177,7 +10174,7 @@
         <v>7</v>
       </c>
       <c r="G225" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H225">
         <v>0</v>
@@ -10206,7 +10203,7 @@
         <v>7</v>
       </c>
       <c r="G226" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H226">
         <v>0</v>
@@ -10235,7 +10232,7 @@
         <v>7</v>
       </c>
       <c r="G227" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H227">
         <v>0</v>
@@ -10264,7 +10261,7 @@
         <v>7</v>
       </c>
       <c r="G228" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H228">
         <v>0</v>
@@ -10293,7 +10290,7 @@
         <v>7</v>
       </c>
       <c r="G229" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H229">
         <v>0</v>
@@ -10322,7 +10319,7 @@
         <v>7</v>
       </c>
       <c r="G230" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H230">
         <v>0</v>
@@ -10351,7 +10348,7 @@
         <v>7</v>
       </c>
       <c r="G231" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H231">
         <v>0</v>
@@ -10380,7 +10377,7 @@
         <v>7</v>
       </c>
       <c r="G232" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H232">
         <v>0</v>
@@ -10409,7 +10406,7 @@
         <v>7</v>
       </c>
       <c r="G233" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H233">
         <v>0</v>
@@ -10438,7 +10435,7 @@
         <v>7</v>
       </c>
       <c r="G234" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H234">
         <v>0</v>
@@ -10467,7 +10464,7 @@
         <v>7</v>
       </c>
       <c r="G235" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H235">
         <v>0</v>
@@ -10496,7 +10493,7 @@
         <v>7</v>
       </c>
       <c r="G236" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H236">
         <v>0</v>
@@ -10525,7 +10522,7 @@
         <v>7</v>
       </c>
       <c r="G237" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H237">
         <v>0</v>
@@ -10554,7 +10551,7 @@
         <v>7</v>
       </c>
       <c r="G238" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H238">
         <v>0</v>
@@ -10583,7 +10580,7 @@
         <v>7</v>
       </c>
       <c r="G239" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H239">
         <v>0</v>
@@ -10612,7 +10609,7 @@
         <v>7</v>
       </c>
       <c r="G240" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H240">
         <v>0</v>
@@ -10641,7 +10638,7 @@
         <v>7</v>
       </c>
       <c r="G241" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H241">
         <v>0</v>
@@ -10670,7 +10667,7 @@
         <v>7</v>
       </c>
       <c r="G242" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H242">
         <v>0</v>
@@ -10699,7 +10696,7 @@
         <v>7</v>
       </c>
       <c r="G243" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H243">
         <v>0</v>
@@ -10728,7 +10725,7 @@
         <v>7</v>
       </c>
       <c r="G244" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H244">
         <v>0</v>
@@ -10757,7 +10754,7 @@
         <v>7</v>
       </c>
       <c r="G245" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H245">
         <v>0</v>
@@ -10786,7 +10783,7 @@
         <v>7</v>
       </c>
       <c r="G246" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H246">
         <v>0</v>
@@ -10815,7 +10812,7 @@
         <v>7</v>
       </c>
       <c r="G247" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H247">
         <v>0</v>
@@ -10844,7 +10841,7 @@
         <v>7</v>
       </c>
       <c r="G248" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H248">
         <v>0</v>
@@ -10873,7 +10870,7 @@
         <v>7</v>
       </c>
       <c r="G249" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H249">
         <v>0</v>
@@ -10902,7 +10899,7 @@
         <v>7</v>
       </c>
       <c r="G250" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H250">
         <v>0</v>
@@ -10931,7 +10928,7 @@
         <v>7</v>
       </c>
       <c r="G251" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H251">
         <v>0</v>
@@ -10960,7 +10957,7 @@
         <v>7</v>
       </c>
       <c r="G252" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H252">
         <v>0</v>
@@ -10989,7 +10986,7 @@
         <v>7</v>
       </c>
       <c r="G253" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H253">
         <v>0</v>
@@ -11018,7 +11015,7 @@
         <v>7</v>
       </c>
       <c r="G254" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H254">
         <v>0</v>
@@ -11047,7 +11044,7 @@
         <v>7</v>
       </c>
       <c r="G255" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H255">
         <v>0</v>
@@ -11076,7 +11073,7 @@
         <v>7</v>
       </c>
       <c r="G256" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H256">
         <v>0</v>
@@ -11105,7 +11102,7 @@
         <v>7</v>
       </c>
       <c r="G257" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H257">
         <v>0</v>
@@ -11134,7 +11131,7 @@
         <v>7</v>
       </c>
       <c r="G258" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H258">
         <v>0</v>
@@ -11163,7 +11160,7 @@
         <v>7</v>
       </c>
       <c r="G259" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H259">
         <v>0</v>
@@ -11192,7 +11189,7 @@
         <v>7</v>
       </c>
       <c r="G260" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H260">
         <v>0</v>
@@ -11221,7 +11218,7 @@
         <v>7</v>
       </c>
       <c r="G261" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H261">
         <v>0</v>
@@ -11250,7 +11247,7 @@
         <v>7</v>
       </c>
       <c r="G262" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H262">
         <v>0</v>
@@ -11279,7 +11276,7 @@
         <v>7</v>
       </c>
       <c r="G263" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H263">
         <v>0</v>
@@ -11308,7 +11305,7 @@
         <v>7</v>
       </c>
       <c r="G264" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H264">
         <v>0</v>
@@ -11337,7 +11334,7 @@
         <v>7</v>
       </c>
       <c r="G265" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H265">
         <v>0</v>
@@ -11366,7 +11363,7 @@
         <v>7</v>
       </c>
       <c r="G266" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H266">
         <v>0</v>
@@ -11395,7 +11392,7 @@
         <v>7</v>
       </c>
       <c r="G267" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H267">
         <v>0</v>
@@ -11424,7 +11421,7 @@
         <v>7</v>
       </c>
       <c r="G268" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H268">
         <v>0</v>
@@ -11453,7 +11450,7 @@
         <v>7</v>
       </c>
       <c r="G269" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H269">
         <v>0</v>
@@ -11482,7 +11479,7 @@
         <v>7</v>
       </c>
       <c r="G270" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H270">
         <v>0</v>
@@ -11511,7 +11508,7 @@
         <v>7</v>
       </c>
       <c r="G271" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H271">
         <v>0</v>
@@ -11540,7 +11537,7 @@
         <v>7</v>
       </c>
       <c r="G272" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H272">
         <v>0</v>
@@ -11558,7 +11555,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88DF7B89-3137-4483-A2A9-559F907A912A}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
@@ -11884,20 +11881,27 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871B8469-CA4D-495B-9C72-1DE61BB7D586}">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
     <col min="2" max="2" width="30.08984375" customWidth="1"/>
     <col min="7" max="7" width="17.7265625" customWidth="1"/>
-    <col min="8" max="8" width="16.36328125" customWidth="1"/>
+    <col min="8" max="8" width="13.26953125" customWidth="1"/>
+    <col min="9" max="10" width="5.08984375" customWidth="1"/>
+    <col min="11" max="11" width="10.08984375" customWidth="1"/>
+    <col min="12" max="12" width="13.6328125" customWidth="1"/>
+    <col min="13" max="14" width="5.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:26">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11919,14 +11923,15 @@
       <c r="H1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="M1" s="11"/>
+      <c r="N1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="O1" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:26">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -11939,12 +11944,12 @@
       <c r="D2" s="6">
         <v>7908</v>
       </c>
-      <c r="E2" s="5"/>
+      <c r="E2" s="12"/>
       <c r="F2" t="s">
         <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H2">
         <v>0</v>
@@ -11953,7 +11958,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:26">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -11966,21 +11971,26 @@
       <c r="D3" s="6">
         <v>22051</v>
       </c>
-      <c r="E3" s="5"/>
+      <c r="E3" s="12">
+        <v>0.4</v>
+      </c>
       <c r="F3" t="s">
         <v>7</v>
       </c>
       <c r="G3" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H3">
         <v>0</v>
       </c>
-      <c r="O3" s="11" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="N3">
+        <v>2.5</v>
+      </c>
+      <c r="O3" s="10" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -11993,21 +12003,26 @@
       <c r="D4" s="6">
         <v>3747</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="12">
+        <v>0.35</v>
+      </c>
       <c r="F4" t="s">
         <v>7</v>
       </c>
       <c r="G4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H4">
         <v>0</v>
       </c>
-      <c r="O4" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="N4">
+        <v>1.2</v>
+      </c>
+      <c r="O4" s="9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -12020,18 +12035,18 @@
       <c r="D5" s="6">
         <v>8000</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="E5" s="12"/>
       <c r="F5" t="s">
         <v>7</v>
       </c>
       <c r="G5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16">
+        <v>0.89</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -12044,18 +12059,23 @@
       <c r="D6" s="6">
         <v>18049</v>
       </c>
-      <c r="E6" s="5"/>
+      <c r="E6" s="12">
+        <v>0.35</v>
+      </c>
       <c r="F6" t="s">
         <v>7</v>
       </c>
       <c r="G6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H6">
-        <v>0.89</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -12065,21 +12085,26 @@
       <c r="C7" s="6">
         <v>8</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="6">
         <v>9516</v>
       </c>
-      <c r="E7" s="5"/>
+      <c r="E7" s="12">
+        <v>0.33</v>
+      </c>
       <c r="F7" t="s">
         <v>7</v>
       </c>
       <c r="G7" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="N7">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -12089,24 +12114,29 @@
       <c r="C8" s="6">
         <v>8</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="6">
         <v>7820.6</v>
       </c>
-      <c r="E8" s="5"/>
+      <c r="E8" s="12">
+        <v>0.4</v>
+      </c>
       <c r="F8" t="s">
         <v>7</v>
       </c>
       <c r="G8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H8">
         <v>0</v>
       </c>
+      <c r="N8">
+        <v>1.2</v>
+      </c>
       <c r="O8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -12116,24 +12146,27 @@
       <c r="C9" s="6">
         <v>8</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="6">
         <v>16062.2</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="E9" s="12">
+        <v>0.5</v>
+      </c>
       <c r="F9" t="s">
         <v>7</v>
       </c>
       <c r="G9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H9">
         <v>0</v>
       </c>
-      <c r="P9" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="N9">
+        <v>1.2</v>
+      </c>
+      <c r="P9" s="9"/>
+    </row>
+    <row r="10" spans="1:26">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -12147,21 +12180,19 @@
         <f>197+806+1229 +4257 +8015</f>
         <v>14504</v>
       </c>
-      <c r="E10" s="5"/>
+      <c r="E10" s="12"/>
       <c r="F10" t="s">
         <v>7</v>
       </c>
       <c r="G10" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H10">
         <v>0</v>
       </c>
-      <c r="P10" s="10" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="P10" s="9"/>
+    </row>
+    <row r="11" spans="1:26">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -12174,44 +12205,45 @@
       <c r="D11" s="6">
         <v>30932</v>
       </c>
-      <c r="E11" s="5"/>
+      <c r="E11" s="12"/>
       <c r="F11" t="s">
         <v>7</v>
       </c>
       <c r="G11" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H11">
         <v>0</v>
       </c>
       <c r="O11" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C12" s="6">
         <v>8</v>
       </c>
-      <c r="D12">
-        <v>471</v>
+      <c r="D12" s="6">
+        <v>2328</v>
+      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" t="s">
+        <v>7</v>
       </c>
       <c r="G12" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H12">
         <v>0</v>
       </c>
-      <c r="N12">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
+    </row>
+    <row r="13" spans="1:26">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -12221,45 +12253,47 @@
       <c r="C13" s="6">
         <v>8</v>
       </c>
-      <c r="D13">
-        <v>2328</v>
-      </c>
+      <c r="D13" s="6">
+        <f>12666 +14503 +13974 +5670 + 3804</f>
+        <v>50617</v>
+      </c>
+      <c r="E13" s="12"/>
       <c r="F13" t="s">
         <v>7</v>
       </c>
       <c r="G13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:26">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C14" s="6">
         <v>8</v>
       </c>
       <c r="D14" s="6">
-        <f>12666 +14503 +13974 +5670 + 3804</f>
-        <v>50617</v>
-      </c>
-      <c r="E14" s="5"/>
+        <f>2108 + 79 +672</f>
+        <v>2859</v>
+      </c>
+      <c r="E14" s="12"/>
       <c r="F14" t="s">
         <v>7</v>
       </c>
       <c r="G14" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H14">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:26">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -12269,58 +12303,66 @@
       <c r="C15" s="6">
         <v>8</v>
       </c>
-      <c r="D15" s="7">
-        <f>2108 + 79 +672</f>
-        <v>2859</v>
-      </c>
-      <c r="E15" s="5"/>
+      <c r="D15" s="6">
+        <v>4644</v>
+      </c>
+      <c r="E15" s="12"/>
       <c r="F15" t="s">
         <v>7</v>
       </c>
       <c r="G15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="N15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="O15" s="6">
+        <v>8</v>
+      </c>
+      <c r="P15" s="6">
+        <v>471</v>
+      </c>
+      <c r="R15" t="s">
+        <v>7</v>
+      </c>
+      <c r="S15" t="s">
+        <v>34</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="Z15">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26">
       <c r="A16" s="1">
         <v>14</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>15</v>
+      <c r="B16" s="8" t="s">
+        <v>35</v>
       </c>
       <c r="C16" s="6">
         <v>8</v>
       </c>
-      <c r="D16" s="7">
-        <v>4644</v>
-      </c>
-      <c r="E16" s="5"/>
+      <c r="D16" s="6">
+        <v>5317</v>
+      </c>
       <c r="F16" t="s">
         <v>7</v>
       </c>
       <c r="G16" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="H16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C17" s="6">
-        <v>8</v>
-      </c>
-      <c r="D17">
-        <v>5317</v>
-      </c>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>

<commit_message>
adding dummy RES scenario
</commit_message>
<xml_diff>
--- a/data/Power_plants.xlsx
+++ b/data/Power_plants.xlsx
@@ -8,20 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\isanchezjimene\Documents\TraderesCode\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5813530-B465-4B92-A542-EC2AF3DD3381}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39DB3D7-9A3B-42BB-A6E5-43F225058E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28815" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="extendedDE" sheetId="1" r:id="rId1"/>
     <sheet name="extendedNL" sheetId="6" r:id="rId2"/>
     <sheet name="powerplants_grouped" sheetId="3" r:id="rId3"/>
-    <sheet name="germany2019" sheetId="5" r:id="rId4"/>
-    <sheet name="Sheet4" sheetId="4" r:id="rId5"/>
+    <sheet name="groupedDE_RES" sheetId="8" r:id="rId4"/>
+    <sheet name="germany2019" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId7"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1176" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1235" uniqueCount="43">
   <si>
     <t>Technology</t>
   </si>
@@ -3492,7 +3493,7 @@
   <dimension ref="A1:J272"/>
   <sheetViews>
     <sheetView zoomScale="77" zoomScaleNormal="77" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -11624,8 +11625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E6B6640-7659-40BC-BB1F-545A343E7684}">
   <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView zoomScale="250" zoomScaleNormal="250" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:I1048576"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -13846,7 +13847,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -14208,11 +14209,549 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1842032F-786B-416F-9171-8FFE55F32C1D}">
+  <dimension ref="A1:I18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I27" sqref="I27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="2" width="14.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="12"/>
+      <c r="B1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" s="15" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="13">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="4">
+        <v>8</v>
+      </c>
+      <c r="D2" s="6">
+        <v>4644.4034000000001</v>
+      </c>
+      <c r="E2" s="5">
+        <v>0.35162268780797246</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="12">
+        <v>0</v>
+      </c>
+      <c r="I2" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="13">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="4">
+        <v>8</v>
+      </c>
+      <c r="D3" s="6">
+        <v>31358.328999999998</v>
+      </c>
+      <c r="E3" s="5">
+        <v>0.53826095601515933</v>
+      </c>
+      <c r="F3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H3" s="12">
+        <v>0</v>
+      </c>
+      <c r="I3" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="13">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="4">
+        <v>8</v>
+      </c>
+      <c r="D4" s="6">
+        <v>5000</v>
+      </c>
+      <c r="E4" s="5">
+        <v>1</v>
+      </c>
+      <c r="F4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="12">
+        <v>0</v>
+      </c>
+      <c r="I4" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="13">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="4">
+        <v>8</v>
+      </c>
+      <c r="D5" s="6">
+        <v>3652.9</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.35399077947121271</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="12">
+        <v>0</v>
+      </c>
+      <c r="I5" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="13">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="4">
+        <v>8</v>
+      </c>
+      <c r="D6" s="6">
+        <v>8858.7499999999982</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0.7811457116585705</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="12">
+        <v>0</v>
+      </c>
+      <c r="I6" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="13">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="4">
+        <v>8</v>
+      </c>
+      <c r="D7" s="6">
+        <v>20779.019999999997</v>
+      </c>
+      <c r="E7" s="5">
+        <v>0.36004079896582097</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="12">
+        <v>0</v>
+      </c>
+      <c r="I7" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="13">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="4">
+        <v>8</v>
+      </c>
+      <c r="D8" s="6">
+        <v>8599</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0.33</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H8" s="12">
+        <v>0</v>
+      </c>
+      <c r="I8" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="13">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="4">
+        <v>8</v>
+      </c>
+      <c r="D9" s="6">
+        <v>8194.3024999999998</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0.37414216973934089</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H9" s="12">
+        <v>0</v>
+      </c>
+      <c r="I9" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="13">
+        <v>8</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="4">
+        <v>8</v>
+      </c>
+      <c r="D10" s="6">
+        <v>53555.516075797081</v>
+      </c>
+      <c r="E10" s="5">
+        <v>1</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H10" s="12">
+        <v>0</v>
+      </c>
+      <c r="I10" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="13">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="4">
+        <v>8</v>
+      </c>
+      <c r="D11" s="6">
+        <v>10271.799999999999</v>
+      </c>
+      <c r="E11" s="5">
+        <v>1</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="12">
+        <v>0</v>
+      </c>
+      <c r="I11" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="13">
+        <v>10</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" s="4">
+        <v>8</v>
+      </c>
+      <c r="D12" s="6">
+        <v>20000</v>
+      </c>
+      <c r="E12" s="5">
+        <v>1</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="12">
+        <v>0</v>
+      </c>
+      <c r="I12" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="13">
+        <v>2</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="4">
+        <v>8</v>
+      </c>
+      <c r="D13" s="6">
+        <v>20000</v>
+      </c>
+      <c r="E13" s="5">
+        <v>1</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="12">
+        <v>0</v>
+      </c>
+      <c r="I13" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="13">
+        <v>2</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" s="4">
+        <v>8</v>
+      </c>
+      <c r="D14" s="6">
+        <v>20000</v>
+      </c>
+      <c r="E14" s="5">
+        <v>1</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H14" s="12">
+        <v>0</v>
+      </c>
+      <c r="I14" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="13">
+        <v>2</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" s="4">
+        <v>8</v>
+      </c>
+      <c r="D15" s="6">
+        <v>5000</v>
+      </c>
+      <c r="E15" s="5">
+        <v>1</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="12">
+        <v>0</v>
+      </c>
+      <c r="I15" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="13">
+        <v>2</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="4">
+        <v>8</v>
+      </c>
+      <c r="D16" s="6">
+        <v>5000</v>
+      </c>
+      <c r="E16" s="5">
+        <v>1</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="12">
+        <v>0</v>
+      </c>
+      <c r="I16" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9">
+      <c r="A17" s="13">
+        <v>2</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="4">
+        <v>8</v>
+      </c>
+      <c r="D17" s="6">
+        <v>5000</v>
+      </c>
+      <c r="E17" s="5">
+        <v>1</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="12">
+        <v>0</v>
+      </c>
+      <c r="I17" s="12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9">
+      <c r="A18" s="13">
+        <v>2</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="4">
+        <v>8</v>
+      </c>
+      <c r="D18" s="6">
+        <v>5000</v>
+      </c>
+      <c r="E18" s="5">
+        <v>1</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="12">
+        <v>0</v>
+      </c>
+      <c r="I18" s="12">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871B8469-CA4D-495B-9C72-1DE61BB7D586}">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -14659,7 +15198,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CE56270-BB9F-4A65-A808-F3AE5E04B4CD}">
   <dimension ref="A3:D15"/>
   <sheetViews>

</xml_diff>

<commit_message>
Testing capacity market to see next year demand
</commit_message>
<xml_diff>
--- a/data/Power_plants.xlsx
+++ b/data/Power_plants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96DBC084-4D47-4ED4-9B4C-8B937055AE1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8760742-4394-45A4-B9C6-EDAE747450D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-15" windowWidth="29040" windowHeight="15840" tabRatio="840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="9" r:id="rId1"/>
@@ -23170,8 +23170,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91B88372-FD70-4A88-9C48-DBF8E6D97E61}">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -23691,8 +23691,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCCA0DB4-82B5-4F45-9627-77778B586330}">
   <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
refactoring / cleaning code
</commit_message>
<xml_diff>
--- a/data/Power_plants.xlsx
+++ b/data/Power_plants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9069CFB3-4610-40C5-A047-CAC8D636237D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFDE20B5-F5FB-451C-8E93-DEACFF44AB6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12315" yWindow="-16350" windowWidth="29040" windowHeight="15840" tabRatio="971" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-16485" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="971" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="groupedNLGAS" sheetId="20" r:id="rId1"/>
@@ -44,7 +44,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="2" r:id="rId16"/>
+    <pivotCache cacheId="4" r:id="rId16"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -102,7 +102,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4389" uniqueCount="459">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4391" uniqueCount="460">
   <si>
     <t>Technology</t>
   </si>
@@ -1479,6 +1479,9 @@
   </si>
   <si>
     <t>index</t>
+  </si>
+  <si>
+    <t>&lt; this years are dummy, only to test</t>
   </si>
 </sst>
 </file>
@@ -2579,7 +2582,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8EBABEF3-7A12-4A97-8F01-EC0882F5F9E8}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8EBABEF3-7A12-4A97-8F01-EC0882F5F9E8}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="O1:P13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField axis="axisRow" showAll="0">
@@ -31401,7 +31404,7 @@
   <dimension ref="A1:L45"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -32868,7 +32871,7 @@
   </sheetPr>
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A31" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -34303,8 +34306,8 @@
   </sheetPr>
   <dimension ref="A1:P51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O16" sqref="O16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -34348,7 +34351,9 @@
       <c r="J1" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="K1" s="12"/>
+      <c r="K1" s="12" t="s">
+        <v>457</v>
+      </c>
       <c r="O1" s="2" t="s">
         <v>20</v>
       </c>
@@ -34426,7 +34431,12 @@
       <c r="J3" s="11">
         <v>0</v>
       </c>
-      <c r="K3" s="11"/>
+      <c r="K3" s="11">
+        <v>2020</v>
+      </c>
+      <c r="M3" t="s">
+        <v>459</v>
+      </c>
       <c r="O3" s="3" t="s">
         <v>439</v>
       </c>
@@ -34465,7 +34475,9 @@
       <c r="J4" s="11">
         <v>0</v>
       </c>
-      <c r="K4" s="11"/>
+      <c r="K4" s="11">
+        <v>2020</v>
+      </c>
       <c r="O4" s="3" t="s">
         <v>9</v>
       </c>
@@ -34504,7 +34516,9 @@
       <c r="J5" s="11">
         <v>0</v>
       </c>
-      <c r="K5" s="11"/>
+      <c r="K5" s="11">
+        <v>2024</v>
+      </c>
       <c r="O5" s="3" t="s">
         <v>42</v>
       </c>
@@ -36105,8 +36119,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB94089A-EE04-4A8F-A9CF-12445972E5C2}">
   <dimension ref="A1:O190"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
correcting iteration year for 0
</commit_message>
<xml_diff>
--- a/data/Power_plants.xlsx
+++ b/data/Power_plants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E92C08-85F0-4CE4-A076-5D4FB01004BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE55AFE4-6746-4724-839D-E699954736FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-14505" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="971" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="971" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="groupedNLGAS" sheetId="20" r:id="rId1"/>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4649" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4651" uniqueCount="472">
   <si>
     <t>Technology</t>
   </si>
@@ -1740,8 +1740,8 @@
     <xf numFmtId="1" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -2000,13 +2000,37 @@
       <sheetData sheetId="5" refreshError="1"/>
       <sheetData sheetId="6" refreshError="1"/>
       <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="8">
+        <row r="1">
+          <cell r="B1" t="str">
+            <v>Technology</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="9">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>traderes technology</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="10" refreshError="1"/>
       <sheetData sheetId="11" refreshError="1"/>
       <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="13">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>Name</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="14">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>Name</v>
+          </cell>
+        </row>
+      </sheetData>
       <sheetData sheetId="15" refreshError="1"/>
       <sheetData sheetId="16" refreshError="1"/>
       <sheetData sheetId="17" refreshError="1"/>
@@ -43961,10 +43985,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q20" sqref="P20:Q20"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -44109,7 +44133,7 @@
         <v>15</v>
       </c>
       <c r="C6">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D6" s="4">
         <v>4500</v>
@@ -44137,7 +44161,7 @@
         <v>15</v>
       </c>
       <c r="C7">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="D7" s="4">
         <v>4500</v>
@@ -44165,7 +44189,7 @@
         <v>15</v>
       </c>
       <c r="C8">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D8" s="4">
         <v>4500</v>
@@ -44179,7 +44203,7 @@
       <c r="G8">
         <v>0</v>
       </c>
-      <c r="I8" s="25">
+      <c r="I8" s="24">
         <f>SUM(D5:D10)</f>
         <v>25757</v>
       </c>
@@ -44196,7 +44220,7 @@
         <v>15</v>
       </c>
       <c r="C9">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D9" s="4">
         <v>3257</v>
@@ -44224,7 +44248,7 @@
         <v>15</v>
       </c>
       <c r="C10">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="D10" s="4">
         <v>4500</v>
@@ -44777,7 +44801,7 @@
       <c r="A32" s="1">
         <v>51</v>
       </c>
-      <c r="B32" s="24" t="s">
+      <c r="B32" s="25" t="s">
         <v>32</v>
       </c>
       <c r="C32">
@@ -44804,7 +44828,7 @@
         <v>434</v>
       </c>
       <c r="C33">
-        <v>20</v>
+        <v>1</v>
       </c>
       <c r="D33" s="4">
         <v>1700</v>
@@ -44817,6 +44841,29 @@
       </c>
       <c r="G33">
         <v>0.9</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="1">
+        <v>53</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" s="4">
+        <v>11000</v>
+      </c>
+      <c r="E34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
writing shedders files automatic  / change dispatch every year
</commit_message>
<xml_diff>
--- a/data/Power_plants.xlsx
+++ b/data/Power_plants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D8EF668-7E49-4729-87E4-A1641D12D21E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{412FE152-A9B0-4621-B6D2-91BA1354CC6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="971" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,7 +112,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4707" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4709" uniqueCount="472">
   <si>
     <t>Technology</t>
   </si>
@@ -1811,7 +1811,7 @@
       <sheetName val="NewTechnologies"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="2">
           <cell r="A2" t="str">
@@ -1839,7 +1839,7 @@
         </row>
         <row r="5">
           <cell r="A5" t="str">
-            <v>PV_commercial_systems</v>
+            <v>PV</v>
           </cell>
         </row>
         <row r="6">
@@ -2002,34 +2002,34 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -42354,8 +42354,8 @@
   </sheetPr>
   <dimension ref="A1:O51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E38" sqref="E38"/>
+    <sheetView topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -43971,8 +43971,8 @@
   </sheetPr>
   <dimension ref="A1:Q34"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView showRuler="0" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -44861,10 +44861,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:Q39"/>
+  <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -45163,7 +45163,7 @@
         <v>13</v>
       </c>
       <c r="D12" s="26">
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="E12" t="s">
         <v>38</v>
@@ -45189,7 +45189,7 @@
         <v>12</v>
       </c>
       <c r="D13" s="26">
-        <v>5000</v>
+        <v>6000</v>
       </c>
       <c r="E13" t="s">
         <v>38</v>
@@ -45500,7 +45500,7 @@
         <v>15</v>
       </c>
       <c r="D25" s="4">
-        <v>1700</v>
+        <v>1000</v>
       </c>
       <c r="E25" t="s">
         <v>38</v>
@@ -45668,7 +45668,7 @@
         <v>19</v>
       </c>
       <c r="D32">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="E32" t="s">
         <v>38</v>
@@ -45692,7 +45692,7 @@
         <v>18</v>
       </c>
       <c r="D33">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="E33" t="s">
         <v>38</v>
@@ -45716,7 +45716,7 @@
         <v>12</v>
       </c>
       <c r="D34">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="E34" t="s">
         <v>38</v>
@@ -45737,7 +45737,7 @@
         <v>462</v>
       </c>
       <c r="C35">
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="D35">
         <v>3000</v>
@@ -45754,43 +45754,41 @@
       <c r="I35" s="23"/>
     </row>
     <row r="36" spans="1:9">
+      <c r="A36" s="1">
+        <v>55</v>
+      </c>
+      <c r="B36" t="s">
+        <v>6</v>
+      </c>
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36">
+        <v>0.5</v>
+      </c>
+      <c r="E36" t="s">
+        <v>38</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
       <c r="I36" s="23"/>
-    </row>
-    <row r="37" spans="1:9">
-      <c r="A37" s="1">
-        <v>40</v>
-      </c>
-      <c r="B37" t="s">
-        <v>12</v>
-      </c>
-      <c r="C37">
-        <v>1</v>
-      </c>
-      <c r="D37" s="4">
-        <v>5663.9430000000002</v>
-      </c>
-      <c r="E37" t="s">
-        <v>38</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-      <c r="G37">
-        <v>0</v>
-      </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" s="1">
-        <v>41</v>
-      </c>
-      <c r="B38" s="25" t="s">
-        <v>32</v>
+        <v>40</v>
+      </c>
+      <c r="B38" t="s">
+        <v>12</v>
       </c>
       <c r="C38">
         <v>1</v>
       </c>
-      <c r="D38">
-        <v>41</v>
+      <c r="D38" s="4">
+        <v>5663.9430000000002</v>
       </c>
       <c r="E38" t="s">
         <v>38</v>
@@ -45804,24 +45802,47 @@
     </row>
     <row r="39" spans="1:9">
       <c r="A39" s="1">
+        <v>41</v>
+      </c>
+      <c r="B39" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39">
+        <v>41</v>
+      </c>
+      <c r="E39" t="s">
+        <v>38</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="1">
         <v>46</v>
       </c>
-      <c r="B39" t="s">
+      <c r="B40" t="s">
         <v>32</v>
       </c>
-      <c r="C39">
+      <c r="C40">
         <v>20</v>
       </c>
-      <c r="D39">
+      <c r="D40">
         <v>1000</v>
       </c>
-      <c r="E39" t="s">
-        <v>38</v>
-      </c>
-      <c r="F39">
-        <v>0</v>
-      </c>
-      <c r="G39">
+      <c r="E40" t="s">
+        <v>38</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
         <v>0</v>
       </c>
     </row>
@@ -45838,7 +45859,7 @@
   </sheetPr>
   <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E30" sqref="E30"/>
     </sheetView>
   </sheetViews>
@@ -46445,8 +46466,8 @@
   </sheetPr>
   <dimension ref="A1:J67"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>

</xml_diff>

<commit_message>
power plants with onshore
</commit_message>
<xml_diff>
--- a/data/Power_plants.xlsx
+++ b/data/Power_plants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CDB8019-2CA9-4068-94E8-CE483E0059AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8231714B-2A6A-43D5-9754-92133483A48C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="971" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="971" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="groupedNLGAS" sheetId="20" r:id="rId1"/>
@@ -18,43 +18,44 @@
     <sheet name="superGroupedNL" sheetId="15" r:id="rId3"/>
     <sheet name="extendedNL" sheetId="22" r:id="rId4"/>
     <sheet name="groupedDecarbonizedNLwithGas" sheetId="31" r:id="rId5"/>
-    <sheet name="groupedDecarbonizedNL" sheetId="29" r:id="rId6"/>
-    <sheet name="futureDecarbonizedNL" sheetId="33" r:id="rId7"/>
-    <sheet name="DecarbonizedNL" sheetId="28" r:id="rId8"/>
-    <sheet name="AnalysisforNiPlants" sheetId="21" r:id="rId9"/>
-    <sheet name="groupedNLRES" sheetId="23" r:id="rId10"/>
-    <sheet name="NL2010RES" sheetId="25" r:id="rId11"/>
-    <sheet name="Sheet1" sheetId="27" r:id="rId12"/>
-    <sheet name="NL_withplanneddecommissions" sheetId="26" r:id="rId13"/>
-    <sheet name="groupedDecarbonizedFLEXNET" sheetId="24" r:id="rId14"/>
-    <sheet name="groupedNL" sheetId="16" r:id="rId15"/>
-    <sheet name="extendedDEmoreoptimal" sheetId="12" r:id="rId16"/>
-    <sheet name="extendedDE" sheetId="1" r:id="rId17"/>
-    <sheet name="powerplants_grouped_DE" sheetId="3" r:id="rId18"/>
-    <sheet name="germany2019" sheetId="5" r:id="rId19"/>
-    <sheet name="dutchGermanPlants2015_from_emla" sheetId="13" r:id="rId20"/>
+    <sheet name="groupedDecarbonizedNL_notechlim" sheetId="34" r:id="rId6"/>
+    <sheet name="groupedDecarbonizedNL" sheetId="29" r:id="rId7"/>
+    <sheet name="futureDecarbonizedNL" sheetId="33" r:id="rId8"/>
+    <sheet name="DecarbonizedNL" sheetId="28" r:id="rId9"/>
+    <sheet name="AnalysisforNiPlants" sheetId="21" r:id="rId10"/>
+    <sheet name="groupedNLRES" sheetId="23" r:id="rId11"/>
+    <sheet name="NL2010RES" sheetId="25" r:id="rId12"/>
+    <sheet name="Sheet1" sheetId="27" r:id="rId13"/>
+    <sheet name="NL_withplanneddecommissions" sheetId="26" r:id="rId14"/>
+    <sheet name="groupedDecarbonizedFLEXNET" sheetId="24" r:id="rId15"/>
+    <sheet name="groupedNL" sheetId="16" r:id="rId16"/>
+    <sheet name="extendedDEmoreoptimal" sheetId="12" r:id="rId17"/>
+    <sheet name="extendedDE" sheetId="1" r:id="rId18"/>
+    <sheet name="powerplants_grouped_DE" sheetId="3" r:id="rId19"/>
+    <sheet name="germany2019" sheetId="5" r:id="rId20"/>
+    <sheet name="dutchGermanPlants2015_from_emla" sheetId="13" r:id="rId21"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId21"/>
+    <externalReference r:id="rId22"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">AnalysisforNiPlants!$B$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">DecarbonizedNL!$A$1:$H$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">dutchGermanPlants2015_from_emla!$A$1:$H$440</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">extendedDE!$B$1:$J$272</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">extendedDEmoreoptimal!$B$1:$J$193</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">AnalysisforNiPlants!$B$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">DecarbonizedNL!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">dutchGermanPlants2015_from_emla!$A$1:$H$440</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">extendedDE!$B$1:$J$272</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">extendedDEmoreoptimal!$B$1:$J$193</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">extendedNL!$A$1:$J$51</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">groupedDecarbonizedFLEXNET!$A$1:$I$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">groupedNL!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">groupedDecarbonizedFLEXNET!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">groupedNL!$A$1:$J$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">groupedNLGAS!$A$1:$J$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">groupedNLRES!$A$1:$J$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">NL_withplanneddecommissions!$A$1:$K$190</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">groupedNLRES!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">NL_withplanneddecommissions!$A$1:$K$190</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">superGroupedNL!$A$1:$J$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId22"/>
-    <pivotCache cacheId="1" r:id="rId23"/>
+    <pivotCache cacheId="0" r:id="rId23"/>
+    <pivotCache cacheId="1" r:id="rId24"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -112,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4754" uniqueCount="475">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4874" uniqueCount="475">
   <si>
     <t>Technology</t>
   </si>
@@ -4657,6 +4658,230 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD4198A0-7CB3-4BB1-94E1-721EECB3BDAC}">
+  <sheetPr>
+    <tabColor rgb="FFFFC000"/>
+  </sheetPr>
+  <dimension ref="A1:F12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="28.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" customWidth="1"/>
+    <col min="3" max="4" width="13.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="12"/>
+      <c r="B1" s="12" t="s">
+        <v>440</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>441</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="12" t="s">
+        <v>439</v>
+      </c>
+      <c r="B2" s="4">
+        <v>40.207000000000001</v>
+      </c>
+      <c r="C2" s="11">
+        <v>38</v>
+      </c>
+      <c r="D2" s="13">
+        <f t="shared" ref="D2:D12" si="0">B2-C2</f>
+        <v>2.2070000000000007</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="13">
+        <v>484</v>
+      </c>
+      <c r="C3" s="15">
+        <v>486</v>
+      </c>
+      <c r="D3" s="13">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4">
+        <f>1.768 + 631</f>
+        <v>632.76800000000003</v>
+      </c>
+      <c r="C4" s="15">
+        <v>1243</v>
+      </c>
+      <c r="D4" s="13">
+        <f t="shared" si="0"/>
+        <v>-610.23199999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4">
+        <v>962.69</v>
+      </c>
+      <c r="C5" s="11">
+        <v>957</v>
+      </c>
+      <c r="D5" s="13">
+        <f t="shared" si="0"/>
+        <v>5.6900000000000546</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="13">
+        <v>1103</v>
+      </c>
+      <c r="C6" s="14">
+        <v>1103</v>
+      </c>
+      <c r="D6" s="13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="12">
+        <v>4060</v>
+      </c>
+      <c r="C7" s="11">
+        <v>4631</v>
+      </c>
+      <c r="D7" s="13">
+        <f t="shared" si="0"/>
+        <v>-571</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="13">
+        <v>4236.9939999999997</v>
+      </c>
+      <c r="C8" s="15">
+        <v>3669</v>
+      </c>
+      <c r="D8" s="13">
+        <f t="shared" si="0"/>
+        <v>567.99399999999969</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="13">
+        <v>6789.9099999999989</v>
+      </c>
+      <c r="C9" s="11">
+        <v>3937</v>
+      </c>
+      <c r="D9" s="13">
+        <f t="shared" si="0"/>
+        <v>2852.9099999999989</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="13">
+        <v>7586</v>
+      </c>
+      <c r="C10" s="14">
+        <f>15570-C11-C15</f>
+        <v>7069</v>
+      </c>
+      <c r="D10" s="13">
+        <f t="shared" si="0"/>
+        <v>517</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" s="12">
+        <v>8501.9630099999995</v>
+      </c>
+      <c r="C11" s="14">
+        <v>8501</v>
+      </c>
+      <c r="D11" s="13">
+        <f t="shared" si="0"/>
+        <v>0.96300999999948544</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="12" t="s">
+        <v>443</v>
+      </c>
+      <c r="B12" s="13">
+        <f>SUM(B2:B11)</f>
+        <v>34397.532009999995</v>
+      </c>
+      <c r="C12" s="13">
+        <f>SUM(C2:C11)</f>
+        <v>31634</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>2763.5320099999954</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:D1" xr:uid="{CD4198A0-7CB3-4BB1-94E1-721EECB3BDAC}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:D12">
+      <sortCondition ref="B1"/>
+    </sortState>
+  </autoFilter>
+  <conditionalFormatting sqref="D2:D11">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67609830-ACCB-49F0-B751-AE24D0F6CF61}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -5907,7 +6132,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5DC26A1-8AAE-49C1-B239-84231B4324DA}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -7342,7 +7567,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B60C3C6E-8400-4F42-A1F0-82CC35A1E938}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -7482,7 +7707,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB94089A-EE04-4A8F-A9CF-12445972E5C2}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -13978,7 +14203,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85AAE1DC-B1F2-40C9-B131-9296BF39A7D3}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -14662,7 +14887,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCCA0DB4-82B5-4F45-9627-77778B586330}">
   <dimension ref="A1:K12"/>
   <sheetViews>
@@ -15105,7 +15330,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DF78530-F1D3-4B7A-B937-9D785DB65B2F}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J193"/>
@@ -21192,7 +21417,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M272"/>
   <sheetViews>
@@ -29957,7 +30182,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88DF7B89-3137-4483-A2A9-559F907A912A}">
   <dimension ref="A1:I34"/>
   <sheetViews>
@@ -30982,7 +31207,35 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88C4D45E-47BE-4484-8166-1FE6AE7D2D6F}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T39" sqref="T39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>469</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871B8469-CA4D-495B-9C72-1DE61BB7D586}">
   <dimension ref="A1:Z17"/>
   <sheetViews>
@@ -31434,35 +31687,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88C4D45E-47BE-4484-8166-1FE6AE7D2D6F}">
-  <sheetPr>
-    <tabColor rgb="FFFFFF00"/>
-  </sheetPr>
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T39" sqref="T39"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>469</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EE2FE5B-BFDE-4C21-9291-DDF53677D345}">
   <dimension ref="A1:I381"/>
   <sheetViews>
@@ -44879,14 +45104,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8276941-6CB9-425B-B187-B06A7EEE7BC6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E5C317A-A841-4977-A917-D22655607894}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:N53"/>
+  <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A4" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
+      <selection activeCell="J49" sqref="J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -46082,20 +46307,63 @@
       </c>
     </row>
     <row r="50" spans="1:7">
-      <c r="A50" s="1"/>
+      <c r="A50" s="1">
+        <v>70</v>
+      </c>
+      <c r="B50" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50">
+        <v>23</v>
+      </c>
+      <c r="D50">
+        <v>3000</v>
+      </c>
+      <c r="E50" t="s">
+        <v>38</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="1">
+        <v>71</v>
+      </c>
+      <c r="B51" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51">
+        <v>10</v>
+      </c>
+      <c r="D51">
+        <v>3000</v>
+      </c>
+      <c r="E51" t="s">
+        <v>38</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
     </row>
     <row r="52" spans="1:7">
       <c r="A52" s="1">
-        <v>53</v>
-      </c>
-      <c r="B52" t="s">
-        <v>434</v>
+        <v>72</v>
+      </c>
+      <c r="B52" s="29" t="s">
+        <v>13</v>
       </c>
       <c r="C52">
-        <v>1</v>
-      </c>
-      <c r="D52" s="28">
-        <v>0.5</v>
+        <v>5</v>
+      </c>
+      <c r="D52">
+        <v>3000</v>
       </c>
       <c r="E52" t="s">
         <v>38</v>
@@ -46104,29 +46372,98 @@
         <v>0</v>
       </c>
       <c r="G52">
-        <v>0.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="A53" s="1">
+        <v>73</v>
+      </c>
+      <c r="B53" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C53">
+        <v>3</v>
+      </c>
+      <c r="D53">
+        <v>3000</v>
+      </c>
+      <c r="E53" t="s">
+        <v>38</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
+      <c r="A54" s="1">
+        <v>74</v>
+      </c>
+      <c r="B54" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54">
+        <v>1</v>
+      </c>
+      <c r="D54">
+        <v>3000</v>
+      </c>
+      <c r="E54" t="s">
+        <v>38</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="1">
+        <v>53</v>
+      </c>
+      <c r="B58" t="s">
+        <v>434</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="E58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="1">
         <v>54</v>
       </c>
-      <c r="B53" t="s">
+      <c r="B59" t="s">
         <v>6</v>
       </c>
-      <c r="C53">
-        <v>1</v>
-      </c>
-      <c r="D53" s="28">
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59" s="28">
         <v>0.5</v>
       </c>
-      <c r="E53" t="s">
-        <v>38</v>
-      </c>
-      <c r="F53">
-        <v>0</v>
-      </c>
-      <c r="G53">
+      <c r="E59" t="s">
+        <v>38</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
         <v>0</v>
       </c>
     </row>
@@ -46137,6 +46474,1264 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8276941-6CB9-425B-B187-B06A7EEE7BC6}">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
+  <dimension ref="A1:N53"/>
+  <sheetViews>
+    <sheetView showRuler="0" topLeftCell="A4" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
+      <selection activeCell="P39" sqref="P39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="2" width="35.90625" customWidth="1"/>
+    <col min="7" max="7" width="13.90625" customWidth="1"/>
+    <col min="10" max="10" width="28.90625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" t="s">
+        <v>447</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="1">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4">
+        <v>5663.9430000000002</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="I2" s="23"/>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="1">
+        <v>23</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>20</v>
+      </c>
+      <c r="D3" s="4">
+        <v>2400</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="1">
+        <v>24</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4">
+        <v>16</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2400</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="23"/>
+    </row>
+    <row r="5" spans="1:14" ht="16" customHeight="1">
+      <c r="A5" s="1">
+        <v>25</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="D5" s="4">
+        <v>2400</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="I5" s="23"/>
+      <c r="K5" s="4">
+        <f>D5*3</f>
+        <v>7200</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="16" customHeight="1">
+      <c r="A6" s="1">
+        <v>26</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2400</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="I6" s="23"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:14" ht="16" customHeight="1">
+      <c r="A7" s="1">
+        <v>27</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" s="4">
+        <v>2400</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="I7" s="23"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:14" ht="16" customHeight="1">
+      <c r="A8" s="1">
+        <v>28</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8">
+        <v>24</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="I8" s="23"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:14" ht="16" customHeight="1">
+      <c r="A9" s="1">
+        <v>29</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9">
+        <v>23</v>
+      </c>
+      <c r="D9" s="4">
+        <v>2500</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="I9" s="23"/>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:14" ht="16" customHeight="1">
+      <c r="A10" s="1">
+        <v>30</v>
+      </c>
+      <c r="B10" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="19">
+        <v>21</v>
+      </c>
+      <c r="D10" s="31">
+        <v>3000</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" s="19">
+        <v>0</v>
+      </c>
+      <c r="G10" s="19">
+        <v>0</v>
+      </c>
+      <c r="I10" s="23"/>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:14" ht="16" customHeight="1">
+      <c r="A11" s="1">
+        <v>31</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>19</v>
+      </c>
+      <c r="D11" s="4">
+        <v>3000</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="I11" s="23"/>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:14" ht="16" customHeight="1">
+      <c r="A12" s="1">
+        <v>32</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12">
+        <v>18</v>
+      </c>
+      <c r="D12" s="4">
+        <v>3000</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="I12" s="23"/>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" s="1">
+        <v>33</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13">
+        <v>17</v>
+      </c>
+      <c r="D13" s="4">
+        <v>3000</v>
+      </c>
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="I13" s="23"/>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:14" ht="14" customHeight="1">
+      <c r="A14" s="1">
+        <v>34</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C14">
+        <v>16</v>
+      </c>
+      <c r="D14" s="4">
+        <v>3000</v>
+      </c>
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="I14" s="23"/>
+      <c r="K14" s="4"/>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="1">
+        <v>35</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>15</v>
+      </c>
+      <c r="D15" s="4">
+        <v>3000</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="I15" s="23"/>
+      <c r="L15" s="3"/>
+      <c r="N15" s="4"/>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="1">
+        <v>36</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <v>14</v>
+      </c>
+      <c r="D16" s="4">
+        <v>3000</v>
+      </c>
+      <c r="E16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="I16" s="23"/>
+      <c r="L16" s="3"/>
+      <c r="N16" s="4"/>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="1">
+        <v>37</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17">
+        <v>13</v>
+      </c>
+      <c r="D17" s="4">
+        <v>3000</v>
+      </c>
+      <c r="E17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="I17" s="23"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="3"/>
+      <c r="N17" s="4"/>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="1">
+        <v>38</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>12</v>
+      </c>
+      <c r="D18" s="4">
+        <v>3000</v>
+      </c>
+      <c r="E18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="I18" s="23"/>
+      <c r="J18" t="s">
+        <v>471</v>
+      </c>
+      <c r="L18" s="3"/>
+      <c r="N18" s="4"/>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="1">
+        <v>39</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C19">
+        <v>11</v>
+      </c>
+      <c r="D19" s="4">
+        <v>3500</v>
+      </c>
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="I19" s="23"/>
+      <c r="J19" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14">
+      <c r="A20" s="1">
+        <v>40</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20">
+        <v>10</v>
+      </c>
+      <c r="D20" s="4">
+        <v>3500</v>
+      </c>
+      <c r="E20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="I20" s="23"/>
+    </row>
+    <row r="21" spans="1:14">
+      <c r="A21" s="1">
+        <v>41</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C21">
+        <v>9</v>
+      </c>
+      <c r="D21" s="4">
+        <v>3500</v>
+      </c>
+      <c r="E21" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="J21" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14">
+      <c r="A22" s="1">
+        <v>42</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22">
+        <v>8</v>
+      </c>
+      <c r="D22" s="4">
+        <v>3500</v>
+      </c>
+      <c r="E22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14">
+      <c r="A23" s="1">
+        <v>43</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23">
+        <v>7</v>
+      </c>
+      <c r="D23" s="4">
+        <v>3500</v>
+      </c>
+      <c r="E23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14">
+      <c r="A24" s="1">
+        <v>44</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C24">
+        <v>6</v>
+      </c>
+      <c r="D24" s="4">
+        <v>3500</v>
+      </c>
+      <c r="E24" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="1">
+        <v>45</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C25">
+        <v>5</v>
+      </c>
+      <c r="D25" s="4">
+        <v>3500</v>
+      </c>
+      <c r="E25" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="1">
+        <v>46</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C26">
+        <v>4</v>
+      </c>
+      <c r="D26" s="4">
+        <v>3500</v>
+      </c>
+      <c r="E26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="1">
+        <v>47</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27">
+        <v>3</v>
+      </c>
+      <c r="D27" s="4">
+        <v>3500</v>
+      </c>
+      <c r="E27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="1">
+        <v>48</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" s="4">
+        <v>3850</v>
+      </c>
+      <c r="E28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="1">
+        <v>49</v>
+      </c>
+      <c r="B29" s="29" t="s">
+        <v>15</v>
+      </c>
+      <c r="C29" s="19">
+        <v>1</v>
+      </c>
+      <c r="D29" s="30">
+        <v>3000</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F29" s="19">
+        <v>0</v>
+      </c>
+      <c r="G29" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="1">
+        <v>50</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C30">
+        <v>24</v>
+      </c>
+      <c r="D30" s="27">
+        <v>3000</v>
+      </c>
+      <c r="E30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="I30" s="23"/>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="1">
+        <v>51</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C31">
+        <v>22</v>
+      </c>
+      <c r="D31" s="27">
+        <v>3000</v>
+      </c>
+      <c r="E31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="1">
+        <v>52</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C32">
+        <v>20</v>
+      </c>
+      <c r="D32" s="27">
+        <v>3000</v>
+      </c>
+      <c r="E32" t="s">
+        <v>38</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="I32" s="23"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="1">
+        <v>53</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C33">
+        <v>18</v>
+      </c>
+      <c r="D33" s="27">
+        <v>3000</v>
+      </c>
+      <c r="E33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="I33" s="23"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="1">
+        <v>54</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C34">
+        <v>16</v>
+      </c>
+      <c r="D34" s="27">
+        <v>3000</v>
+      </c>
+      <c r="E34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="I34" s="23"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="1">
+        <v>55</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C35">
+        <v>14</v>
+      </c>
+      <c r="D35" s="27">
+        <v>3000</v>
+      </c>
+      <c r="E35" t="s">
+        <v>38</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="I35" s="23"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="1">
+        <v>56</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36">
+        <v>10</v>
+      </c>
+      <c r="D36" s="27">
+        <v>3000</v>
+      </c>
+      <c r="E36" t="s">
+        <v>38</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+      <c r="I36" s="23"/>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="1">
+        <v>57</v>
+      </c>
+      <c r="B37" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37">
+        <v>8</v>
+      </c>
+      <c r="D37" s="30">
+        <v>3000</v>
+      </c>
+      <c r="E37" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F37" s="19">
+        <v>0</v>
+      </c>
+      <c r="G37" s="19">
+        <v>0</v>
+      </c>
+      <c r="I37" s="23"/>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="1">
+        <v>58</v>
+      </c>
+      <c r="B38" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="19">
+        <v>6</v>
+      </c>
+      <c r="D38" s="30">
+        <v>4000</v>
+      </c>
+      <c r="E38" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F38" s="19">
+        <v>0</v>
+      </c>
+      <c r="G38" s="19">
+        <v>0</v>
+      </c>
+      <c r="I38" s="23"/>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="1">
+        <v>59</v>
+      </c>
+      <c r="B39" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C39" s="19">
+        <v>4</v>
+      </c>
+      <c r="D39" s="30">
+        <v>3000</v>
+      </c>
+      <c r="E39" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F39" s="19">
+        <v>0</v>
+      </c>
+      <c r="G39" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="1">
+        <v>60</v>
+      </c>
+      <c r="B40" s="29" t="s">
+        <v>14</v>
+      </c>
+      <c r="C40" s="19">
+        <v>3</v>
+      </c>
+      <c r="D40" s="30">
+        <v>3000</v>
+      </c>
+      <c r="E40" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F40" s="19">
+        <v>0</v>
+      </c>
+      <c r="G40" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="1">
+        <v>61</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C41">
+        <v>2</v>
+      </c>
+      <c r="D41" s="27">
+        <v>3000</v>
+      </c>
+      <c r="E41" t="s">
+        <v>38</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="1">
+        <v>62</v>
+      </c>
+      <c r="B42" t="s">
+        <v>462</v>
+      </c>
+      <c r="C42">
+        <v>26</v>
+      </c>
+      <c r="D42" s="28">
+        <v>1500</v>
+      </c>
+      <c r="E42" t="s">
+        <v>38</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="1">
+        <v>63</v>
+      </c>
+      <c r="B43" t="s">
+        <v>462</v>
+      </c>
+      <c r="C43">
+        <v>22</v>
+      </c>
+      <c r="D43" s="28">
+        <v>1500</v>
+      </c>
+      <c r="E43" t="s">
+        <v>38</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="1">
+        <v>64</v>
+      </c>
+      <c r="B44" t="s">
+        <v>462</v>
+      </c>
+      <c r="C44">
+        <v>18</v>
+      </c>
+      <c r="D44" s="28">
+        <v>1500</v>
+      </c>
+      <c r="E44" t="s">
+        <v>38</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="1">
+        <v>65</v>
+      </c>
+      <c r="B45" t="s">
+        <v>462</v>
+      </c>
+      <c r="C45">
+        <v>14</v>
+      </c>
+      <c r="D45" s="28">
+        <v>1500</v>
+      </c>
+      <c r="E45" t="s">
+        <v>38</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="1">
+        <v>66</v>
+      </c>
+      <c r="B46" t="s">
+        <v>462</v>
+      </c>
+      <c r="C46">
+        <v>10</v>
+      </c>
+      <c r="D46" s="28">
+        <v>1500</v>
+      </c>
+      <c r="E46" t="s">
+        <v>38</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="1">
+        <v>67</v>
+      </c>
+      <c r="B47" t="s">
+        <v>462</v>
+      </c>
+      <c r="C47">
+        <v>8</v>
+      </c>
+      <c r="D47" s="28">
+        <v>1500</v>
+      </c>
+      <c r="E47" t="s">
+        <v>38</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="1">
+        <v>68</v>
+      </c>
+      <c r="B48" t="s">
+        <v>462</v>
+      </c>
+      <c r="C48">
+        <v>4</v>
+      </c>
+      <c r="D48" s="28">
+        <v>2000</v>
+      </c>
+      <c r="E48" t="s">
+        <v>38</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="1">
+        <v>69</v>
+      </c>
+      <c r="B49" t="s">
+        <v>462</v>
+      </c>
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49" s="28">
+        <v>2000</v>
+      </c>
+      <c r="E49" t="s">
+        <v>38</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="1"/>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="1">
+        <v>53</v>
+      </c>
+      <c r="B52" t="s">
+        <v>434</v>
+      </c>
+      <c r="C52">
+        <v>1</v>
+      </c>
+      <c r="D52" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="E52" t="s">
+        <v>38</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="1">
+        <v>54</v>
+      </c>
+      <c r="B53" t="s">
+        <v>6</v>
+      </c>
+      <c r="C53">
+        <v>1</v>
+      </c>
+      <c r="D53" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="E53" t="s">
+        <v>38</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43471EED-B6C7-4F44-860D-1AE180707620}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -46972,7 +48567,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE12E6AE-0A69-4EFB-8C68-8C862108BAC1}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -48761,228 +50356,4 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD4198A0-7CB3-4BB1-94E1-721EECB3BDAC}">
-  <sheetPr>
-    <tabColor rgb="FFFFC000"/>
-  </sheetPr>
-  <dimension ref="A1:F12"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
-  <cols>
-    <col min="1" max="1" width="28.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.81640625" customWidth="1"/>
-    <col min="3" max="4" width="13.453125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="12"/>
-      <c r="B1" s="12" t="s">
-        <v>440</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>441</v>
-      </c>
-      <c r="D1" s="12" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="12" t="s">
-        <v>439</v>
-      </c>
-      <c r="B2" s="4">
-        <v>40.207000000000001</v>
-      </c>
-      <c r="C2" s="11">
-        <v>38</v>
-      </c>
-      <c r="D2" s="13">
-        <f t="shared" ref="D2:D12" si="0">B2-C2</f>
-        <v>2.2070000000000007</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="12" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="13">
-        <v>484</v>
-      </c>
-      <c r="C3" s="15">
-        <v>486</v>
-      </c>
-      <c r="D3" s="13">
-        <f t="shared" si="0"/>
-        <v>-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4">
-        <f>1.768 + 631</f>
-        <v>632.76800000000003</v>
-      </c>
-      <c r="C4" s="15">
-        <v>1243</v>
-      </c>
-      <c r="D4" s="13">
-        <f t="shared" si="0"/>
-        <v>-610.23199999999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="4">
-        <v>962.69</v>
-      </c>
-      <c r="C5" s="11">
-        <v>957</v>
-      </c>
-      <c r="D5" s="13">
-        <f t="shared" si="0"/>
-        <v>5.6900000000000546</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="13">
-        <v>1103</v>
-      </c>
-      <c r="C6" s="14">
-        <v>1103</v>
-      </c>
-      <c r="D6" s="13">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F6" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="12">
-        <v>4060</v>
-      </c>
-      <c r="C7" s="11">
-        <v>4631</v>
-      </c>
-      <c r="D7" s="13">
-        <f t="shared" si="0"/>
-        <v>-571</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="12" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="13">
-        <v>4236.9939999999997</v>
-      </c>
-      <c r="C8" s="15">
-        <v>3669</v>
-      </c>
-      <c r="D8" s="13">
-        <f t="shared" si="0"/>
-        <v>567.99399999999969</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9" s="12" t="s">
-        <v>15</v>
-      </c>
-      <c r="B9" s="13">
-        <v>6789.9099999999989</v>
-      </c>
-      <c r="C9" s="11">
-        <v>3937</v>
-      </c>
-      <c r="D9" s="13">
-        <f t="shared" si="0"/>
-        <v>2852.9099999999989</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="13">
-        <v>7586</v>
-      </c>
-      <c r="C10" s="14">
-        <f>15570-C11-C15</f>
-        <v>7069</v>
-      </c>
-      <c r="D10" s="13">
-        <f t="shared" si="0"/>
-        <v>517</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
-      <c r="A11" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="12">
-        <v>8501.9630099999995</v>
-      </c>
-      <c r="C11" s="14">
-        <v>8501</v>
-      </c>
-      <c r="D11" s="13">
-        <f t="shared" si="0"/>
-        <v>0.96300999999948544</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="12" t="s">
-        <v>443</v>
-      </c>
-      <c r="B12" s="13">
-        <f>SUM(B2:B11)</f>
-        <v>34397.532009999995</v>
-      </c>
-      <c r="C12" s="13">
-        <f>SUM(C2:C11)</f>
-        <v>31634</v>
-      </c>
-      <c r="D12">
-        <f t="shared" si="0"/>
-        <v>2763.5320099999954</v>
-      </c>
-    </row>
-  </sheetData>
-  <autoFilter ref="B1:D1" xr:uid="{CD4198A0-7CB3-4BB1-94E1-721EECB3BDAC}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:D12">
-      <sortCondition ref="B1"/>
-    </sortState>
-  </autoFilter>
-  <conditionalFormatting sqref="D2:D11">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
check profitability in futur market
</commit_message>
<xml_diff>
--- a/data/Power_plants.xlsx
+++ b/data/Power_plants.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
-  <workbookPr/>
+  <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7236F364-1F01-4CB2-95D1-E03274F2BF0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2AB4C0-C51C-4D09-9EFC-C508C15F4473}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="971" firstSheet="3" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="971" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="groupedNLGAS" sheetId="20" r:id="rId1"/>
@@ -2860,7 +2860,7 @@
       <sheetName val="NewTechnologies"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="2">
           <cell r="A2" t="str">
@@ -2890,11 +2890,13 @@
           <cell r="A5" t="str">
             <v>PV</v>
           </cell>
+          <cell r="B5"/>
         </row>
         <row r="6">
           <cell r="A6" t="str">
             <v>PV_residential</v>
           </cell>
+          <cell r="B6"/>
         </row>
         <row r="7">
           <cell r="A7" t="str">
@@ -2908,6 +2910,7 @@
           <cell r="A8" t="str">
             <v>Biomass_CHP_wood_pellets_PH</v>
           </cell>
+          <cell r="B8"/>
         </row>
         <row r="9">
           <cell r="A9" t="str">
@@ -2921,41 +2924,49 @@
           <cell r="A10" t="str">
             <v>CCGT_CHP_backpressure_DH</v>
           </cell>
+          <cell r="B10"/>
         </row>
         <row r="11">
           <cell r="A11" t="str">
             <v>CCGT_CHP_backpressure_PH</v>
           </cell>
+          <cell r="B11"/>
         </row>
         <row r="12">
           <cell r="A12" t="str">
             <v>CCS</v>
           </cell>
+          <cell r="B12"/>
         </row>
         <row r="13">
           <cell r="A13" t="str">
             <v>CSP_Parabolic</v>
           </cell>
+          <cell r="B13"/>
         </row>
         <row r="14">
           <cell r="A14" t="str">
             <v>CSP_Tower</v>
           </cell>
+          <cell r="B14"/>
         </row>
         <row r="15">
           <cell r="A15" t="str">
             <v>Hydrogen_to_Jet_Fuel</v>
           </cell>
+          <cell r="B15"/>
         </row>
         <row r="16">
           <cell r="A16" t="str">
             <v>Hydropower_ROR</v>
           </cell>
+          <cell r="B16"/>
         </row>
         <row r="17">
           <cell r="A17" t="str">
             <v>Hydropower_reservoir_large</v>
           </cell>
+          <cell r="B17"/>
         </row>
         <row r="18">
           <cell r="A18" t="str">
@@ -2969,6 +2980,7 @@
           <cell r="A19" t="str">
             <v>Hydropower_reservoir_small</v>
           </cell>
+          <cell r="B19"/>
         </row>
         <row r="20">
           <cell r="A20" t="str">
@@ -2982,11 +2994,13 @@
           <cell r="A21" t="str">
             <v>Nuclear_CHP_DH</v>
           </cell>
+          <cell r="B21"/>
         </row>
         <row r="22">
           <cell r="A22" t="str">
             <v>Nuclear_CHP_PH</v>
           </cell>
+          <cell r="B22"/>
         </row>
         <row r="23">
           <cell r="A23" t="str">
@@ -3000,26 +3014,31 @@
           <cell r="A24" t="str">
             <v>PEM_Electrolyzer</v>
           </cell>
+          <cell r="B24"/>
         </row>
         <row r="25">
           <cell r="A25" t="str">
             <v>Power_to_Jet_Fuel</v>
           </cell>
+          <cell r="B25"/>
         </row>
         <row r="26">
           <cell r="A26" t="str">
             <v>Wave_energy</v>
           </cell>
+          <cell r="B26"/>
         </row>
         <row r="27">
           <cell r="A27" t="str">
             <v>Lithium_ion_battery</v>
           </cell>
+          <cell r="B27"/>
         </row>
         <row r="28">
           <cell r="A28" t="str">
             <v>Pumped_hydro</v>
           </cell>
+          <cell r="B28"/>
         </row>
         <row r="29">
           <cell r="A29" t="str">
@@ -3049,38 +3068,39 @@
           <cell r="A32" t="str">
             <v>fuel_cell</v>
           </cell>
+          <cell r="B32"/>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -5692,8 +5712,8 @@
   </sheetPr>
   <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A7" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
-      <selection activeCell="J57" sqref="J57"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A11" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
+      <selection activeCell="W30" sqref="W30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -5702,6 +5722,8 @@
     <col min="7" max="7" width="13.88671875" customWidth="1"/>
     <col min="10" max="10" width="28.88671875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.44140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11">

</xml_diff>

<commit_message>
past revenues were not reading correctly so plants lifetime was not extended
</commit_message>
<xml_diff>
--- a/data/Power_plants.xlsx
+++ b/data/Power_plants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65D5F8A9-0186-428A-9F6A-8A07DAEC9D1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0AE56C8-8884-46C1-ADFA-9727E74C4C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="971" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -117,7 +117,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5267" uniqueCount="479">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5270" uniqueCount="479">
   <si>
     <t>Technology</t>
   </si>
@@ -47521,7 +47521,7 @@
   <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -47667,7 +47667,7 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -47897,7 +47897,30 @@
       </c>
     </row>
     <row r="15" spans="1:13">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15">
+        <v>24</v>
+      </c>
+      <c r="D15">
+        <v>1000</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="1"/>

</xml_diff>

<commit_message>
making nuclear again fix during all simulation.
</commit_message>
<xml_diff>
--- a/data/Power_plants.xlsx
+++ b/data/Power_plants.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8441B182-38DE-4DBE-B08D-0ABFE57510E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582915A0-7C7B-43F2-B2AA-B885DE77DC78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="971" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -6071,7 +6071,7 @@
   <dimension ref="A1:N60"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6116,7 +6116,7 @@
         <v>12</v>
       </c>
       <c r="C2">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="D2" s="4">
         <v>1000</v>
@@ -6139,7 +6139,7 @@
         <v>12</v>
       </c>
       <c r="C3">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="D3" s="4">
         <v>1000</v>
@@ -6162,7 +6162,7 @@
         <v>12</v>
       </c>
       <c r="C4">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="D4" s="4">
         <v>1000</v>
@@ -6185,7 +6185,7 @@
         <v>12</v>
       </c>
       <c r="C5">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D5" s="4">
         <v>700</v>

</xml_diff>

<commit_message>
updating DATA back to traderes
Electrolyzers: 29090MW (new investment)
Nuclear: 3684MW (initial capacity + 0 new investment)
NL H2 price: 45 €/MWh
</commit_message>
<xml_diff>
--- a/data/Power_plants.xlsx
+++ b/data/Power_plants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{582915A0-7C7B-43F2-B2AA-B885DE77DC78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{962C1260-011A-4782-A6A1-38C9F2A09BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="971" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="971" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="groupedNLGAS" sheetId="20" r:id="rId1"/>
@@ -58,9 +58,9 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId27"/>
-    <pivotCache cacheId="1" r:id="rId28"/>
-    <pivotCache cacheId="2" r:id="rId29"/>
+    <pivotCache cacheId="2" r:id="rId27"/>
+    <pivotCache cacheId="3" r:id="rId28"/>
+    <pivotCache cacheId="4" r:id="rId29"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5413" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5413" uniqueCount="486">
   <si>
     <t>Technology</t>
   </si>
@@ -1562,6 +1562,21 @@
   <si>
     <t>hydrogen combined cycle</t>
   </si>
+  <si>
+    <t>Solar PV large</t>
+  </si>
+  <si>
+    <t>Wind Offshore</t>
+  </si>
+  <si>
+    <t>hydrogen turbine</t>
+  </si>
+  <si>
+    <t>Lithium ion battery</t>
+  </si>
+  <si>
+    <t>Biofuel</t>
+  </si>
 </sst>
 </file>
 
@@ -2865,227 +2880,218 @@
       <sheetName val="NewTechnologies"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="0"/>
       <sheetData sheetId="1">
         <row r="2">
           <cell r="A2" t="str">
-            <v>WTG_offshore</v>
+            <v>Biofuel</v>
           </cell>
           <cell r="B2" t="str">
-            <v>Offshore wind PGT</v>
+            <v>Biomass CHP</v>
           </cell>
         </row>
         <row r="3">
           <cell r="A3" t="str">
-            <v>WTG_onshore</v>
-          </cell>
-          <cell r="B3" t="str">
-            <v>Onshore wind PGT</v>
+            <v>Biomass_CHP_wood_pellets_PH</v>
           </cell>
         </row>
         <row r="4">
           <cell r="A4" t="str">
-            <v>PV_utility_systems</v>
+            <v>CCGT</v>
           </cell>
           <cell r="B4" t="str">
-            <v>Photovoltaic PGT</v>
+            <v>CCGT</v>
           </cell>
         </row>
         <row r="5">
           <cell r="A5" t="str">
-            <v>PV</v>
+            <v>CCGT_CHP_backpressure_DH</v>
           </cell>
         </row>
         <row r="6">
           <cell r="A6" t="str">
-            <v>PV_residential</v>
+            <v>CCGT_CHP_backpressure_PH</v>
           </cell>
         </row>
         <row r="7">
           <cell r="A7" t="str">
-            <v>Biomass_CHP_wood_pellets_DH</v>
-          </cell>
-          <cell r="B7" t="str">
-            <v>Biomass CHP</v>
+            <v>CCS</v>
           </cell>
         </row>
         <row r="8">
           <cell r="A8" t="str">
-            <v>Biomass_CHP_wood_pellets_PH</v>
+            <v>Coal PSC</v>
+          </cell>
+          <cell r="B8" t="str">
+            <v>Coal PSC</v>
           </cell>
         </row>
         <row r="9">
           <cell r="A9" t="str">
-            <v>CCGT</v>
-          </cell>
-          <cell r="B9" t="str">
-            <v>CCGT</v>
+            <v>CSP_Parabolic</v>
           </cell>
         </row>
         <row r="10">
           <cell r="A10" t="str">
-            <v>CCGT_CHP_backpressure_DH</v>
+            <v>CSP_Tower</v>
           </cell>
         </row>
         <row r="11">
           <cell r="A11" t="str">
-            <v>CCGT_CHP_backpressure_PH</v>
+            <v>electrolyzer</v>
           </cell>
         </row>
         <row r="12">
           <cell r="A12" t="str">
-            <v>CCS</v>
+            <v>Fuel oil PGT</v>
+          </cell>
+          <cell r="B12" t="str">
+            <v>Fuel oil PGT</v>
           </cell>
         </row>
         <row r="13">
           <cell r="A13" t="str">
-            <v>CSP_Parabolic</v>
+            <v>fuel_cell</v>
           </cell>
         </row>
         <row r="14">
           <cell r="A14" t="str">
-            <v>CSP_Tower</v>
+            <v>hydrogen CHP</v>
           </cell>
         </row>
         <row r="15">
           <cell r="A15" t="str">
-            <v>Hydrogen_to_Jet_Fuel</v>
+            <v>hydrogen combined cycle</v>
           </cell>
         </row>
         <row r="16">
           <cell r="A16" t="str">
-            <v>Hydropower_ROR</v>
+            <v>Hydrogen_to_Jet_Fuel</v>
           </cell>
         </row>
         <row r="17">
           <cell r="A17" t="str">
-            <v>Hydropower_reservoir_large</v>
+            <v>hydrogen turbine</v>
           </cell>
         </row>
         <row r="18">
           <cell r="A18" t="str">
-            <v>Hydropower_reservoir_medium</v>
-          </cell>
-          <cell r="B18" t="str">
-            <v>Hydroelectric</v>
+            <v>Hydropower_reservoir_large</v>
           </cell>
         </row>
         <row r="19">
           <cell r="A19" t="str">
-            <v>Hydropower_reservoir_small</v>
+            <v>Hydropower</v>
+          </cell>
+          <cell r="B19" t="str">
+            <v>Hydroelectric</v>
           </cell>
         </row>
         <row r="20">
           <cell r="A20" t="str">
-            <v>Nuclear</v>
-          </cell>
-          <cell r="B20" t="str">
-            <v>Nuclear PGT</v>
+            <v>Hydropower_reservoir_small</v>
           </cell>
         </row>
         <row r="21">
           <cell r="A21" t="str">
-            <v>Nuclear_CHP_DH</v>
+            <v>Hydropower_ROR</v>
           </cell>
         </row>
         <row r="22">
           <cell r="A22" t="str">
-            <v>Nuclear_CHP_PH</v>
+            <v>Lignite PSC</v>
+          </cell>
+          <cell r="B22" t="str">
+            <v>Lignite PSC</v>
           </cell>
         </row>
         <row r="23">
           <cell r="A23" t="str">
-            <v>OCGT</v>
-          </cell>
-          <cell r="B23" t="str">
-            <v>OCGT</v>
+            <v>Lithium ion battery</v>
           </cell>
         </row>
         <row r="24">
           <cell r="A24" t="str">
-            <v>PEM_Electrolyzer</v>
+            <v>Nuclear</v>
+          </cell>
+          <cell r="B24" t="str">
+            <v>Nuclear PGT</v>
           </cell>
         </row>
         <row r="25">
           <cell r="A25" t="str">
-            <v>Power_to_Jet_Fuel</v>
+            <v>Nuclear_CHP_DH</v>
           </cell>
         </row>
         <row r="26">
           <cell r="A26" t="str">
-            <v>Wave_energy</v>
+            <v>Nuclear_CHP_PH</v>
           </cell>
         </row>
         <row r="27">
           <cell r="A27" t="str">
-            <v>Lithium_ion_battery</v>
+            <v>OCGT</v>
+          </cell>
+          <cell r="B27" t="str">
+            <v>OCGT</v>
           </cell>
         </row>
         <row r="28">
           <cell r="A28" t="str">
-            <v>Pumped_hydro</v>
+            <v>PEM_Electrolyzer</v>
           </cell>
         </row>
         <row r="29">
           <cell r="A29" t="str">
-            <v>Coal PSC</v>
-          </cell>
-          <cell r="B29" t="str">
-            <v>Coal PSC</v>
+            <v>Power_to_Jet_Fuel</v>
           </cell>
         </row>
         <row r="30">
           <cell r="A30" t="str">
-            <v>Lignite PSC</v>
-          </cell>
-          <cell r="B30" t="str">
-            <v>Lignite PSC</v>
+            <v>Pumped hydro</v>
           </cell>
         </row>
         <row r="31">
           <cell r="A31" t="str">
-            <v>Fuel oil PGT</v>
-          </cell>
-          <cell r="B31" t="str">
-            <v>Fuel oil PGT</v>
+            <v>PV</v>
           </cell>
         </row>
         <row r="32">
           <cell r="A32" t="str">
-            <v>fuel_cell</v>
+            <v>Solar PV rooftop</v>
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
-      <sheetData sheetId="17" refreshError="1"/>
-      <sheetData sheetId="18" refreshError="1"/>
-      <sheetData sheetId="19" refreshError="1"/>
-      <sheetData sheetId="20" refreshError="1"/>
-      <sheetData sheetId="21" refreshError="1"/>
-      <sheetData sheetId="22" refreshError="1"/>
-      <sheetData sheetId="23" refreshError="1"/>
-      <sheetData sheetId="24" refreshError="1"/>
-      <sheetData sheetId="25" refreshError="1"/>
-      <sheetData sheetId="26" refreshError="1"/>
-      <sheetData sheetId="27" refreshError="1"/>
-      <sheetData sheetId="28" refreshError="1"/>
-      <sheetData sheetId="29" refreshError="1"/>
-      <sheetData sheetId="30" refreshError="1"/>
-      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
+      <sheetData sheetId="17"/>
+      <sheetData sheetId="18"/>
+      <sheetData sheetId="19"/>
+      <sheetData sheetId="20"/>
+      <sheetData sheetId="21"/>
+      <sheetData sheetId="22"/>
+      <sheetData sheetId="23"/>
+      <sheetData sheetId="24"/>
+      <sheetData sheetId="25"/>
+      <sheetData sheetId="26"/>
+      <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
+      <sheetData sheetId="29"/>
+      <sheetData sheetId="30"/>
+      <sheetData sheetId="31"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -4684,7 +4690,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8EBABEF3-7A12-4A97-8F01-EC0882F5F9E8}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8EBABEF3-7A12-4A97-8F01-EC0882F5F9E8}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="N1:O13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField axis="axisRow" showAll="0">
@@ -4772,7 +4778,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{52009D65-3A52-4DA5-A493-3F3BB57B52DB}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{52009D65-3A52-4DA5-A493-3F3BB57B52DB}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="P6:Q12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -4830,7 +4836,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{74BDB821-21CE-43E4-8468-DFB3CEBCE604}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{74BDB821-21CE-43E4-8468-DFB3CEBCE604}" name="PivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -6068,10 +6074,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:N60"/>
+  <dimension ref="A1:N59"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A18" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="N50" sqref="N50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6326,8 +6332,8 @@
       <c r="A11" s="1">
         <v>28</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>15</v>
+      <c r="B11" s="18" t="s">
+        <v>481</v>
       </c>
       <c r="C11">
         <v>24</v>
@@ -6351,8 +6357,8 @@
       <c r="A12" s="1">
         <v>29</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>15</v>
+      <c r="B12" s="18" t="s">
+        <v>481</v>
       </c>
       <c r="C12">
         <v>23</v>
@@ -6376,8 +6382,8 @@
       <c r="A13" s="1">
         <v>30</v>
       </c>
-      <c r="B13" s="29" t="s">
-        <v>15</v>
+      <c r="B13" s="18" t="s">
+        <v>481</v>
       </c>
       <c r="C13" s="19">
         <v>21</v>
@@ -6401,8 +6407,8 @@
       <c r="A14" s="1">
         <v>31</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>15</v>
+      <c r="B14" s="18" t="s">
+        <v>481</v>
       </c>
       <c r="C14">
         <v>19</v>
@@ -6426,8 +6432,8 @@
       <c r="A15" s="1">
         <v>32</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>15</v>
+      <c r="B15" s="18" t="s">
+        <v>481</v>
       </c>
       <c r="C15">
         <v>18</v>
@@ -6451,8 +6457,8 @@
       <c r="A16" s="1">
         <v>33</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>15</v>
+      <c r="B16" s="18" t="s">
+        <v>481</v>
       </c>
       <c r="C16">
         <v>17</v>
@@ -6476,8 +6482,8 @@
       <c r="A17" s="1">
         <v>34</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>15</v>
+      <c r="B17" s="18" t="s">
+        <v>481</v>
       </c>
       <c r="C17">
         <v>16</v>
@@ -6501,8 +6507,8 @@
       <c r="A18" s="1">
         <v>35</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>15</v>
+      <c r="B18" s="18" t="s">
+        <v>481</v>
       </c>
       <c r="C18">
         <v>15</v>
@@ -6530,8 +6536,8 @@
       <c r="A19" s="1">
         <v>36</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>15</v>
+      <c r="B19" s="18" t="s">
+        <v>481</v>
       </c>
       <c r="C19">
         <v>14</v>
@@ -6559,8 +6565,8 @@
       <c r="A20" s="1">
         <v>37</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>15</v>
+      <c r="B20" s="18" t="s">
+        <v>481</v>
       </c>
       <c r="C20">
         <v>13</v>
@@ -6585,8 +6591,8 @@
       <c r="A21" s="1">
         <v>38</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>15</v>
+      <c r="B21" s="18" t="s">
+        <v>481</v>
       </c>
       <c r="C21">
         <v>12</v>
@@ -6611,8 +6617,8 @@
       <c r="A22" s="1">
         <v>39</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>15</v>
+      <c r="B22" s="18" t="s">
+        <v>481</v>
       </c>
       <c r="C22">
         <v>11</v>
@@ -6635,8 +6641,8 @@
       <c r="A23" s="1">
         <v>40</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>15</v>
+      <c r="B23" s="18" t="s">
+        <v>481</v>
       </c>
       <c r="C23">
         <v>10</v>
@@ -6659,8 +6665,8 @@
       <c r="A24" s="1">
         <v>41</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>15</v>
+      <c r="B24" s="18" t="s">
+        <v>481</v>
       </c>
       <c r="C24">
         <v>9</v>
@@ -6682,8 +6688,8 @@
       <c r="A25" s="1">
         <v>42</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>15</v>
+      <c r="B25" s="18" t="s">
+        <v>481</v>
       </c>
       <c r="C25">
         <v>8</v>
@@ -6705,8 +6711,8 @@
       <c r="A26" s="1">
         <v>43</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>15</v>
+      <c r="B26" s="18" t="s">
+        <v>481</v>
       </c>
       <c r="C26">
         <v>7</v>
@@ -6728,8 +6734,8 @@
       <c r="A27" s="1">
         <v>44</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>15</v>
+      <c r="B27" s="18" t="s">
+        <v>481</v>
       </c>
       <c r="C27">
         <v>6</v>
@@ -6751,8 +6757,8 @@
       <c r="A28" s="1">
         <v>45</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>15</v>
+      <c r="B28" s="18" t="s">
+        <v>481</v>
       </c>
       <c r="C28">
         <v>5</v>
@@ -6774,8 +6780,8 @@
       <c r="A29" s="1">
         <v>46</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>15</v>
+      <c r="B29" s="18" t="s">
+        <v>481</v>
       </c>
       <c r="C29">
         <v>4</v>
@@ -6797,8 +6803,8 @@
       <c r="A30" s="1">
         <v>47</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>15</v>
+      <c r="B30" s="18" t="s">
+        <v>481</v>
       </c>
       <c r="C30">
         <v>3</v>
@@ -6820,8 +6826,8 @@
       <c r="A31" s="1">
         <v>48</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>15</v>
+      <c r="B31" s="18" t="s">
+        <v>481</v>
       </c>
       <c r="C31">
         <v>2</v>
@@ -6843,8 +6849,8 @@
       <c r="A32" s="1">
         <v>49</v>
       </c>
-      <c r="B32" s="29" t="s">
-        <v>15</v>
+      <c r="B32" s="18" t="s">
+        <v>481</v>
       </c>
       <c r="C32" s="19">
         <v>1</v>
@@ -6866,8 +6872,8 @@
       <c r="A33" s="1">
         <v>50</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>14</v>
+      <c r="B33" t="s">
+        <v>482</v>
       </c>
       <c r="C33">
         <v>24</v>
@@ -6890,8 +6896,8 @@
       <c r="A34" s="1">
         <v>51</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>14</v>
+      <c r="B34" t="s">
+        <v>482</v>
       </c>
       <c r="C34">
         <v>22</v>
@@ -6913,8 +6919,8 @@
       <c r="A35" s="1">
         <v>52</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>14</v>
+      <c r="B35" t="s">
+        <v>482</v>
       </c>
       <c r="C35">
         <v>20</v>
@@ -6937,8 +6943,8 @@
       <c r="A36" s="1">
         <v>53</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>14</v>
+      <c r="B36" t="s">
+        <v>482</v>
       </c>
       <c r="C36">
         <v>18</v>
@@ -6961,8 +6967,8 @@
       <c r="A37" s="1">
         <v>54</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>14</v>
+      <c r="B37" t="s">
+        <v>482</v>
       </c>
       <c r="C37">
         <v>16</v>
@@ -6985,8 +6991,8 @@
       <c r="A38" s="1">
         <v>55</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>14</v>
+      <c r="B38" t="s">
+        <v>482</v>
       </c>
       <c r="C38">
         <v>14</v>
@@ -7009,8 +7015,8 @@
       <c r="A39" s="1">
         <v>56</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>14</v>
+      <c r="B39" t="s">
+        <v>482</v>
       </c>
       <c r="C39">
         <v>10</v>
@@ -7033,8 +7039,8 @@
       <c r="A40" s="1">
         <v>57</v>
       </c>
-      <c r="B40" s="29" t="s">
-        <v>14</v>
+      <c r="B40" t="s">
+        <v>482</v>
       </c>
       <c r="C40">
         <v>8</v>
@@ -7057,8 +7063,8 @@
       <c r="A41" s="1">
         <v>58</v>
       </c>
-      <c r="B41" s="29" t="s">
-        <v>14</v>
+      <c r="B41" t="s">
+        <v>482</v>
       </c>
       <c r="C41" s="19">
         <v>6</v>
@@ -7081,8 +7087,8 @@
       <c r="A42" s="1">
         <v>59</v>
       </c>
-      <c r="B42" s="29" t="s">
-        <v>14</v>
+      <c r="B42" t="s">
+        <v>482</v>
       </c>
       <c r="C42" s="19">
         <v>4</v>
@@ -7104,8 +7110,8 @@
       <c r="A43" s="1">
         <v>60</v>
       </c>
-      <c r="B43" s="29" t="s">
-        <v>14</v>
+      <c r="B43" t="s">
+        <v>482</v>
       </c>
       <c r="C43" s="19">
         <v>3</v>
@@ -7127,8 +7133,8 @@
       <c r="A44" s="1">
         <v>61</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>14</v>
+      <c r="B44" t="s">
+        <v>482</v>
       </c>
       <c r="C44">
         <v>2</v>
@@ -7150,8 +7156,8 @@
       <c r="A45" s="1">
         <v>62</v>
       </c>
-      <c r="B45" t="s">
-        <v>461</v>
+      <c r="B45" s="18" t="s">
+        <v>483</v>
       </c>
       <c r="C45">
         <v>28</v>
@@ -7173,8 +7179,8 @@
       <c r="A46" s="1">
         <v>63</v>
       </c>
-      <c r="B46" t="s">
-        <v>461</v>
+      <c r="B46" s="18" t="s">
+        <v>483</v>
       </c>
       <c r="C46">
         <v>26</v>
@@ -7196,8 +7202,8 @@
       <c r="A47" s="1">
         <v>64</v>
       </c>
-      <c r="B47" t="s">
-        <v>461</v>
+      <c r="B47" s="18" t="s">
+        <v>483</v>
       </c>
       <c r="C47">
         <v>24</v>
@@ -7219,8 +7225,8 @@
       <c r="A48" s="1">
         <v>65</v>
       </c>
-      <c r="B48" t="s">
-        <v>461</v>
+      <c r="B48" s="18" t="s">
+        <v>483</v>
       </c>
       <c r="C48">
         <v>22</v>
@@ -7242,8 +7248,8 @@
       <c r="A49" s="1">
         <v>66</v>
       </c>
-      <c r="B49" t="s">
-        <v>461</v>
+      <c r="B49" s="18" t="s">
+        <v>483</v>
       </c>
       <c r="C49">
         <v>20</v>
@@ -7265,8 +7271,8 @@
       <c r="A50" s="1">
         <v>67</v>
       </c>
-      <c r="B50" t="s">
-        <v>461</v>
+      <c r="B50" s="18" t="s">
+        <v>483</v>
       </c>
       <c r="C50">
         <v>18</v>
@@ -7288,8 +7294,8 @@
       <c r="A51" s="1">
         <v>68</v>
       </c>
-      <c r="B51" t="s">
-        <v>461</v>
+      <c r="B51" s="18" t="s">
+        <v>483</v>
       </c>
       <c r="C51">
         <v>16</v>
@@ -7311,8 +7317,8 @@
       <c r="A52" s="1">
         <v>69</v>
       </c>
-      <c r="B52" t="s">
-        <v>461</v>
+      <c r="B52" s="18" t="s">
+        <v>483</v>
       </c>
       <c r="C52">
         <v>14</v>
@@ -7334,8 +7340,8 @@
       <c r="A53" s="1">
         <v>70</v>
       </c>
-      <c r="B53" t="s">
-        <v>461</v>
+      <c r="B53" s="18" t="s">
+        <v>483</v>
       </c>
       <c r="C53">
         <v>12</v>
@@ -7357,8 +7363,8 @@
       <c r="A54" s="1">
         <v>71</v>
       </c>
-      <c r="B54" t="s">
-        <v>461</v>
+      <c r="B54" s="18" t="s">
+        <v>483</v>
       </c>
       <c r="C54">
         <v>10</v>
@@ -7380,8 +7386,8 @@
       <c r="A55" s="1">
         <v>72</v>
       </c>
-      <c r="B55" t="s">
-        <v>461</v>
+      <c r="B55" s="18" t="s">
+        <v>483</v>
       </c>
       <c r="C55">
         <v>8</v>
@@ -7403,8 +7409,8 @@
       <c r="A56" s="1">
         <v>73</v>
       </c>
-      <c r="B56" t="s">
-        <v>461</v>
+      <c r="B56" s="18" t="s">
+        <v>483</v>
       </c>
       <c r="C56">
         <v>6</v>
@@ -7426,8 +7432,8 @@
       <c r="A57" s="1">
         <v>74</v>
       </c>
-      <c r="B57" t="s">
-        <v>461</v>
+      <c r="B57" s="18" t="s">
+        <v>483</v>
       </c>
       <c r="C57">
         <v>4</v>
@@ -7445,12 +7451,35 @@
         <v>0</v>
       </c>
     </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="1">
+        <v>53</v>
+      </c>
+      <c r="B58" s="18" t="s">
+        <v>484</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="E58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>0.9</v>
+      </c>
+    </row>
     <row r="59" spans="1:7">
       <c r="A59" s="1">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B59" t="s">
-        <v>434</v>
+        <v>485</v>
       </c>
       <c r="C59">
         <v>1</v>
@@ -7465,29 +7494,6 @@
         <v>0</v>
       </c>
       <c r="G59">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="60" spans="1:7">
-      <c r="A60" s="1">
-        <v>54</v>
-      </c>
-      <c r="B60" t="s">
-        <v>6</v>
-      </c>
-      <c r="C60">
-        <v>1</v>
-      </c>
-      <c r="D60" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="E60" t="s">
-        <v>38</v>
-      </c>
-      <c r="F60">
-        <v>0</v>
-      </c>
-      <c r="G60">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
testing CM wit ungrouped pps
</commit_message>
<xml_diff>
--- a/data/Power_plants.xlsx
+++ b/data/Power_plants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD68B889-25D5-44A2-853A-9F012853B03D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE04EE0F-CA71-4DD9-8415-11AF1B723FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="971" firstSheet="1" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="971" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="groupedNLGAS" sheetId="20" r:id="rId1"/>
@@ -21,51 +21,52 @@
     <sheet name="groupedDecarbNL_equilib2009" sheetId="36" r:id="rId6"/>
     <sheet name="S2_2015_50retro" sheetId="38" r:id="rId7"/>
     <sheet name="S1_2015_50retro" sheetId="37" r:id="rId8"/>
-    <sheet name="superGroupedNL (2)" sheetId="41" r:id="rId9"/>
-    <sheet name="superGroupedNL" sheetId="15" r:id="rId10"/>
-    <sheet name="groupedDecarbonizedNL_S1" sheetId="40" r:id="rId11"/>
-    <sheet name="groupedDecarbonizedNL2" sheetId="39" r:id="rId12"/>
-    <sheet name="groupedDecarbonizedNL" sheetId="29" r:id="rId13"/>
-    <sheet name="futureDecarbonizedNL" sheetId="33" r:id="rId14"/>
-    <sheet name="DecarbonizedNL" sheetId="28" r:id="rId15"/>
-    <sheet name="AnalysisforNiPlants" sheetId="21" r:id="rId16"/>
-    <sheet name="groupedNLRES" sheetId="23" r:id="rId17"/>
-    <sheet name="NL_withplanneddecommissions" sheetId="26" r:id="rId18"/>
-    <sheet name="NL2010RES" sheetId="25" r:id="rId19"/>
-    <sheet name="Sheet1" sheetId="27" r:id="rId20"/>
-    <sheet name="groupedDecarbonizedFLEXNET" sheetId="24" r:id="rId21"/>
-    <sheet name="groupedNL" sheetId="16" r:id="rId22"/>
-    <sheet name="extendedDEmoreoptimal" sheetId="12" r:id="rId23"/>
-    <sheet name="extendedDE" sheetId="1" r:id="rId24"/>
-    <sheet name="powerplants_grouped_DE" sheetId="3" r:id="rId25"/>
-    <sheet name="germany2019" sheetId="5" r:id="rId26"/>
-    <sheet name="dutchGermanPlants2015_from_emla" sheetId="13" r:id="rId27"/>
+    <sheet name="groupedDecarbonizedNLCRMs" sheetId="42" r:id="rId9"/>
+    <sheet name="superGroupedNL (2)" sheetId="41" r:id="rId10"/>
+    <sheet name="superGroupedNL" sheetId="15" r:id="rId11"/>
+    <sheet name="groupedDecarbonizedNL_S1" sheetId="40" r:id="rId12"/>
+    <sheet name="groupedDecarbonizedNL2" sheetId="39" r:id="rId13"/>
+    <sheet name="groupedDecarbonizedNL" sheetId="29" r:id="rId14"/>
+    <sheet name="futureDecarbonizedNL" sheetId="33" r:id="rId15"/>
+    <sheet name="DecarbonizedNL" sheetId="28" r:id="rId16"/>
+    <sheet name="AnalysisforNiPlants" sheetId="21" r:id="rId17"/>
+    <sheet name="groupedNLRES" sheetId="23" r:id="rId18"/>
+    <sheet name="NL_withplanneddecommissions" sheetId="26" r:id="rId19"/>
+    <sheet name="NL2010RES" sheetId="25" r:id="rId20"/>
+    <sheet name="Sheet1" sheetId="27" r:id="rId21"/>
+    <sheet name="groupedDecarbonizedFLEXNET" sheetId="24" r:id="rId22"/>
+    <sheet name="groupedNL" sheetId="16" r:id="rId23"/>
+    <sheet name="extendedDEmoreoptimal" sheetId="12" r:id="rId24"/>
+    <sheet name="extendedDE" sheetId="1" r:id="rId25"/>
+    <sheet name="powerplants_grouped_DE" sheetId="3" r:id="rId26"/>
+    <sheet name="germany2019" sheetId="5" r:id="rId27"/>
+    <sheet name="dutchGermanPlants2015_from_emla" sheetId="13" r:id="rId28"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId28"/>
+    <externalReference r:id="rId29"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">AnalysisforNiPlants!$B$1:$D$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">DecarbonizedNL!$A$1:$H$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="26" hidden="1">dutchGermanPlants2015_from_emla!$A$1:$H$440</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">extendedDE!$B$1:$J$272</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">extendedDEmoreoptimal!$B$1:$J$193</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">AnalysisforNiPlants!$B$1:$D$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="15" hidden="1">DecarbonizedNL!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="27" hidden="1">dutchGermanPlants2015_from_emla!$A$1:$H$440</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="24" hidden="1">extendedDE!$B$1:$J$272</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">extendedDEmoreoptimal!$B$1:$J$193</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">extendedNL!$A$1:$J$51</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">groupedDecarbonizedFLEXNET!$A$1:$I$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">groupedNL!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">groupedDecarbonizedFLEXNET!$A$1:$I$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="22" hidden="1">groupedNL!$A$1:$J$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">groupedNLGAS!$A$1:$J$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">groupedNLRES!$A$1:$J$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">NL_withplanneddecommissions!$A$1:$K$190</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">superGroupedNL!$A$1:$H$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'superGroupedNL (2)'!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="17" hidden="1">groupedNLRES!$A$1:$J$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="18" hidden="1">NL_withplanneddecommissions!$A$1:$K$190</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">superGroupedNL!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'superGroupedNL (2)'!$A$1:$H$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId29"/>
-    <pivotCache cacheId="1" r:id="rId30"/>
-    <pivotCache cacheId="2" r:id="rId31"/>
-    <pivotCache cacheId="3" r:id="rId32"/>
-    <pivotCache cacheId="4" r:id="rId33"/>
+    <pivotCache cacheId="0" r:id="rId30"/>
+    <pivotCache cacheId="1" r:id="rId31"/>
+    <pivotCache cacheId="2" r:id="rId32"/>
+    <pivotCache cacheId="3" r:id="rId33"/>
+    <pivotCache cacheId="4" r:id="rId34"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -123,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5635" uniqueCount="493">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5760" uniqueCount="495">
   <si>
     <t>Technology</t>
   </si>
@@ -1603,6 +1604,12 @@
   <si>
     <t>hydrogen OCGT</t>
   </si>
+  <si>
+    <t>power plants for second paper</t>
+  </si>
+  <si>
+    <t>no nuclear</t>
+  </si>
 </sst>
 </file>
 
@@ -2908,7 +2915,7 @@
       <sheetName val="NewTechnologies"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
+      <sheetData sheetId="0" refreshError="1"/>
       <sheetData sheetId="1">
         <row r="2">
           <cell r="A2" t="str">
@@ -3071,38 +3078,38 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19"/>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-      <sheetData sheetId="27"/>
-      <sheetData sheetId="28"/>
-      <sheetData sheetId="29"/>
-      <sheetData sheetId="30"/>
-      <sheetData sheetId="31"/>
-      <sheetData sheetId="32"/>
-      <sheetData sheetId="33"/>
+      <sheetData sheetId="2" refreshError="1"/>
+      <sheetData sheetId="3" refreshError="1"/>
+      <sheetData sheetId="4" refreshError="1"/>
+      <sheetData sheetId="5" refreshError="1"/>
+      <sheetData sheetId="6" refreshError="1"/>
+      <sheetData sheetId="7" refreshError="1"/>
+      <sheetData sheetId="8" refreshError="1"/>
+      <sheetData sheetId="9" refreshError="1"/>
+      <sheetData sheetId="10" refreshError="1"/>
+      <sheetData sheetId="11" refreshError="1"/>
+      <sheetData sheetId="12" refreshError="1"/>
+      <sheetData sheetId="13" refreshError="1"/>
+      <sheetData sheetId="14" refreshError="1"/>
+      <sheetData sheetId="15" refreshError="1"/>
+      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="17" refreshError="1"/>
+      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="19" refreshError="1"/>
+      <sheetData sheetId="20" refreshError="1"/>
+      <sheetData sheetId="21" refreshError="1"/>
+      <sheetData sheetId="22" refreshError="1"/>
+      <sheetData sheetId="23" refreshError="1"/>
+      <sheetData sheetId="24" refreshError="1"/>
+      <sheetData sheetId="25" refreshError="1"/>
+      <sheetData sheetId="26" refreshError="1"/>
+      <sheetData sheetId="27" refreshError="1"/>
+      <sheetData sheetId="28" refreshError="1"/>
+      <sheetData sheetId="29" refreshError="1"/>
+      <sheetData sheetId="30" refreshError="1"/>
+      <sheetData sheetId="31" refreshError="1"/>
+      <sheetData sheetId="32" refreshError="1"/>
+      <sheetData sheetId="33" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7189,6 +7196,607 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DED1FE2-7ECD-489A-A2DC-38034E20E145}">
+  <sheetPr>
+    <tabColor rgb="FF0070C0"/>
+  </sheetPr>
+  <dimension ref="A1:M22"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="M25" sqref="M25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13">
+      <c r="A1" t="s">
+        <v>437</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="1"/>
+      <c r="M1" s="5"/>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>481</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <v>18000</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
+        <v>481</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+      <c r="D3">
+        <v>18000</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>481</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>18000</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>481</v>
+      </c>
+      <c r="C5">
+        <v>15</v>
+      </c>
+      <c r="D5">
+        <v>18000</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6" t="s">
+        <v>482</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6">
+        <v>13500</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13">
+      <c r="A7">
+        <v>11</v>
+      </c>
+      <c r="B7" t="s">
+        <v>482</v>
+      </c>
+      <c r="C7">
+        <v>13</v>
+      </c>
+      <c r="D7">
+        <v>13500</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13">
+      <c r="A8">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>482</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>13500</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>492</v>
+      </c>
+      <c r="C9">
+        <v>27</v>
+      </c>
+      <c r="D9">
+        <v>4500</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>492</v>
+      </c>
+      <c r="C10">
+        <v>25</v>
+      </c>
+      <c r="D10">
+        <v>4500</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11">
+        <v>15</v>
+      </c>
+      <c r="B11" t="s">
+        <v>492</v>
+      </c>
+      <c r="C11">
+        <v>23</v>
+      </c>
+      <c r="D11">
+        <v>4500</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12">
+        <v>16</v>
+      </c>
+      <c r="B12" t="s">
+        <v>492</v>
+      </c>
+      <c r="C12">
+        <v>21</v>
+      </c>
+      <c r="D12">
+        <v>4500</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
+        <v>492</v>
+      </c>
+      <c r="C13">
+        <v>19</v>
+      </c>
+      <c r="D13">
+        <v>4500</v>
+      </c>
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14">
+        <v>18</v>
+      </c>
+      <c r="B14" t="s">
+        <v>492</v>
+      </c>
+      <c r="C14">
+        <v>15</v>
+      </c>
+      <c r="D14">
+        <v>4500</v>
+      </c>
+      <c r="E14" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="A15">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>492</v>
+      </c>
+      <c r="C15">
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <v>4500</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13">
+      <c r="A16">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>492</v>
+      </c>
+      <c r="C16">
+        <v>11</v>
+      </c>
+      <c r="D16">
+        <v>4500</v>
+      </c>
+      <c r="E16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>486</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="D17">
+        <v>12000</v>
+      </c>
+      <c r="E17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>484</v>
+      </c>
+      <c r="C18">
+        <v>2</v>
+      </c>
+      <c r="D18">
+        <v>9000</v>
+      </c>
+      <c r="E18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18" t="s">
+        <v>39</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>484</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <v>9000</v>
+      </c>
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20">
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
+        <v>484</v>
+      </c>
+      <c r="C20">
+        <v>12</v>
+      </c>
+      <c r="D20">
+        <v>9000</v>
+      </c>
+      <c r="E20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="A21">
+        <v>25</v>
+      </c>
+      <c r="B21" t="s">
+        <v>484</v>
+      </c>
+      <c r="C21">
+        <v>18</v>
+      </c>
+      <c r="D21">
+        <v>9000</v>
+      </c>
+      <c r="E21" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21" t="s">
+        <v>39</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>484</v>
+      </c>
+      <c r="C22">
+        <v>20</v>
+      </c>
+      <c r="D22">
+        <v>9000</v>
+      </c>
+      <c r="E22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22" t="s">
+        <v>39</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H1" xr:uid="{91B88372-FD70-4A88-9C48-DBF8E6D97E61}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H31">
+      <sortCondition ref="A1"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91B88372-FD70-4A88-9C48-DBF8E6D97E61}">
   <dimension ref="A1:M19"/>
   <sheetViews>
@@ -7664,7 +8272,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5DA2B207-E7EC-4D05-8789-9E26B69EE711}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -7672,7 +8280,7 @@
   <dimension ref="A1:P63"/>
   <sheetViews>
     <sheetView showRuler="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J50" sqref="J50"/>
+      <selection activeCell="B2" sqref="B2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9233,7 +9841,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2CDC36D9-AAB2-484A-A610-206E9EAD9091}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -10778,7 +11386,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8276941-6CB9-425B-B187-B06A7EEE7BC6}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -12281,7 +12889,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43471EED-B6C7-4F44-860D-1AE180707620}">
   <sheetPr>
     <tabColor rgb="FF00B050"/>
@@ -13117,7 +13725,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE12E6AE-0A69-4EFB-8C68-8C862108BAC1}">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
@@ -14908,7 +15516,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD4198A0-7CB3-4BB1-94E1-721EECB3BDAC}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -15132,7 +15740,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67609830-ACCB-49F0-B751-AE24D0F6CF61}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -16383,7 +16991,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB94089A-EE04-4A8F-A9CF-12445972E5C2}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -22879,7 +23487,35 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88C4D45E-47BE-4484-8166-1FE6AE7D2D6F}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="T39" sqref="T39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>468</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5DC26A1-8AAE-49C1-B239-84231B4324DA}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -24314,35 +24950,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88C4D45E-47BE-4484-8166-1FE6AE7D2D6F}">
-  <sheetPr>
-    <tabColor rgb="FFFFFF00"/>
-  </sheetPr>
-  <dimension ref="A1:A2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T39" sqref="T39"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:1">
-      <c r="A1" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
-      <c r="A2" t="s">
-        <v>468</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B60C3C6E-8400-4F42-A1F0-82CC35A1E938}">
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
@@ -24482,7 +25090,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85AAE1DC-B1F2-40C9-B131-9296BF39A7D3}">
   <sheetPr>
     <tabColor rgb="FF92D050"/>
@@ -25166,7 +25774,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCCA0DB4-82B5-4F45-9627-77778B586330}">
   <dimension ref="A1:K12"/>
   <sheetViews>
@@ -25609,7 +26217,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DF78530-F1D3-4B7A-B937-9D785DB65B2F}">
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J193"/>
@@ -31696,7 +32304,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M272"/>
   <sheetViews>
@@ -40461,7 +41069,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88DF7B89-3137-4483-A2A9-559F907A912A}">
   <dimension ref="A1:I34"/>
   <sheetViews>
@@ -41486,7 +42094,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{871B8469-CA4D-495B-9C72-1DE61BB7D586}">
   <dimension ref="A1:Z17"/>
   <sheetViews>
@@ -41938,7 +42546,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EE2FE5B-BFDE-4C21-9291-DDF53677D345}">
   <dimension ref="A1:I381"/>
   <sheetViews>
@@ -60476,22 +61084,32 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DED1FE2-7ECD-489A-A2DC-38034E20E145}">
-  <dimension ref="A1:M22"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38262F14-A446-4EBC-A910-A89BBAE801AB}">
+  <sheetPr>
+    <tabColor rgb="FF0070C0"/>
+  </sheetPr>
+  <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J38" sqref="J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" customWidth="1"/>
+    <col min="2" max="2" width="27.28515625" customWidth="1"/>
+    <col min="7" max="7" width="13.85546875" customWidth="1"/>
+    <col min="10" max="10" width="28.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
-        <v>437</v>
+        <v>446</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -60506,569 +61124,1396 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="I1" s="1"/>
-      <c r="M1" s="5"/>
-    </row>
-    <row r="2" spans="1:13">
-      <c r="A2">
-        <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>481</v>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" s="1">
+        <v>23</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>486</v>
       </c>
       <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>18000</v>
+        <v>20</v>
+      </c>
+      <c r="D2" s="4">
+        <v>2400</v>
       </c>
       <c r="E2" t="s">
         <v>38</v>
       </c>
-      <c r="F2" t="s">
-        <v>39</v>
+      <c r="F2">
+        <v>0</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3">
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" s="1">
+        <v>24</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="C3">
+        <v>16</v>
+      </c>
+      <c r="D3" s="4">
+        <v>2400</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="23"/>
+    </row>
+    <row r="4" spans="1:12" ht="16.149999999999999" customHeight="1">
+      <c r="A4" s="1">
+        <v>25</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4" s="4">
+        <v>2400</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="I4" s="23"/>
+      <c r="K4" s="4"/>
+    </row>
+    <row r="5" spans="1:12" ht="16.149999999999999" customHeight="1">
+      <c r="A5" s="1">
+        <v>26</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="C5">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>481</v>
-      </c>
-      <c r="C3">
-        <v>5</v>
-      </c>
-      <c r="D3">
-        <v>18000</v>
-      </c>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>481</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4">
-        <v>18000</v>
-      </c>
-      <c r="E4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>481</v>
-      </c>
-      <c r="C5">
-        <v>15</v>
-      </c>
-      <c r="D5">
-        <v>18000</v>
+      <c r="D5" s="4">
+        <v>2400</v>
       </c>
       <c r="E5" t="s">
         <v>38</v>
       </c>
-      <c r="F5" t="s">
-        <v>39</v>
+      <c r="F5">
+        <v>0</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6">
-        <v>10</v>
-      </c>
-      <c r="B6" t="s">
-        <v>482</v>
+      <c r="I5" s="23"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="4"/>
+    </row>
+    <row r="6" spans="1:12" ht="16.149999999999999" customHeight="1">
+      <c r="A6" s="1">
+        <v>27</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>486</v>
       </c>
       <c r="C6">
         <v>2</v>
       </c>
       <c r="D6">
-        <v>13500</v>
+        <v>2400</v>
       </c>
       <c r="E6" t="s">
         <v>38</v>
       </c>
-      <c r="F6" t="s">
-        <v>39</v>
+      <c r="F6">
+        <v>0</v>
       </c>
       <c r="G6">
         <v>0</v>
       </c>
-      <c r="H6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7">
-        <v>11</v>
-      </c>
-      <c r="B7" t="s">
-        <v>482</v>
+      <c r="I6" s="23"/>
+      <c r="J6" s="3"/>
+      <c r="K6" s="4"/>
+    </row>
+    <row r="7" spans="1:12" ht="16.149999999999999" customHeight="1">
+      <c r="A7" s="1">
+        <v>28</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>481</v>
       </c>
       <c r="C7">
-        <v>13</v>
+        <v>24</v>
       </c>
       <c r="D7">
-        <v>13500</v>
+        <v>1000</v>
       </c>
       <c r="E7" t="s">
         <v>38</v>
       </c>
-      <c r="F7" t="s">
-        <v>39</v>
+      <c r="F7">
+        <v>0</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8">
-        <v>12</v>
-      </c>
-      <c r="B8" t="s">
-        <v>482</v>
+      <c r="I7" s="23"/>
+      <c r="J7" s="3"/>
+      <c r="K7" s="4"/>
+    </row>
+    <row r="8" spans="1:12" ht="16.149999999999999" customHeight="1">
+      <c r="A8" s="1">
+        <v>29</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>481</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>23</v>
       </c>
       <c r="D8">
-        <v>13500</v>
+        <v>2500</v>
       </c>
       <c r="E8" t="s">
         <v>38</v>
       </c>
-      <c r="F8" t="s">
-        <v>39</v>
+      <c r="F8">
+        <v>0</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>492</v>
+      <c r="I8" s="23"/>
+      <c r="K8" s="4"/>
+    </row>
+    <row r="9" spans="1:12" ht="16.149999999999999" customHeight="1">
+      <c r="A9" s="1">
+        <v>30</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>481</v>
       </c>
       <c r="C9">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D9">
-        <v>4500</v>
+        <v>3000</v>
       </c>
       <c r="E9" t="s">
         <v>38</v>
       </c>
-      <c r="F9" t="s">
-        <v>39</v>
+      <c r="F9">
+        <v>0</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10">
-        <v>14</v>
-      </c>
-      <c r="B10" t="s">
-        <v>492</v>
+      <c r="I9" s="23"/>
+      <c r="J9" t="s">
+        <v>493</v>
+      </c>
+      <c r="K9" s="4"/>
+    </row>
+    <row r="10" spans="1:12" ht="16.149999999999999" customHeight="1">
+      <c r="A10" s="1">
+        <v>31</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>481</v>
       </c>
       <c r="C10">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="D10">
-        <v>4500</v>
+        <v>3000</v>
       </c>
       <c r="E10" t="s">
         <v>38</v>
       </c>
-      <c r="F10" t="s">
-        <v>39</v>
+      <c r="F10">
+        <v>0</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
-        <v>492</v>
+      <c r="I10" s="23"/>
+      <c r="J10" t="s">
+        <v>494</v>
+      </c>
+      <c r="K10" s="4"/>
+    </row>
+    <row r="11" spans="1:12" ht="16.149999999999999" customHeight="1">
+      <c r="A11" s="1">
+        <v>32</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>481</v>
       </c>
       <c r="C11">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D11">
-        <v>4500</v>
+        <v>3000</v>
       </c>
       <c r="E11" t="s">
         <v>38</v>
       </c>
-      <c r="F11" t="s">
-        <v>39</v>
+      <c r="F11">
+        <v>0</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12">
+      <c r="I11" s="23"/>
+      <c r="K11" s="4"/>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="1">
+        <v>33</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="C12">
+        <v>17</v>
+      </c>
+      <c r="D12">
+        <v>3000</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="I12" s="23"/>
+      <c r="K12" s="4"/>
+    </row>
+    <row r="13" spans="1:12" ht="13.9" customHeight="1">
+      <c r="A13" s="1">
+        <v>34</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="C13">
         <v>16</v>
       </c>
-      <c r="B12" t="s">
-        <v>492</v>
-      </c>
-      <c r="C12">
-        <v>21</v>
-      </c>
-      <c r="D12">
-        <v>4500</v>
-      </c>
-      <c r="E12" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13">
-        <v>17</v>
-      </c>
-      <c r="B13" t="s">
-        <v>492</v>
-      </c>
-      <c r="C13">
-        <v>19</v>
-      </c>
       <c r="D13">
-        <v>4500</v>
+        <v>3000</v>
       </c>
       <c r="E13" t="s">
         <v>38</v>
       </c>
-      <c r="F13" t="s">
-        <v>39</v>
+      <c r="F13">
+        <v>0</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
-      <c r="H13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14">
-        <v>18</v>
-      </c>
-      <c r="B14" t="s">
-        <v>492</v>
+      <c r="I13" s="23"/>
+      <c r="K13" s="4"/>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" s="1">
+        <v>35</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>481</v>
       </c>
       <c r="C14">
         <v>15</v>
       </c>
       <c r="D14">
-        <v>4500</v>
+        <v>3000</v>
       </c>
       <c r="E14" t="s">
         <v>38</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="I14" s="23"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" s="1">
+        <v>36</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
+      </c>
+      <c r="D15" s="4">
+        <v>3000</v>
+      </c>
+      <c r="E15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="I15" s="23"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" s="1">
+        <v>37</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="C16">
+        <v>13</v>
+      </c>
+      <c r="D16" s="4">
+        <v>3000</v>
+      </c>
+      <c r="E16" t="s">
+        <v>38</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="I16" s="23"/>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" s="1">
+        <v>38</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="C17">
+        <v>12</v>
+      </c>
+      <c r="D17" s="4">
+        <v>3000</v>
+      </c>
+      <c r="E17" t="s">
+        <v>38</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="I17" s="23"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" s="1">
         <v>39</v>
       </c>
-      <c r="G14">
-        <v>0</v>
-      </c>
-      <c r="H14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13">
-      <c r="A15">
-        <v>19</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="B18" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="C18">
+        <v>11</v>
+      </c>
+      <c r="D18" s="4">
+        <v>3500</v>
+      </c>
+      <c r="E18" t="s">
+        <v>38</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="I18" s="23"/>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" s="1">
+        <v>40</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19" s="4">
+        <v>3500</v>
+      </c>
+      <c r="E19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="I19" s="23"/>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" s="1">
+        <v>41</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="C20">
+        <v>9</v>
+      </c>
+      <c r="D20" s="4">
+        <v>3500</v>
+      </c>
+      <c r="E20" t="s">
+        <v>38</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" s="1">
+        <v>42</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="C21">
+        <v>8</v>
+      </c>
+      <c r="D21" s="4">
+        <v>3500</v>
+      </c>
+      <c r="E21" t="s">
+        <v>38</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12">
+      <c r="A22" s="1">
+        <v>43</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="C22">
+        <v>7</v>
+      </c>
+      <c r="D22" s="4">
+        <v>3500</v>
+      </c>
+      <c r="E22" t="s">
+        <v>38</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12">
+      <c r="A23" s="1">
+        <v>44</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="C23">
+        <v>6</v>
+      </c>
+      <c r="D23" s="4">
+        <v>3500</v>
+      </c>
+      <c r="E23" t="s">
+        <v>38</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12">
+      <c r="A24" s="1">
+        <v>45</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="C24">
+        <v>5</v>
+      </c>
+      <c r="D24" s="4">
+        <v>3500</v>
+      </c>
+      <c r="E24" t="s">
+        <v>38</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12">
+      <c r="A25" s="1">
+        <v>46</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="C25">
+        <v>4</v>
+      </c>
+      <c r="D25" s="4">
+        <v>3500</v>
+      </c>
+      <c r="E25" t="s">
+        <v>38</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12">
+      <c r="A26" s="1">
+        <v>47</v>
+      </c>
+      <c r="B26" t="s">
+        <v>481</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+      <c r="D26">
+        <v>3500</v>
+      </c>
+      <c r="E26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12">
+      <c r="A27" s="1">
+        <v>48</v>
+      </c>
+      <c r="B27" t="s">
+        <v>482</v>
+      </c>
+      <c r="C27">
+        <v>24</v>
+      </c>
+      <c r="D27">
+        <v>3000</v>
+      </c>
+      <c r="E27" t="s">
+        <v>38</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>0</v>
+      </c>
+      <c r="I27" s="23"/>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" s="1">
+        <v>49</v>
+      </c>
+      <c r="B28" t="s">
+        <v>482</v>
+      </c>
+      <c r="C28">
+        <v>22</v>
+      </c>
+      <c r="D28">
+        <v>3000</v>
+      </c>
+      <c r="E28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F28">
+        <v>0</v>
+      </c>
+      <c r="G28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" s="1">
+        <v>50</v>
+      </c>
+      <c r="B29" t="s">
+        <v>482</v>
+      </c>
+      <c r="C29">
+        <v>20</v>
+      </c>
+      <c r="D29">
+        <v>3000</v>
+      </c>
+      <c r="E29" t="s">
+        <v>38</v>
+      </c>
+      <c r="F29">
+        <v>0</v>
+      </c>
+      <c r="G29">
+        <v>0</v>
+      </c>
+      <c r="I29" s="23"/>
+    </row>
+    <row r="30" spans="1:12">
+      <c r="A30" s="1">
+        <v>51</v>
+      </c>
+      <c r="B30" t="s">
+        <v>482</v>
+      </c>
+      <c r="C30">
+        <v>18</v>
+      </c>
+      <c r="D30">
+        <v>3000</v>
+      </c>
+      <c r="E30" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30">
+        <v>0</v>
+      </c>
+      <c r="G30">
+        <v>0</v>
+      </c>
+      <c r="I30" s="23"/>
+    </row>
+    <row r="31" spans="1:12">
+      <c r="A31" s="1">
+        <v>52</v>
+      </c>
+      <c r="B31" t="s">
+        <v>482</v>
+      </c>
+      <c r="C31">
+        <v>16</v>
+      </c>
+      <c r="D31">
+        <v>3000</v>
+      </c>
+      <c r="E31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F31">
+        <v>0</v>
+      </c>
+      <c r="G31">
+        <v>0</v>
+      </c>
+      <c r="I31" s="23"/>
+    </row>
+    <row r="32" spans="1:12">
+      <c r="A32" s="1">
+        <v>53</v>
+      </c>
+      <c r="B32" t="s">
+        <v>482</v>
+      </c>
+      <c r="C32">
+        <v>14</v>
+      </c>
+      <c r="D32">
+        <v>3000</v>
+      </c>
+      <c r="E32" t="s">
+        <v>38</v>
+      </c>
+      <c r="F32">
+        <v>0</v>
+      </c>
+      <c r="G32">
+        <v>0</v>
+      </c>
+      <c r="I32" s="23"/>
+    </row>
+    <row r="33" spans="1:9">
+      <c r="A33" s="1">
+        <v>54</v>
+      </c>
+      <c r="B33" t="s">
+        <v>482</v>
+      </c>
+      <c r="C33">
+        <v>10</v>
+      </c>
+      <c r="D33">
+        <v>3000</v>
+      </c>
+      <c r="E33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F33">
+        <v>0</v>
+      </c>
+      <c r="G33">
+        <v>0</v>
+      </c>
+      <c r="I33" s="23"/>
+    </row>
+    <row r="34" spans="1:9">
+      <c r="A34" s="1">
+        <v>55</v>
+      </c>
+      <c r="B34" t="s">
+        <v>482</v>
+      </c>
+      <c r="C34">
+        <v>8</v>
+      </c>
+      <c r="D34">
+        <v>3000</v>
+      </c>
+      <c r="E34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F34">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="I34" s="23"/>
+    </row>
+    <row r="35" spans="1:9">
+      <c r="A35" s="1">
+        <v>56</v>
+      </c>
+      <c r="B35" t="s">
+        <v>482</v>
+      </c>
+      <c r="C35">
+        <v>6</v>
+      </c>
+      <c r="D35">
+        <v>4000</v>
+      </c>
+      <c r="E35" t="s">
+        <v>38</v>
+      </c>
+      <c r="F35">
+        <v>0</v>
+      </c>
+      <c r="G35">
+        <v>0</v>
+      </c>
+      <c r="I35" s="23"/>
+    </row>
+    <row r="36" spans="1:9">
+      <c r="A36" s="1">
+        <v>57</v>
+      </c>
+      <c r="B36" t="s">
+        <v>482</v>
+      </c>
+      <c r="C36">
+        <v>4</v>
+      </c>
+      <c r="D36">
+        <v>3000</v>
+      </c>
+      <c r="E36" t="s">
+        <v>38</v>
+      </c>
+      <c r="F36">
+        <v>0</v>
+      </c>
+      <c r="G36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9">
+      <c r="A37" s="1">
+        <v>58</v>
+      </c>
+      <c r="B37" t="s">
+        <v>482</v>
+      </c>
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>3000</v>
+      </c>
+      <c r="E37" t="s">
+        <v>38</v>
+      </c>
+      <c r="F37">
+        <v>0</v>
+      </c>
+      <c r="G37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9">
+      <c r="A38" s="1">
+        <v>59</v>
+      </c>
+      <c r="B38" t="s">
+        <v>482</v>
+      </c>
+      <c r="C38">
+        <v>2</v>
+      </c>
+      <c r="D38">
+        <v>3000</v>
+      </c>
+      <c r="E38" t="s">
+        <v>38</v>
+      </c>
+      <c r="F38">
+        <v>0</v>
+      </c>
+      <c r="G38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9">
+      <c r="A39" s="1">
+        <v>60</v>
+      </c>
+      <c r="B39" t="s">
         <v>492</v>
       </c>
-      <c r="C15">
-        <v>13</v>
-      </c>
-      <c r="D15">
-        <v>4500</v>
-      </c>
-      <c r="E15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F15" t="s">
-        <v>39</v>
-      </c>
-      <c r="G15">
-        <v>0</v>
-      </c>
-      <c r="H15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13">
-      <c r="A16">
+      <c r="C39">
+        <v>28</v>
+      </c>
+      <c r="D39">
+        <v>1500</v>
+      </c>
+      <c r="E39" t="s">
+        <v>38</v>
+      </c>
+      <c r="F39">
+        <v>0</v>
+      </c>
+      <c r="G39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9">
+      <c r="A40" s="1">
+        <v>61</v>
+      </c>
+      <c r="B40" t="s">
+        <v>492</v>
+      </c>
+      <c r="C40">
+        <v>26</v>
+      </c>
+      <c r="D40">
+        <v>1500</v>
+      </c>
+      <c r="E40" t="s">
+        <v>38</v>
+      </c>
+      <c r="F40">
+        <v>0</v>
+      </c>
+      <c r="G40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9">
+      <c r="A41" s="1">
+        <v>62</v>
+      </c>
+      <c r="B41" t="s">
+        <v>492</v>
+      </c>
+      <c r="C41">
+        <v>24</v>
+      </c>
+      <c r="D41">
+        <v>1500</v>
+      </c>
+      <c r="E41" t="s">
+        <v>38</v>
+      </c>
+      <c r="F41">
+        <v>0</v>
+      </c>
+      <c r="G41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9">
+      <c r="A42" s="1">
+        <v>63</v>
+      </c>
+      <c r="B42" t="s">
+        <v>492</v>
+      </c>
+      <c r="C42">
+        <v>22</v>
+      </c>
+      <c r="D42">
+        <v>1500</v>
+      </c>
+      <c r="E42" t="s">
+        <v>38</v>
+      </c>
+      <c r="F42">
+        <v>0</v>
+      </c>
+      <c r="G42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9">
+      <c r="A43" s="1">
+        <v>64</v>
+      </c>
+      <c r="B43" t="s">
+        <v>492</v>
+      </c>
+      <c r="C43">
         <v>20</v>
       </c>
-      <c r="B16" t="s">
+      <c r="D43">
+        <v>1500</v>
+      </c>
+      <c r="E43" t="s">
+        <v>38</v>
+      </c>
+      <c r="F43">
+        <v>0</v>
+      </c>
+      <c r="G43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9">
+      <c r="A44" s="1">
+        <v>65</v>
+      </c>
+      <c r="B44" t="s">
         <v>492</v>
       </c>
-      <c r="C16">
-        <v>11</v>
-      </c>
-      <c r="D16">
-        <v>4500</v>
-      </c>
-      <c r="E16" t="s">
-        <v>38</v>
-      </c>
-      <c r="F16" t="s">
-        <v>39</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17">
-        <v>21</v>
-      </c>
-      <c r="B17" t="s">
-        <v>486</v>
-      </c>
-      <c r="C17">
+      <c r="C44">
+        <v>18</v>
+      </c>
+      <c r="D44">
+        <v>1500</v>
+      </c>
+      <c r="E44" t="s">
+        <v>38</v>
+      </c>
+      <c r="F44">
+        <v>0</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9">
+      <c r="A45" s="1">
+        <v>66</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="C45">
+        <v>16</v>
+      </c>
+      <c r="D45" s="28">
+        <v>1500</v>
+      </c>
+      <c r="E45" t="s">
+        <v>38</v>
+      </c>
+      <c r="F45">
+        <v>0</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9">
+      <c r="A46" s="1">
+        <v>67</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="C46">
+        <v>14</v>
+      </c>
+      <c r="D46" s="28">
+        <v>1500</v>
+      </c>
+      <c r="E46" t="s">
+        <v>38</v>
+      </c>
+      <c r="F46">
+        <v>0</v>
+      </c>
+      <c r="G46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9">
+      <c r="A47" s="1">
+        <v>68</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="C47">
+        <v>12</v>
+      </c>
+      <c r="D47" s="28">
+        <v>1500</v>
+      </c>
+      <c r="E47" t="s">
+        <v>38</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9">
+      <c r="A48" s="1">
+        <v>69</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="C48">
+        <v>10</v>
+      </c>
+      <c r="D48" s="28">
+        <v>1500</v>
+      </c>
+      <c r="E48" t="s">
+        <v>38</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
+      <c r="A49" s="1">
+        <v>70</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="C49">
+        <v>8</v>
+      </c>
+      <c r="D49" s="28">
+        <v>1500</v>
+      </c>
+      <c r="E49" t="s">
+        <v>38</v>
+      </c>
+      <c r="F49">
+        <v>0</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
+      <c r="A50" s="1">
+        <v>71</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="C50">
+        <v>6</v>
+      </c>
+      <c r="D50" s="28">
+        <v>1500</v>
+      </c>
+      <c r="E50" t="s">
+        <v>38</v>
+      </c>
+      <c r="F50">
+        <v>0</v>
+      </c>
+      <c r="G50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
+      <c r="A51" s="1">
+        <v>72</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="C51">
+        <v>4</v>
+      </c>
+      <c r="D51" s="28">
+        <v>1500</v>
+      </c>
+      <c r="E51" t="s">
+        <v>38</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
+      <c r="A52" s="1">
+        <v>73</v>
+      </c>
+      <c r="B52" t="s">
+        <v>434</v>
+      </c>
+      <c r="C52">
+        <v>2</v>
+      </c>
+      <c r="D52" s="28">
+        <v>2000</v>
+      </c>
+      <c r="E52" t="s">
+        <v>38</v>
+      </c>
+      <c r="F52">
+        <v>0</v>
+      </c>
+      <c r="G52">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
+      <c r="A53" s="1">
+        <v>74</v>
+      </c>
+      <c r="B53" t="s">
+        <v>434</v>
+      </c>
+      <c r="C53">
+        <v>8</v>
+      </c>
+      <c r="D53" s="28">
+        <v>2000</v>
+      </c>
+      <c r="E53" t="s">
+        <v>38</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="12" customHeight="1">
+      <c r="A54" s="1">
+        <v>75</v>
+      </c>
+      <c r="B54" t="s">
+        <v>434</v>
+      </c>
+      <c r="C54">
+        <v>16</v>
+      </c>
+      <c r="D54" s="28">
+        <v>2000</v>
+      </c>
+      <c r="E54" t="s">
+        <v>38</v>
+      </c>
+      <c r="F54">
+        <v>0</v>
+      </c>
+      <c r="G54">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
+      <c r="A55" s="1">
+        <v>76</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C55">
+        <v>15</v>
+      </c>
+      <c r="D55" s="4">
+        <v>400</v>
+      </c>
+      <c r="E55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
+      <c r="A59" s="1">
+        <v>78</v>
+      </c>
+      <c r="B59" t="s">
+        <v>434</v>
+      </c>
+      <c r="C59">
+        <v>10</v>
+      </c>
+      <c r="D59" s="28">
+        <v>4000</v>
+      </c>
+      <c r="E59" t="s">
+        <v>38</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
+      <c r="A60" s="1">
+        <v>79</v>
+      </c>
+      <c r="B60" t="s">
+        <v>434</v>
+      </c>
+      <c r="C60">
+        <v>14</v>
+      </c>
+      <c r="D60" s="28">
+        <v>4000</v>
+      </c>
+      <c r="E60" t="s">
+        <v>38</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
+      <c r="A61" s="1">
+        <v>80</v>
+      </c>
+      <c r="B61" t="s">
+        <v>434</v>
+      </c>
+      <c r="C61">
+        <v>18</v>
+      </c>
+      <c r="D61" s="28">
+        <v>4000</v>
+      </c>
+      <c r="E61" t="s">
+        <v>38</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
+      <c r="A62" s="1">
+        <v>54</v>
+      </c>
+      <c r="B62" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62">
         <v>1</v>
       </c>
-      <c r="D17">
-        <v>12000</v>
-      </c>
-      <c r="E17" t="s">
-        <v>38</v>
-      </c>
-      <c r="F17" t="s">
-        <v>39</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-      <c r="H17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8">
-      <c r="A18">
-        <v>22</v>
-      </c>
-      <c r="B18" t="s">
-        <v>484</v>
-      </c>
-      <c r="C18">
-        <v>2</v>
-      </c>
-      <c r="D18">
-        <v>9000</v>
-      </c>
-      <c r="E18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8">
-      <c r="A19">
-        <v>23</v>
-      </c>
-      <c r="B19" t="s">
-        <v>484</v>
-      </c>
-      <c r="C19">
-        <v>7</v>
-      </c>
-      <c r="D19">
-        <v>9000</v>
-      </c>
-      <c r="E19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20">
-        <v>24</v>
-      </c>
-      <c r="B20" t="s">
-        <v>484</v>
-      </c>
-      <c r="C20">
-        <v>12</v>
-      </c>
-      <c r="D20">
-        <v>9000</v>
-      </c>
-      <c r="E20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F20" t="s">
-        <v>39</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8">
-      <c r="A21">
-        <v>25</v>
-      </c>
-      <c r="B21" t="s">
-        <v>484</v>
-      </c>
-      <c r="C21">
-        <v>18</v>
-      </c>
-      <c r="D21">
-        <v>9000</v>
-      </c>
-      <c r="E21" t="s">
-        <v>38</v>
-      </c>
-      <c r="F21" t="s">
-        <v>39</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="H21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8">
-      <c r="A22">
-        <v>26</v>
-      </c>
-      <c r="B22" t="s">
-        <v>484</v>
-      </c>
-      <c r="C22">
-        <v>20</v>
-      </c>
-      <c r="D22">
-        <v>9000</v>
-      </c>
-      <c r="E22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F22" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
+      <c r="D62" s="28">
+        <v>0.5</v>
+      </c>
+      <c r="E62" t="s">
+        <v>38</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H1" xr:uid="{91B88372-FD70-4A88-9C48-DBF8E6D97E61}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H31">
-      <sortCondition ref="A1"/>
-    </sortState>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
not grouping dispatchable techs
</commit_message>
<xml_diff>
--- a/data/Power_plants.xlsx
+++ b/data/Power_plants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE04EE0F-CA71-4DD9-8415-11AF1B723FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{682A1D3D-651D-426C-85ED-DE074E5F4566}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="971" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="971" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="groupedNLGAS" sheetId="20" r:id="rId1"/>
@@ -67,6 +67,7 @@
     <pivotCache cacheId="2" r:id="rId32"/>
     <pivotCache cacheId="3" r:id="rId33"/>
     <pivotCache cacheId="4" r:id="rId34"/>
+    <pivotCache cacheId="5" r:id="rId35"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -124,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5760" uniqueCount="495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5785" uniqueCount="506">
   <si>
     <t>Technology</t>
   </si>
@@ -1609,6 +1610,39 @@
   </si>
   <si>
     <t>no nuclear</t>
+  </si>
+  <si>
+    <t>WindOn</t>
+  </si>
+  <si>
+    <t>WindOff</t>
+  </si>
+  <si>
+    <t>SunPV</t>
+  </si>
+  <si>
+    <t>Gas</t>
+  </si>
+  <si>
+    <t>0,00</t>
+  </si>
+  <si>
+    <t>H2 STEG new</t>
+  </si>
+  <si>
+    <t>Li-ion battery</t>
+  </si>
+  <si>
+    <t>Biomass</t>
+  </si>
+  <si>
+    <t>Biogas</t>
+  </si>
+  <si>
+    <t>Hydro conventional</t>
+  </si>
+  <si>
+    <t>RESE others</t>
   </si>
 </sst>
 </file>
@@ -3329,6 +3363,39 @@
     </cacheField>
     <cacheField name="Age" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="40"/>
+    </cacheField>
+    <cacheField name="Capacity" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.5" maxValue="4000"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ingrid Sanchez Jimenez" refreshedDate="45371.89120208333" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="62" xr:uid="{884F8BB3-C46E-4B47-9F1C-DF0C002AFF80}">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="B1:D1048576" sheet="groupedDecarbonizedNLCRMs"/>
+  </cacheSource>
+  <cacheFields count="3">
+    <cacheField name="Technology" numFmtId="0">
+      <sharedItems containsBlank="1" count="8">
+        <s v="Wind Onshore"/>
+        <s v="Solar PV large"/>
+        <s v="Wind Offshore"/>
+        <s v="hydrogen OCGT"/>
+        <s v="Lithium_ion_battery"/>
+        <s v="Nuclear"/>
+        <m/>
+        <s v="Biomass_CHP_wood_pellets_DH"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Age" numFmtId="0">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="28"/>
     </cacheField>
     <cacheField name="Capacity" numFmtId="0">
       <sharedItems containsString="0" containsBlank="1" containsNumber="1" minValue="0.5" maxValue="4000"/>
@@ -5663,6 +5730,321 @@
 </pivotCacheRecords>
 </file>
 
+<file path=xl/pivotCache/pivotCacheRecords6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="62">
+  <r>
+    <x v="0"/>
+    <n v="20"/>
+    <n v="2400"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="16"/>
+    <n v="2400"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="12"/>
+    <n v="2400"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="7"/>
+    <n v="2400"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="2"/>
+    <n v="2400"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="24"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="23"/>
+    <n v="2500"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="21"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="19"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="18"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="17"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="16"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="15"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="14"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="13"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="12"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="11"/>
+    <n v="3500"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="10"/>
+    <n v="3500"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="9"/>
+    <n v="3500"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="8"/>
+    <n v="3500"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="7"/>
+    <n v="3500"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="6"/>
+    <n v="3500"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="5"/>
+    <n v="3500"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="4"/>
+    <n v="3500"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="3"/>
+    <n v="3500"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="24"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="22"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="20"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="18"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="16"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="14"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="10"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="8"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="6"/>
+    <n v="4000"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="4"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="3"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="2"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="28"/>
+    <n v="1500"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="26"/>
+    <n v="1500"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="24"/>
+    <n v="1500"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="22"/>
+    <n v="1500"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="20"/>
+    <n v="1500"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="18"/>
+    <n v="1500"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="16"/>
+    <n v="1500"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="14"/>
+    <n v="1500"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="12"/>
+    <n v="1500"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="10"/>
+    <n v="1500"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="8"/>
+    <n v="1500"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="6"/>
+    <n v="1500"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="4"/>
+    <n v="1500"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="2"/>
+    <n v="2000"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="8"/>
+    <n v="2000"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="16"/>
+    <n v="2000"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="15"/>
+    <n v="400"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="6"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="6"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="10"/>
+    <n v="4000"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="14"/>
+    <n v="4000"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="18"/>
+    <n v="4000"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="1"/>
+    <n v="0.5"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <m/>
+    <m/>
+  </r>
+</pivotCacheRecords>
+</file>
+
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8EBABEF3-7A12-4A97-8F01-EC0882F5F9E8}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="N1:O13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
@@ -5752,6 +6134,76 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{42B9EE56-CA82-4652-A089-20D343A6C0FE}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="M2:N11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="3">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="9">
+        <item x="7"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="0"/>
+        <item x="6"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Capacity" fld="2" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{10D1ECBC-A7C8-4A99-B4B2-F89CFCF70C3C}" name="PivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="O3:P13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
@@ -5825,7 +6277,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{44DB7B8B-0C79-4D4C-8E28-80C290F64FA5}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="K4:L11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
@@ -5891,7 +6343,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6BF26451-E31D-47E6-8F31-F8B5E9E2F19D}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="M2:N11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
@@ -5961,7 +6413,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{74BDB821-21CE-43E4-8468-DFB3CEBCE604}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
@@ -7203,7 +7655,7 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M25" sqref="M25"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -61088,10 +61540,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:L62"/>
+  <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J38" sqref="J38"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="A21" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M53" sqref="M53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -61101,13 +61553,12 @@
     <col min="10" max="10" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
         <v>446</v>
       </c>
@@ -61130,7 +61581,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:14">
       <c r="A2" s="1">
         <v>23</v>
       </c>
@@ -61152,8 +61603,14 @@
       <c r="G2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:12">
+      <c r="M2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="N2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
       <c r="A3" s="1">
         <v>24</v>
       </c>
@@ -61176,8 +61633,14 @@
         <v>0</v>
       </c>
       <c r="I3" s="23"/>
-    </row>
-    <row r="4" spans="1:12" ht="16.149999999999999" customHeight="1">
+      <c r="M3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="N3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="16.149999999999999" customHeight="1">
       <c r="A4" s="1">
         <v>25</v>
       </c>
@@ -61201,8 +61664,14 @@
       </c>
       <c r="I4" s="23"/>
       <c r="K4" s="4"/>
-    </row>
-    <row r="5" spans="1:12" ht="16.149999999999999" customHeight="1">
+      <c r="M4" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="N4">
+        <v>19500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="16.149999999999999" customHeight="1">
       <c r="A5" s="1">
         <v>26</v>
       </c>
@@ -61227,8 +61696,14 @@
       <c r="I5" s="23"/>
       <c r="J5" s="3"/>
       <c r="K5" s="4"/>
-    </row>
-    <row r="6" spans="1:12" ht="16.149999999999999" customHeight="1">
+      <c r="M5" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="N5">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="16.149999999999999" customHeight="1">
       <c r="A6" s="1">
         <v>27</v>
       </c>
@@ -61253,8 +61728,14 @@
       <c r="I6" s="23"/>
       <c r="J6" s="3"/>
       <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="1:12" ht="16.149999999999999" customHeight="1">
+      <c r="M6" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N6">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" ht="16.149999999999999" customHeight="1">
       <c r="A7" s="1">
         <v>28</v>
       </c>
@@ -61279,8 +61760,14 @@
       <c r="I7" s="23"/>
       <c r="J7" s="3"/>
       <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="1:12" ht="16.149999999999999" customHeight="1">
+      <c r="M7" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="N7">
+        <v>62000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="16.149999999999999" customHeight="1">
       <c r="A8" s="1">
         <v>29</v>
       </c>
@@ -61304,8 +61791,14 @@
       </c>
       <c r="I8" s="23"/>
       <c r="K8" s="4"/>
-    </row>
-    <row r="9" spans="1:12" ht="16.149999999999999" customHeight="1">
+      <c r="M8" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="N8">
+        <v>37000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="16.149999999999999" customHeight="1">
       <c r="A9" s="1">
         <v>30</v>
       </c>
@@ -61332,8 +61825,14 @@
         <v>493</v>
       </c>
       <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="1:12" ht="16.149999999999999" customHeight="1">
+      <c r="M9" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="N9">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="16.149999999999999" customHeight="1">
       <c r="A10" s="1">
         <v>31</v>
       </c>
@@ -61360,8 +61859,11 @@
         <v>494</v>
       </c>
       <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="1:12" ht="16.149999999999999" customHeight="1">
+      <c r="M10" s="3" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="16.149999999999999" customHeight="1">
       <c r="A11" s="1">
         <v>32</v>
       </c>
@@ -61385,8 +61887,14 @@
       </c>
       <c r="I11" s="23"/>
       <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="1:12">
+      <c r="M11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="N11">
+        <v>148900.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
       <c r="A12" s="1">
         <v>33</v>
       </c>
@@ -61411,7 +61919,7 @@
       <c r="I12" s="23"/>
       <c r="K12" s="4"/>
     </row>
-    <row r="13" spans="1:12" ht="13.9" customHeight="1">
+    <row r="13" spans="1:14" ht="13.9" customHeight="1">
       <c r="A13" s="1">
         <v>34</v>
       </c>
@@ -61436,7 +61944,7 @@
       <c r="I13" s="23"/>
       <c r="K13" s="4"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:14">
       <c r="A14" s="1">
         <v>35</v>
       </c>
@@ -61461,7 +61969,7 @@
       <c r="I14" s="23"/>
       <c r="L14" s="3"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:14">
       <c r="A15" s="1">
         <v>36</v>
       </c>
@@ -61484,9 +61992,18 @@
         <v>0</v>
       </c>
       <c r="I15" s="23"/>
-      <c r="L15" s="3"/>
-    </row>
-    <row r="16" spans="1:12">
+      <c r="J15" t="s">
+        <v>495</v>
+      </c>
+      <c r="K15">
+        <v>12</v>
+      </c>
+      <c r="L15" s="3">
+        <f>K15*1000</f>
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
       <c r="A16" s="1">
         <v>37</v>
       </c>
@@ -61509,9 +62026,22 @@
         <v>0</v>
       </c>
       <c r="I16" s="23"/>
-      <c r="L16" s="3"/>
-    </row>
-    <row r="17" spans="1:12">
+      <c r="J16" t="s">
+        <v>496</v>
+      </c>
+      <c r="K16">
+        <v>57</v>
+      </c>
+      <c r="L16" s="3">
+        <f t="shared" ref="L16:L25" si="0">K16*1000</f>
+        <v>57000</v>
+      </c>
+      <c r="M16">
+        <f>L16-GETPIVOTDATA("Capacity",$M$2,"Technology","Wind Offshore")</f>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13">
       <c r="A17" s="1">
         <v>38</v>
       </c>
@@ -61534,9 +62064,22 @@
         <v>0</v>
       </c>
       <c r="I17" s="23"/>
-      <c r="L17" s="3"/>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="J17" t="s">
+        <v>497</v>
+      </c>
+      <c r="K17">
+        <v>107</v>
+      </c>
+      <c r="L17" s="3">
+        <f t="shared" si="0"/>
+        <v>107000</v>
+      </c>
+      <c r="M17">
+        <f>L17-GETPIVOTDATA("Capacity",$M$2,"Technology","Solar PV large")</f>
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13">
       <c r="A18" s="1">
         <v>39</v>
       </c>
@@ -61559,8 +62102,18 @@
         <v>0</v>
       </c>
       <c r="I18" s="23"/>
-    </row>
-    <row r="19" spans="1:12">
+      <c r="J18" t="s">
+        <v>498</v>
+      </c>
+      <c r="K18" t="s">
+        <v>499</v>
+      </c>
+      <c r="L18" s="3" t="e">
+        <f t="shared" si="0"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13">
       <c r="A19" s="1">
         <v>40</v>
       </c>
@@ -61583,8 +62136,18 @@
         <v>0</v>
       </c>
       <c r="I19" s="23"/>
-    </row>
-    <row r="20" spans="1:12">
+      <c r="J19" t="s">
+        <v>12</v>
+      </c>
+      <c r="K19">
+        <v>0.48</v>
+      </c>
+      <c r="L19" s="3">
+        <f t="shared" si="0"/>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13">
       <c r="A20" s="1">
         <v>41</v>
       </c>
@@ -61606,8 +62169,22 @@
       <c r="G20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:12">
+      <c r="J20" t="s">
+        <v>500</v>
+      </c>
+      <c r="K20">
+        <v>8.4499999999999993</v>
+      </c>
+      <c r="L20" s="3">
+        <f t="shared" si="0"/>
+        <v>8450</v>
+      </c>
+      <c r="M20">
+        <f>L20-GETPIVOTDATA("Capacity",$M$2,"Technology","hydrogen OCGT")</f>
+        <v>-11050</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13">
       <c r="A21" s="1">
         <v>42</v>
       </c>
@@ -61629,8 +62206,22 @@
       <c r="G21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:12">
+      <c r="J21" t="s">
+        <v>501</v>
+      </c>
+      <c r="K21">
+        <v>26</v>
+      </c>
+      <c r="L21" s="3">
+        <f t="shared" si="0"/>
+        <v>26000</v>
+      </c>
+      <c r="M21">
+        <f>L21-GETPIVOTDATA("Capacity",$M$2,"Technology","Lithium_ion_battery")</f>
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13">
       <c r="A22" s="1">
         <v>43</v>
       </c>
@@ -61652,8 +62243,18 @@
       <c r="G22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:12">
+      <c r="J22" t="s">
+        <v>502</v>
+      </c>
+      <c r="K22">
+        <v>4.38</v>
+      </c>
+      <c r="L22" s="3">
+        <f t="shared" si="0"/>
+        <v>4380</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13">
       <c r="A23" s="1">
         <v>44</v>
       </c>
@@ -61675,8 +62276,18 @@
       <c r="G23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:12">
+      <c r="J23" t="s">
+        <v>503</v>
+      </c>
+      <c r="K23">
+        <v>1.58</v>
+      </c>
+      <c r="L23" s="3">
+        <f t="shared" si="0"/>
+        <v>1580</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13">
       <c r="A24" s="1">
         <v>45</v>
       </c>
@@ -61698,8 +62309,18 @@
       <c r="G24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:12">
+      <c r="J24" t="s">
+        <v>504</v>
+      </c>
+      <c r="K24">
+        <v>0.04</v>
+      </c>
+      <c r="L24" s="3">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13">
       <c r="A25" s="1">
         <v>46</v>
       </c>
@@ -61721,8 +62342,18 @@
       <c r="G25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:12">
+      <c r="J25" t="s">
+        <v>505</v>
+      </c>
+      <c r="K25">
+        <v>0.45</v>
+      </c>
+      <c r="L25" s="3">
+        <f t="shared" si="0"/>
+        <v>450</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13">
       <c r="A26" s="1">
         <v>47</v>
       </c>
@@ -61745,7 +62376,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:13">
       <c r="A27" s="1">
         <v>48</v>
       </c>
@@ -61769,7 +62400,7 @@
       </c>
       <c r="I27" s="23"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:13">
       <c r="A28" s="1">
         <v>49</v>
       </c>
@@ -61792,7 +62423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:13">
       <c r="A29" s="1">
         <v>50</v>
       </c>
@@ -61816,7 +62447,7 @@
       </c>
       <c r="I29" s="23"/>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:13">
       <c r="A30" s="1">
         <v>51</v>
       </c>
@@ -61840,7 +62471,7 @@
       </c>
       <c r="I30" s="23"/>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:13">
       <c r="A31" s="1">
         <v>52</v>
       </c>
@@ -61864,7 +62495,7 @@
       </c>
       <c r="I31" s="23"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:13">
       <c r="A32" s="1">
         <v>53</v>
       </c>
@@ -62037,7 +62668,7 @@
         <v>492</v>
       </c>
       <c r="C39">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D39">
         <v>1500</v>
@@ -62060,7 +62691,7 @@
         <v>492</v>
       </c>
       <c r="C40">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D40">
         <v>1500</v>
@@ -62083,7 +62714,7 @@
         <v>492</v>
       </c>
       <c r="C41">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="D41">
         <v>1500</v>
@@ -62106,7 +62737,7 @@
         <v>492</v>
       </c>
       <c r="C42">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="D42">
         <v>1500</v>
@@ -62129,7 +62760,7 @@
         <v>492</v>
       </c>
       <c r="C43">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="D43">
         <v>1500</v>
@@ -62152,7 +62783,7 @@
         <v>492</v>
       </c>
       <c r="C44">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="D44">
         <v>1500</v>
@@ -62175,7 +62806,7 @@
         <v>492</v>
       </c>
       <c r="C45">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D45" s="28">
         <v>1500</v>
@@ -62198,7 +62829,7 @@
         <v>492</v>
       </c>
       <c r="C46">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="D46" s="28">
         <v>1500</v>
@@ -62221,7 +62852,7 @@
         <v>492</v>
       </c>
       <c r="C47">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D47" s="28">
         <v>1500</v>
@@ -62244,7 +62875,7 @@
         <v>492</v>
       </c>
       <c r="C48">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D48" s="28">
         <v>1500</v>
@@ -62263,11 +62894,11 @@
       <c r="A49" s="1">
         <v>70</v>
       </c>
-      <c r="B49" s="3" t="s">
-        <v>492</v>
+      <c r="B49" t="s">
+        <v>484</v>
       </c>
       <c r="C49">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="D49" s="28">
         <v>1500</v>
@@ -62279,21 +62910,21 @@
         <v>0</v>
       </c>
       <c r="G49">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="A50" s="1">
         <v>71</v>
       </c>
-      <c r="B50" s="3" t="s">
-        <v>492</v>
+      <c r="B50" t="s">
+        <v>484</v>
       </c>
       <c r="C50">
         <v>6</v>
       </c>
       <c r="D50" s="28">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="E50" t="s">
         <v>38</v>
@@ -62302,21 +62933,21 @@
         <v>0</v>
       </c>
       <c r="G50">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="51" spans="1:7">
       <c r="A51" s="1">
         <v>72</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>492</v>
+      <c r="B51" t="s">
+        <v>484</v>
       </c>
       <c r="C51">
         <v>4</v>
       </c>
       <c r="D51" s="28">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="E51" t="s">
         <v>38</v>
@@ -62325,7 +62956,7 @@
         <v>0</v>
       </c>
       <c r="G51">
-        <v>0</v>
+        <v>0.9</v>
       </c>
     </row>
     <row r="52" spans="1:7">
@@ -62333,7 +62964,7 @@
         <v>73</v>
       </c>
       <c r="B52" t="s">
-        <v>434</v>
+        <v>484</v>
       </c>
       <c r="C52">
         <v>2</v>
@@ -62356,7 +62987,7 @@
         <v>74</v>
       </c>
       <c r="B53" t="s">
-        <v>434</v>
+        <v>484</v>
       </c>
       <c r="C53">
         <v>8</v>
@@ -62379,7 +63010,7 @@
         <v>75</v>
       </c>
       <c r="B54" t="s">
-        <v>434</v>
+        <v>484</v>
       </c>
       <c r="C54">
         <v>16</v>
@@ -62401,34 +63032,80 @@
       <c r="A55" s="1">
         <v>76</v>
       </c>
-      <c r="B55" s="3" t="s">
+      <c r="B55" t="s">
+        <v>484</v>
+      </c>
+      <c r="C55">
+        <v>10</v>
+      </c>
+      <c r="D55" s="28">
+        <v>2000</v>
+      </c>
+      <c r="E55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F55">
+        <v>0</v>
+      </c>
+      <c r="G55">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
+      <c r="A56" s="1">
+        <v>76</v>
+      </c>
+      <c r="B56" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C55">
+      <c r="C56">
         <v>15</v>
       </c>
-      <c r="D55" s="4">
+      <c r="D56" s="4">
         <v>400</v>
       </c>
-      <c r="E55" t="s">
-        <v>38</v>
-      </c>
-      <c r="F55">
-        <v>0</v>
-      </c>
-      <c r="G55">
-        <v>0</v>
+      <c r="E56" t="s">
+        <v>38</v>
+      </c>
+      <c r="F56">
+        <v>0</v>
+      </c>
+      <c r="G56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
+      <c r="A58" s="1">
+        <v>78</v>
+      </c>
+      <c r="B58" t="s">
+        <v>434</v>
+      </c>
+      <c r="C58">
+        <v>10</v>
+      </c>
+      <c r="D58" s="28">
+        <v>4000</v>
+      </c>
+      <c r="E58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>0.9</v>
       </c>
     </row>
     <row r="59" spans="1:7">
       <c r="A59" s="1">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B59" t="s">
         <v>434</v>
       </c>
       <c r="C59">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D59" s="28">
         <v>4000</v>
@@ -62445,13 +63122,13 @@
     </row>
     <row r="60" spans="1:7">
       <c r="A60" s="1">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B60" t="s">
         <v>434</v>
       </c>
       <c r="C60">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D60" s="28">
         <v>4000</v>
@@ -62468,16 +63145,16 @@
     </row>
     <row r="61" spans="1:7">
       <c r="A61" s="1">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="B61" t="s">
-        <v>434</v>
+        <v>6</v>
       </c>
       <c r="C61">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="D61" s="28">
-        <v>4000</v>
+        <v>0.5</v>
       </c>
       <c r="E61" t="s">
         <v>38</v>
@@ -62486,34 +63163,11 @@
         <v>0</v>
       </c>
       <c r="G61">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="62" spans="1:7">
-      <c r="A62" s="1">
-        <v>54</v>
-      </c>
-      <c r="B62" t="s">
-        <v>6</v>
-      </c>
-      <c r="C62">
-        <v>1</v>
-      </c>
-      <c r="D62" s="28">
-        <v>0.5</v>
-      </c>
-      <c r="E62" t="s">
-        <v>38</v>
-      </c>
-      <c r="F62">
-        <v>0</v>
-      </c>
-      <c r="G62">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
grouped pp and not plotting
</commit_message>
<xml_diff>
--- a/data/Power_plants.xlsx
+++ b/data/Power_plants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68951A2B-6141-4636-AE90-6242BCF98706}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F3CE916-3EDF-4D29-9D6F-23F2B6C926B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="971" firstSheet="4" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-30900" yWindow="12795" windowWidth="29040" windowHeight="17640" tabRatio="971" firstSheet="4" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="groupedNLGAS" sheetId="20" r:id="rId1"/>
@@ -70,8 +70,8 @@
     <pivotCache cacheId="2" r:id="rId33"/>
     <pivotCache cacheId="3" r:id="rId34"/>
     <pivotCache cacheId="4" r:id="rId35"/>
-    <pivotCache cacheId="5" r:id="rId36"/>
-    <pivotCache cacheId="6" r:id="rId37"/>
+    <pivotCache cacheId="10" r:id="rId36"/>
+    <pivotCache cacheId="14" r:id="rId37"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -129,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5936" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5928" uniqueCount="508">
   <si>
     <t>Technology</t>
   </si>
@@ -1835,7 +1835,7 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1891,6 +1891,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Calculation" xfId="2" builtinId="22"/>
@@ -3401,25 +3402,29 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ingrid Sanchez Jimenez" refreshedDate="45386.642498379631" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="16" xr:uid="{3DAADDF0-D4A0-4A0E-BC91-0115A55A44C6}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ingrid Sanchez Jimenez" refreshedDate="45449.42704386574" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="15" xr:uid="{3DAADDF0-D4A0-4A0E-BC91-0115A55A44C6}">
   <cacheSource type="worksheet">
     <worksheetSource ref="B1:D16" sheet="superGroupedNL (2)"/>
   </cacheSource>
   <cacheFields count="3">
     <cacheField name="Technology" numFmtId="0">
-      <sharedItems count="5">
+      <sharedItems containsBlank="1" count="9">
+        <s v="hydrogen OCGT"/>
+        <s v="Lithium ion battery 4"/>
         <s v="Solar PV large"/>
         <s v="Wind Offshore"/>
-        <s v="hydrogen OCGT"/>
         <s v="Wind Onshore"/>
-        <s v="Lithium ion battery"/>
+        <s v="Nuclear"/>
+        <s v="hydrogen CCGT"/>
+        <m/>
+        <s v="Lithium ion battery" u="1"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Age" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="3" maxValue="18"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="5" maxValue="8"/>
     </cacheField>
     <cacheField name="Capacity" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="4000" maxValue="16000"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="400" maxValue="70000"/>
     </cacheField>
   </cacheFields>
   <extLst>
@@ -3431,7 +3436,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ingrid Sanchez Jimenez" refreshedDate="45421.990643287034" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="61" xr:uid="{884F8BB3-C46E-4B47-9F1C-DF0C002AFF80}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Ingrid Sanchez Jimenez" refreshedDate="45449.427179166669" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="75" xr:uid="{884F8BB3-C46E-4B47-9F1C-DF0C002AFF80}">
   <cacheSource type="worksheet">
     <worksheetSource ref="B1:D1048576" sheet="groupedDecarbonizedNLCRMs"/>
   </cacheSource>
@@ -3440,7 +3445,6 @@
       <sharedItems containsBlank="1" count="12">
         <s v="hydrogen OCGT"/>
         <s v="hydrogen CCGT"/>
-        <s v="Lithium ion battery"/>
         <s v="Nuclear"/>
         <s v="Solar PV large"/>
         <s v="Wind Offshore"/>
@@ -3448,6 +3452,7 @@
         <s v="Biofuel"/>
         <s v="Lithium ion battery 4"/>
         <m/>
+        <s v="Lithium ion battery" u="1"/>
         <s v="Biomass_CHP_wood_pellets_DH" u="1"/>
         <s v="Lithium_ion_battery" u="1"/>
       </sharedItems>
@@ -5789,165 +5794,300 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="16">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="15">
   <r>
     <x v="0"/>
-    <n v="3"/>
-    <n v="16000"/>
+    <n v="5"/>
+    <n v="5000"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="6"/>
+    <n v="5000"/>
   </r>
   <r>
     <x v="0"/>
     <n v="7"/>
-    <n v="16000"/>
+    <n v="4000"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="8"/>
+    <n v="4000"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="6"/>
+    <n v="4000"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <n v="5"/>
+    <n v="70000"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="5"/>
+    <n v="39000"/>
+  </r>
+  <r>
+    <x v="4"/>
+    <n v="5"/>
+    <n v="12000"/>
+  </r>
+  <r>
+    <x v="5"/>
+    <n v="8"/>
+    <n v="400"/>
+  </r>
+  <r>
+    <x v="6"/>
+    <n v="8"/>
+    <n v="2000"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="7"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="7"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="7"/>
+    <m/>
+    <m/>
+  </r>
+  <r>
+    <x v="7"/>
+    <m/>
+    <m/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="75">
+  <r>
+    <x v="0"/>
+    <n v="23"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="20"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="18"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="16"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="13"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="10"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="7"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="5"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="3"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <n v="2"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="22"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="19"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="17"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="15"/>
+    <n v="1000"/>
   </r>
   <r>
     <x v="0"/>
     <n v="12"/>
-    <n v="16000"/>
+    <n v="1000"/>
   </r>
   <r>
     <x v="0"/>
-    <n v="17"/>
-    <n v="16000"/>
+    <n v="9"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="6"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="4"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <n v="2"/>
+    <n v="1000"/>
   </r>
   <r>
     <x v="1"/>
-    <n v="4"/>
-    <n v="13000"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="10"/>
-    <n v="13000"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="18"/>
-    <n v="13000"/>
+    <n v="1"/>
+    <n v="1000"/>
   </r>
   <r>
     <x v="2"/>
+    <n v="15"/>
+    <n v="400"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="22"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="23"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="21"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="19"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="18"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="17"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="16"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="15"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="14"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="13"/>
+    <n v="3000"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="12"/>
+    <n v="4000"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="11"/>
+    <n v="4000"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="10"/>
+    <n v="4000"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="9"/>
+    <n v="4000"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="8"/>
+    <n v="4000"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="7"/>
+    <n v="4000"/>
+  </r>
+  <r>
+    <x v="3"/>
+    <n v="6"/>
+    <n v="4000"/>
+  </r>
+  <r>
+    <x v="3"/>
     <n v="5"/>
     <n v="4000"/>
   </r>
   <r>
-    <x v="2"/>
-    <n v="7"/>
-    <n v="4000"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="9"/>
-    <n v="4000"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="11"/>
-    <n v="4000"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="13"/>
+    <x v="3"/>
+    <n v="4"/>
     <n v="4000"/>
   </r>
   <r>
     <x v="3"/>
     <n v="3"/>
-    <n v="12000"/>
+    <n v="4000"/>
   </r>
   <r>
     <x v="4"/>
-    <n v="6"/>
-    <n v="7000"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <n v="16"/>
-    <n v="7000"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <n v="10"/>
-    <n v="7000"/>
-  </r>
-</pivotCacheRecords>
-</file>
-
-<file path=xl/pivotCache/pivotCacheRecords7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="61">
-  <r>
-    <x v="0"/>
-    <n v="23"/>
-    <n v="2000"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <n v="20"/>
-    <n v="2000"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <n v="18"/>
-    <n v="2000"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <n v="16"/>
-    <n v="2000"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <n v="13"/>
-    <n v="2000"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <n v="10"/>
-    <n v="2000"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <n v="7"/>
-    <n v="2000"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <n v="5"/>
-    <n v="2000"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <n v="3"/>
-    <n v="2000"/>
-  </r>
-  <r>
-    <x v="1"/>
-    <n v="2"/>
-    <n v="2000"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="10"/>
-    <n v="2000"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <n v="1"/>
-    <n v="2000"/>
-  </r>
-  <r>
-    <x v="3"/>
-    <n v="15"/>
-    <n v="400"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <n v="22"/>
+    <n v="29"/>
     <n v="3000"/>
   </r>
   <r>
     <x v="4"/>
-    <n v="23"/>
+    <n v="26"/>
     <n v="3000"/>
   </r>
   <r>
@@ -5957,17 +6097,7 @@
   </r>
   <r>
     <x v="4"/>
-    <n v="19"/>
-    <n v="3000"/>
-  </r>
-  <r>
-    <x v="4"/>
     <n v="18"/>
-    <n v="3000"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <n v="17"/>
     <n v="3000"/>
   </r>
   <r>
@@ -5977,63 +6107,28 @@
   </r>
   <r>
     <x v="4"/>
-    <n v="15"/>
-    <n v="3000"/>
-  </r>
-  <r>
-    <x v="4"/>
     <n v="14"/>
     <n v="3000"/>
   </r>
   <r>
     <x v="4"/>
-    <n v="13"/>
+    <n v="10"/>
     <n v="3000"/>
   </r>
   <r>
     <x v="4"/>
-    <n v="12"/>
-    <n v="4000"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <n v="11"/>
-    <n v="4000"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <n v="10"/>
-    <n v="4000"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <n v="9"/>
-    <n v="4000"/>
-  </r>
-  <r>
-    <x v="4"/>
     <n v="8"/>
-    <n v="4000"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <n v="7"/>
-    <n v="4000"/>
+    <n v="3000"/>
   </r>
   <r>
     <x v="4"/>
     <n v="6"/>
-    <n v="4000"/>
-  </r>
-  <r>
-    <x v="4"/>
-    <n v="5"/>
-    <n v="4000"/>
+    <n v="3000"/>
   </r>
   <r>
     <x v="4"/>
     <n v="4"/>
-    <n v="4000"/>
+    <n v="3000"/>
   </r>
   <r>
     <x v="4"/>
@@ -6041,142 +6136,117 @@
     <n v="4000"/>
   </r>
   <r>
-    <x v="5"/>
-    <n v="29"/>
-    <n v="3000"/>
+    <x v="4"/>
+    <n v="2"/>
+    <n v="4000"/>
   </r>
   <r>
     <x v="5"/>
-    <n v="26"/>
-    <n v="3000"/>
+    <n v="27"/>
+    <n v="2400"/>
   </r>
   <r>
     <x v="5"/>
-    <n v="21"/>
-    <n v="3000"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <n v="18"/>
-    <n v="3000"/>
+    <n v="22"/>
+    <n v="2400"/>
   </r>
   <r>
     <x v="5"/>
     <n v="16"/>
-    <n v="3000"/>
+    <n v="2400"/>
   </r>
   <r>
     <x v="5"/>
-    <n v="14"/>
-    <n v="3000"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <n v="10"/>
-    <n v="3000"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <n v="8"/>
-    <n v="3000"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <n v="6"/>
-    <n v="3000"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <n v="4"/>
-    <n v="4000"/>
-  </r>
-  <r>
-    <x v="5"/>
-    <n v="3"/>
-    <n v="4000"/>
+    <n v="7"/>
+    <n v="2400"/>
   </r>
   <r>
     <x v="5"/>
     <n v="2"/>
-    <n v="4000"/>
-  </r>
-  <r>
-    <x v="6"/>
-    <n v="27"/>
     <n v="2400"/>
   </r>
   <r>
     <x v="6"/>
-    <n v="22"/>
-    <n v="2400"/>
+    <n v="1"/>
+    <n v="1"/>
   </r>
   <r>
-    <x v="6"/>
-    <n v="16"/>
-    <n v="2400"/>
+    <x v="7"/>
+    <n v="24"/>
+    <n v="1000"/>
   </r>
   <r>
-    <x v="6"/>
-    <n v="7"/>
-    <n v="2400"/>
+    <x v="7"/>
+    <n v="23"/>
+    <n v="1000"/>
   </r>
   <r>
-    <x v="6"/>
-    <n v="2"/>
-    <n v="2400"/>
+    <x v="7"/>
+    <n v="21"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="18"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="15"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="12"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="9"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="6"/>
+    <n v="1000"/>
+  </r>
+  <r>
+    <x v="7"/>
+    <n v="3"/>
+    <n v="1000"/>
   </r>
   <r>
     <x v="7"/>
     <n v="1"/>
-    <n v="1"/>
+    <n v="1000"/>
   </r>
   <r>
     <x v="8"/>
-    <n v="2"/>
-    <n v="1"/>
-  </r>
-  <r>
-    <x v="9"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="9"/>
+    <x v="8"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="9"/>
+    <x v="8"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="9"/>
+    <x v="8"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="9"/>
+    <x v="8"/>
     <m/>
     <m/>
   </r>
   <r>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="9"/>
-    <m/>
-    <m/>
-  </r>
-  <r>
-    <x v="9"/>
+    <x v="8"/>
     <m/>
     <m/>
   </r>
@@ -6272,23 +6342,23 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{42B9EE56-CA82-4652-A089-20D343A6C0FE}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="M2:N13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{42B9EE56-CA82-4652-A089-20D343A6C0FE}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="M2:N12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
       <items count="13">
         <item m="1" x="10"/>
         <item x="0"/>
         <item m="1" x="11"/>
+        <item x="2"/>
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
+        <item x="8"/>
+        <item m="1" x="9"/>
+        <item x="7"/>
+        <item x="1"/>
         <item x="6"/>
-        <item x="9"/>
-        <item x="2"/>
-        <item x="8"/>
-        <item x="1"/>
-        <item x="7"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -6298,7 +6368,7 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="11">
+  <rowItems count="10">
     <i>
       <x v="1"/>
     </i>
@@ -6316,9 +6386,6 @@
     </i>
     <i>
       <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
     </i>
     <i>
       <x v="9"/>
@@ -6352,23 +6419,23 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D1CCD9EA-0970-4B56-991F-5E17BA3890E2}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="M2:N13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D1CCD9EA-0970-4B56-991F-5E17BA3890E2}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="M2:N12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
       <items count="13">
         <item m="1" x="10"/>
         <item x="0"/>
         <item m="1" x="11"/>
+        <item x="2"/>
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
+        <item x="8"/>
+        <item m="1" x="9"/>
+        <item x="7"/>
+        <item x="1"/>
         <item x="6"/>
-        <item x="9"/>
-        <item x="2"/>
-        <item x="8"/>
-        <item x="1"/>
-        <item x="7"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -6378,7 +6445,7 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="11">
+  <rowItems count="10">
     <i>
       <x v="1"/>
     </i>
@@ -6396,9 +6463,6 @@
     </i>
     <i>
       <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
     </i>
     <i>
       <x v="9"/>
@@ -6432,16 +6496,20 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6921BF19-FF47-46A9-B714-2923E27A754D}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="L2:M8" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6921BF19-FF47-46A9-B714-2923E27A754D}" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="L2:M11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
-      <items count="6">
+      <items count="10">
+        <item x="0"/>
+        <item m="1" x="8"/>
         <item x="2"/>
+        <item x="3"/>
         <item x="4"/>
-        <item x="0"/>
         <item x="1"/>
-        <item x="3"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -6451,12 +6519,9 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="6">
+  <rowItems count="9">
     <i>
       <x/>
-    </i>
-    <i>
-      <x v="1"/>
     </i>
     <i>
       <x v="2"/>
@@ -6466,6 +6531,18 @@
     </i>
     <i>
       <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
     </i>
     <i t="grand">
       <x/>
@@ -8031,7 +8108,7 @@
       <c r="M3" s="3" t="s">
         <v>492</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="33">
         <v>18000</v>
       </c>
     </row>
@@ -8062,7 +8139,7 @@
       <c r="M4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="33">
         <v>400</v>
       </c>
     </row>
@@ -8094,7 +8171,7 @@
       <c r="M5" s="3" t="s">
         <v>481</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="33">
         <v>70000</v>
       </c>
     </row>
@@ -8126,8 +8203,8 @@
       <c r="M6" s="3" t="s">
         <v>482</v>
       </c>
-      <c r="N6">
-        <v>39000</v>
+      <c r="N6" s="33">
+        <v>38000</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="16.149999999999999" customHeight="1">
@@ -8158,7 +8235,7 @@
       <c r="M7" s="3" t="s">
         <v>486</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="33">
         <v>12000</v>
       </c>
     </row>
@@ -8189,6 +8266,7 @@
       <c r="M8" s="3" t="s">
         <v>487</v>
       </c>
+      <c r="N8" s="33"/>
     </row>
     <row r="9" spans="1:14" ht="16.149999999999999" customHeight="1">
       <c r="A9" s="1">
@@ -8218,10 +8296,10 @@
       </c>
       <c r="K9" s="4"/>
       <c r="M9" s="3" t="s">
-        <v>484</v>
-      </c>
-      <c r="N9">
-        <v>4000</v>
+        <v>506</v>
+      </c>
+      <c r="N9" s="33">
+        <v>10000</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="16.149999999999999" customHeight="1">
@@ -8252,10 +8330,10 @@
       </c>
       <c r="K10" s="4"/>
       <c r="M10" s="3" t="s">
-        <v>506</v>
-      </c>
-      <c r="N10">
-        <v>1</v>
+        <v>507</v>
+      </c>
+      <c r="N10" s="33">
+        <v>2000</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="16.149999999999999" customHeight="1">
@@ -8283,10 +8361,10 @@
       <c r="I11" s="23"/>
       <c r="K11" s="4"/>
       <c r="M11" s="3" t="s">
-        <v>507</v>
-      </c>
-      <c r="N11">
-        <v>2000</v>
+        <v>485</v>
+      </c>
+      <c r="N11" s="33">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -8314,10 +8392,10 @@
       <c r="I12" s="23"/>
       <c r="K12" s="4"/>
       <c r="M12" s="3" t="s">
-        <v>485</v>
-      </c>
-      <c r="N12">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="N12" s="33">
+        <v>150401</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="13.9" customHeight="1">
@@ -8344,12 +8422,6 @@
       </c>
       <c r="I13" s="23"/>
       <c r="K13" s="4"/>
-      <c r="M13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N13">
-        <v>145402</v>
-      </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="1">
@@ -8445,7 +8517,7 @@
       </c>
       <c r="M16">
         <f>L16-GETPIVOTDATA("Capacity",$M$2,"Technology","Wind Offshore")</f>
-        <v>18000</v>
+        <v>19000</v>
       </c>
     </row>
     <row r="17" spans="1:13">
@@ -9490,17 +9562,17 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="23.140625" customWidth="1"/>
     <col min="6" max="6" width="22.42578125" customWidth="1"/>
-    <col min="12" max="12" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -9592,12 +9664,12 @@
       <c r="L3" s="3" t="s">
         <v>492</v>
       </c>
-      <c r="M3">
-        <v>20000</v>
+      <c r="M3" s="33">
+        <v>18000</v>
       </c>
       <c r="N3">
         <f>GETPIVOTDATA("Capacity",$L$2,"Technology","hydrogen OCGT")*0.9</f>
-        <v>18000</v>
+        <v>16200</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -9626,14 +9698,14 @@
         <v>0</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>484</v>
-      </c>
-      <c r="M4">
-        <v>21000</v>
+        <v>481</v>
+      </c>
+      <c r="M4" s="33">
+        <v>70000</v>
       </c>
       <c r="N4">
         <f>GETPIVOTDATA("Capacity",$L$2,"Technology","hydrogen OCGT")*0.5</f>
-        <v>10000</v>
+        <v>9000</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -9662,14 +9734,14 @@
         <v>0</v>
       </c>
       <c r="L5" s="3" t="s">
-        <v>481</v>
-      </c>
-      <c r="M5">
-        <v>64000</v>
+        <v>482</v>
+      </c>
+      <c r="M5" s="33">
+        <v>39000</v>
       </c>
       <c r="N5">
         <f>GETPIVOTDATA("Capacity",$L$2,"Technology","hydrogen OCGT")*0.1</f>
-        <v>2000</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="6" spans="1:14">
@@ -9698,14 +9770,14 @@
         <v>0.9</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>482</v>
-      </c>
-      <c r="M6">
-        <v>39000</v>
+        <v>486</v>
+      </c>
+      <c r="M6" s="33">
+        <v>12000</v>
       </c>
       <c r="N6">
         <f>GETPIVOTDATA("Capacity",$L$2,"Technology","hydrogen OCGT")*0.13</f>
-        <v>2600</v>
+        <v>2340</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -9734,14 +9806,14 @@
         <v>0</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>486</v>
-      </c>
-      <c r="M7">
-        <v>12000</v>
+        <v>506</v>
+      </c>
+      <c r="M7" s="33">
+        <v>4000</v>
       </c>
       <c r="N7">
         <f>GETPIVOTDATA("Capacity",$L$2,"Technology","hydrogen OCGT")*0.9</f>
-        <v>18000</v>
+        <v>16200</v>
       </c>
     </row>
     <row r="8" spans="1:14">
@@ -9770,10 +9842,10 @@
         <v>0</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M8">
-        <v>156000</v>
+        <v>12</v>
+      </c>
+      <c r="M8" s="33">
+        <v>400</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -9801,9 +9873,15 @@
       <c r="H9">
         <v>0</v>
       </c>
+      <c r="L9" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="M9" s="33">
+        <v>2000</v>
+      </c>
       <c r="N9">
         <f>SUM(N3:N7)</f>
-        <v>50600</v>
+        <v>45540</v>
       </c>
     </row>
     <row r="10" spans="1:14">
@@ -9831,6 +9909,10 @@
       <c r="H10">
         <v>0</v>
       </c>
+      <c r="L10" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="M10" s="33"/>
     </row>
     <row r="11" spans="1:14">
       <c r="A11">
@@ -9857,120 +9939,94 @@
       <c r="H11">
         <v>0</v>
       </c>
+      <c r="L11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11" s="33">
+        <v>145400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>506</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>6000</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0.9</v>
+      </c>
     </row>
     <row r="16" spans="1:14">
       <c r="N16" s="3"/>
     </row>
-    <row r="17" spans="2:14">
+    <row r="17" spans="12:14">
       <c r="N17" s="3"/>
     </row>
-    <row r="18" spans="2:14">
-      <c r="B18" t="s">
-        <v>481</v>
-      </c>
-      <c r="C18">
-        <v>7</v>
-      </c>
-      <c r="D18">
-        <v>16000</v>
-      </c>
-      <c r="E18" t="s">
-        <v>38</v>
-      </c>
-      <c r="F18" t="s">
-        <v>39</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>0</v>
-      </c>
+    <row r="18" spans="12:14">
       <c r="N18" s="3"/>
     </row>
-    <row r="19" spans="2:14">
-      <c r="B19" t="s">
-        <v>481</v>
-      </c>
-      <c r="C19">
-        <v>12</v>
-      </c>
-      <c r="D19">
-        <v>16000</v>
-      </c>
-      <c r="E19" t="s">
-        <v>38</v>
-      </c>
-      <c r="F19" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0</v>
-      </c>
+    <row r="19" spans="12:14">
       <c r="N19" s="3"/>
     </row>
-    <row r="20" spans="2:14">
-      <c r="B20" t="s">
-        <v>481</v>
-      </c>
-      <c r="C20">
-        <v>14</v>
-      </c>
-      <c r="D20">
-        <v>16000</v>
-      </c>
-      <c r="E20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F20" t="s">
-        <v>39</v>
-      </c>
-      <c r="G20">
-        <v>0</v>
-      </c>
-      <c r="H20">
-        <v>0</v>
-      </c>
+    <row r="20" spans="12:14">
       <c r="N20" s="3"/>
     </row>
-    <row r="21" spans="2:14">
+    <row r="21" spans="12:14">
+      <c r="L21" s="3"/>
+      <c r="M21" s="33"/>
       <c r="N21" s="3"/>
     </row>
-    <row r="22" spans="2:14">
-      <c r="B22" t="s">
-        <v>482</v>
-      </c>
-      <c r="C22">
-        <v>10</v>
-      </c>
-      <c r="D22">
-        <v>13000</v>
-      </c>
-      <c r="E22" t="s">
-        <v>38</v>
-      </c>
-      <c r="F22" t="s">
-        <v>39</v>
-      </c>
-      <c r="G22">
-        <v>0</v>
-      </c>
-      <c r="H22">
-        <v>0</v>
-      </c>
+    <row r="22" spans="12:14">
+      <c r="L22" s="3"/>
+      <c r="M22" s="33"/>
       <c r="N22" s="3"/>
     </row>
-    <row r="23" spans="2:14">
+    <row r="23" spans="12:14">
+      <c r="L23" s="3"/>
+      <c r="M23" s="33"/>
       <c r="N23" s="3"/>
     </row>
-    <row r="24" spans="2:14">
+    <row r="24" spans="12:14">
+      <c r="L24" s="3"/>
+      <c r="M24" s="33"/>
       <c r="N24" s="3"/>
     </row>
-    <row r="25" spans="2:14">
+    <row r="25" spans="12:14">
+      <c r="L25" s="3"/>
+      <c r="M25" s="33"/>
       <c r="N25" s="3"/>
+    </row>
+    <row r="26" spans="12:14">
+      <c r="L26" s="3"/>
+      <c r="M26" s="33"/>
+    </row>
+    <row r="27" spans="12:14">
+      <c r="L27" s="3"/>
+      <c r="M27" s="33"/>
+    </row>
+    <row r="28" spans="12:14">
+      <c r="L28" s="3"/>
+      <c r="M28" s="33"/>
+    </row>
+    <row r="29" spans="12:14">
+      <c r="L29" s="3"/>
+      <c r="M29" s="33"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:H1" xr:uid="{91B88372-FD70-4A88-9C48-DBF8E6D97E61}">
@@ -63276,8 +63332,8 @@
   </sheetPr>
   <dimension ref="A1:N75"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A33" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E65" sqref="E65"/>
+    <sheetView showRuler="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3:N11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -63370,7 +63426,7 @@
       <c r="M3" s="3" t="s">
         <v>492</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="33">
         <v>18000</v>
       </c>
     </row>
@@ -63401,7 +63457,7 @@
       <c r="M4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="33">
         <v>400</v>
       </c>
     </row>
@@ -63433,7 +63489,7 @@
       <c r="M5" s="3" t="s">
         <v>481</v>
       </c>
-      <c r="N5">
+      <c r="N5" s="33">
         <v>70000</v>
       </c>
     </row>
@@ -63465,8 +63521,8 @@
       <c r="M6" s="3" t="s">
         <v>482</v>
       </c>
-      <c r="N6">
-        <v>39000</v>
+      <c r="N6" s="33">
+        <v>38000</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="16.149999999999999" customHeight="1">
@@ -63497,7 +63553,7 @@
       <c r="M7" s="3" t="s">
         <v>486</v>
       </c>
-      <c r="N7">
+      <c r="N7" s="33">
         <v>12000</v>
       </c>
     </row>
@@ -63528,6 +63584,7 @@
       <c r="M8" s="3" t="s">
         <v>487</v>
       </c>
+      <c r="N8" s="33"/>
     </row>
     <row r="9" spans="1:14" ht="16.149999999999999" customHeight="1">
       <c r="A9" s="1">
@@ -63557,10 +63614,10 @@
       </c>
       <c r="K9" s="4"/>
       <c r="M9" s="3" t="s">
-        <v>484</v>
-      </c>
-      <c r="N9">
-        <v>4000</v>
+        <v>506</v>
+      </c>
+      <c r="N9" s="33">
+        <v>10000</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="16.149999999999999" customHeight="1">
@@ -63591,10 +63648,10 @@
       </c>
       <c r="K10" s="4"/>
       <c r="M10" s="3" t="s">
-        <v>506</v>
-      </c>
-      <c r="N10">
-        <v>1</v>
+        <v>507</v>
+      </c>
+      <c r="N10" s="33">
+        <v>2000</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="16.149999999999999" customHeight="1">
@@ -63622,10 +63679,10 @@
       <c r="I11" s="23"/>
       <c r="K11" s="4"/>
       <c r="M11" s="3" t="s">
-        <v>507</v>
-      </c>
-      <c r="N11">
-        <v>2000</v>
+        <v>485</v>
+      </c>
+      <c r="N11" s="33">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:14">
@@ -63654,10 +63711,10 @@
       <c r="I12" s="23"/>
       <c r="K12" s="4"/>
       <c r="M12" s="3" t="s">
-        <v>485</v>
-      </c>
-      <c r="N12">
-        <v>1</v>
+        <v>21</v>
+      </c>
+      <c r="N12" s="33">
+        <v>150401</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="13.9" customHeight="1">
@@ -63685,12 +63742,6 @@
       </c>
       <c r="I13" s="23"/>
       <c r="K13" s="4"/>
-      <c r="M13" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N13">
-        <v>145402</v>
-      </c>
     </row>
     <row r="14" spans="1:14">
       <c r="A14" s="1">
@@ -63789,7 +63840,7 @@
       </c>
       <c r="M16">
         <f>L16-GETPIVOTDATA("Capacity",$M$2,"Technology","Wind Offshore")</f>
-        <v>18000</v>
+        <v>19000</v>
       </c>
     </row>
     <row r="17" spans="1:13">

</xml_diff>

<commit_message>
adding increasing electrolyzers demand
</commit_message>
<xml_diff>
--- a/data/Power_plants.xlsx
+++ b/data/Power_plants.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B12D7ADD-D999-4414-9201-4D11EA130E08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4F68464-4F8C-4749-8EC2-5AF4D9D8C0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21810" yWindow="17250" windowWidth="29040" windowHeight="17640" tabRatio="971" firstSheet="8" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-60" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="971" firstSheet="5" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="groupedNLGAS" sheetId="20" r:id="rId1"/>
@@ -22,10 +22,10 @@
     <sheet name="S2_2015_50retro" sheetId="38" r:id="rId7"/>
     <sheet name="S1_2015_50retro" sheetId="37" r:id="rId8"/>
     <sheet name="groupedDecarbonizedNLCRMs" sheetId="42" r:id="rId9"/>
-    <sheet name="groupedDecarbonizedNLCRMs ( (3)" sheetId="44" r:id="rId10"/>
-    <sheet name="groupedDecarbonizedNLCRMs (2)" sheetId="43" r:id="rId11"/>
-    <sheet name="superGroupedNL (2)" sheetId="41" r:id="rId12"/>
-    <sheet name="superGroupedNL" sheetId="15" r:id="rId13"/>
+    <sheet name="superGroupedNL (2)" sheetId="41" r:id="rId10"/>
+    <sheet name="groupedDecarbonizedNLCRMs ( (3)" sheetId="44" r:id="rId11"/>
+    <sheet name="groupedDecarbonizedNLCRMs (2)" sheetId="43" r:id="rId12"/>
+    <sheet name="superGroupedNL(distH2)" sheetId="15" r:id="rId13"/>
     <sheet name="groupedDecarbonizedNL_S1" sheetId="40" r:id="rId14"/>
     <sheet name="groupedDecarbonizedNL2" sheetId="39" r:id="rId15"/>
     <sheet name="groupedDecarbonizedNL" sheetId="29" r:id="rId16"/>
@@ -56,26 +56,26 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">extendedNL!$A$1:$J$51</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="23" hidden="1">groupedDecarbonizedFLEXNET!$A$1:$I$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">groupedDecarbonizedNLCRMs!$A$1:$G$75</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'groupedDecarbonizedNLCRMs ( (3)'!$A$1:$G$75</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'groupedDecarbonizedNLCRMs (2)'!$A$1:$G$51</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'groupedDecarbonizedNLCRMs ( (3)'!$A$1:$G$75</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'groupedDecarbonizedNLCRMs (2)'!$A$1:$G$51</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="24" hidden="1">groupedNL!$A$1:$J$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">groupedNLGAS!$A$1:$J$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="19" hidden="1">groupedNLRES!$A$1:$J$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="20" hidden="1">NL_withplanneddecommissions!$A$1:$K$190</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">superGroupedNL!$A$1:$H$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'superGroupedNL (2)'!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'superGroupedNL (2)'!$A$1:$H$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'superGroupedNL(distH2)'!$A$1:$H$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId32"/>
-    <pivotCache cacheId="1" r:id="rId33"/>
-    <pivotCache cacheId="2" r:id="rId34"/>
-    <pivotCache cacheId="3" r:id="rId35"/>
-    <pivotCache cacheId="4" r:id="rId36"/>
-    <pivotCache cacheId="5" r:id="rId37"/>
-    <pivotCache cacheId="6" r:id="rId38"/>
-    <pivotCache cacheId="7" r:id="rId39"/>
-    <pivotCache cacheId="8" r:id="rId40"/>
+    <pivotCache cacheId="9" r:id="rId32"/>
+    <pivotCache cacheId="10" r:id="rId33"/>
+    <pivotCache cacheId="11" r:id="rId34"/>
+    <pivotCache cacheId="12" r:id="rId35"/>
+    <pivotCache cacheId="13" r:id="rId36"/>
+    <pivotCache cacheId="14" r:id="rId37"/>
+    <pivotCache cacheId="15" r:id="rId38"/>
+    <pivotCache cacheId="16" r:id="rId39"/>
+    <pivotCache cacheId="17" r:id="rId40"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -133,7 +133,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6140" uniqueCount="509">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6143" uniqueCount="509">
   <si>
     <t>Technology</t>
   </si>
@@ -4049,6 +4049,7 @@
       <sheetName val="CapacitySubscriptionConsumer"/>
       <sheetName val="CS_subscribed"/>
       <sheetName val="LoadShedders"/>
+      <sheetName val="yearlyHydrogen"/>
       <sheetName val="LSyearly"/>
       <sheetName val="peakLoad"/>
       <sheetName val="Fuels"/>
@@ -4284,6 +4285,7 @@
       <sheetData sheetId="34"/>
       <sheetData sheetId="35"/>
       <sheetData sheetId="36"/>
+      <sheetData sheetId="37"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -13464,7 +13466,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8EBABEF3-7A12-4A97-8F01-EC0882F5F9E8}" name="PivotTable1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{8EBABEF3-7A12-4A97-8F01-EC0882F5F9E8}" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="N1:O13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="9">
     <pivotField axis="axisRow" showAll="0">
@@ -13552,7 +13554,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{74BDB821-21CE-43E4-8468-DFB3CEBCE604}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{74BDB821-21CE-43E4-8468-DFB3CEBCE604}" name="PivotTable2" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="10">
     <pivotField showAll="0"/>
@@ -13641,7 +13643,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E95E67B3-2599-4954-A361-7612626F384A}" name="PivotTable3" cacheId="7" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E95E67B3-2599-4954-A361-7612626F384A}" name="PivotTable3" cacheId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="J37:K51" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -13743,7 +13745,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{42B9EE56-CA82-4652-A089-20D343A6C0FE}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{42B9EE56-CA82-4652-A089-20D343A6C0FE}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="M2:N12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -13820,23 +13822,20 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E2DF3433-EF20-454D-8329-33CF8700EADF}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="M2:N12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6921BF19-FF47-46A9-B714-2923E27A754D}" name="PivotTable1" cacheId="17" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="L2:M11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
-      <items count="13">
-        <item m="1" x="10"/>
+      <items count="10">
+        <item x="0"/>
+        <item m="1" x="8"/>
         <item x="2"/>
-        <item m="1" x="11"/>
+        <item x="3"/>
         <item x="4"/>
+        <item x="1"/>
         <item x="5"/>
         <item x="6"/>
         <item x="7"/>
-        <item x="8"/>
-        <item m="1" x="9"/>
-        <item x="3"/>
-        <item x="1"/>
-        <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -13846,9 +13845,12 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="10">
+  <rowItems count="9">
     <i>
-      <x v="1"/>
+      <x/>
+    </i>
+    <i>
+      <x v="2"/>
     </i>
     <i>
       <x v="3"/>
@@ -13866,13 +13868,7 @@
       <x v="7"/>
     </i>
     <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i>
-      <x v="11"/>
+      <x v="8"/>
     </i>
     <i t="grand">
       <x/>
@@ -13897,7 +13893,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D1CCD9EA-0970-4B56-991F-5E17BA3890E2}" name="PivotTable1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E2DF3433-EF20-454D-8329-33CF8700EADF}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="M2:N12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -13974,20 +13970,23 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6921BF19-FF47-46A9-B714-2923E27A754D}" name="PivotTable1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="L2:M11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D1CCD9EA-0970-4B56-991F-5E17BA3890E2}" name="PivotTable1" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="M2:N12" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
-      <items count="10">
-        <item x="0"/>
-        <item m="1" x="8"/>
+      <items count="13">
+        <item m="1" x="10"/>
         <item x="2"/>
-        <item x="3"/>
+        <item m="1" x="11"/>
         <item x="4"/>
-        <item x="1"/>
         <item x="5"/>
         <item x="6"/>
         <item x="7"/>
+        <item x="8"/>
+        <item m="1" x="9"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item x="0"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -13997,12 +13996,9 @@
   <rowFields count="1">
     <field x="0"/>
   </rowFields>
-  <rowItems count="9">
+  <rowItems count="10">
     <i>
-      <x/>
-    </i>
-    <i>
-      <x v="2"/>
+      <x v="1"/>
     </i>
     <i>
       <x v="3"/>
@@ -14020,7 +14016,13 @@
       <x v="7"/>
     </i>
     <i>
-      <x v="8"/>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="11"/>
     </i>
     <i t="grand">
       <x/>
@@ -14045,7 +14047,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{10D1ECBC-A7C8-4A99-B4B2-F89CFCF70C3C}" name="PivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{10D1ECBC-A7C8-4A99-B4B2-F89CFCF70C3C}" name="PivotTable2" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="O3:P13" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -14119,7 +14121,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{44DB7B8B-0C79-4D4C-8E28-80C290F64FA5}" name="PivotTable1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{44DB7B8B-0C79-4D4C-8E28-80C290F64FA5}" name="PivotTable1" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="K4:L11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="7">
     <pivotField showAll="0"/>
@@ -14185,7 +14187,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6BF26451-E31D-47E6-8F31-F8B5E9E2F19D}" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{6BF26451-E31D-47E6-8F31-F8B5E9E2F19D}" name="PivotTable1" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="M2:N11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" showAll="0">
@@ -14255,7 +14257,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{571B6CC6-6461-474A-9FDB-17F5A6DE42F6}" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{571B6CC6-6461-474A-9FDB-17F5A6DE42F6}" name="PivotTable2" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="N8:O24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="11">
     <pivotField showAll="0"/>
@@ -15585,13 +15587,507 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBE5F2AB-36C9-45F1-BA2B-9CD5F5EA8A3B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DED1FE2-7ECD-489A-A2DC-38034E20E145}">
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
+  <dimension ref="A1:N29"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" customWidth="1"/>
+    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" t="s">
+        <v>437</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="I1" s="1"/>
+      <c r="M1" s="5"/>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>492</v>
+      </c>
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>4000</v>
+      </c>
+      <c r="E2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="M2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3">
+        <v>21</v>
+      </c>
+      <c r="B3" t="s">
+        <v>492</v>
+      </c>
+      <c r="C3">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>4000</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="M3">
+        <v>16000</v>
+      </c>
+      <c r="N3">
+        <f>GETPIVOTDATA("Capacity",$L$2,"Technology","hydrogen OCGT")*0.9</f>
+        <v>14400</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4">
+        <v>22</v>
+      </c>
+      <c r="B4" t="s">
+        <v>492</v>
+      </c>
+      <c r="C4">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>4000</v>
+      </c>
+      <c r="E4" t="s">
+        <v>38</v>
+      </c>
+      <c r="F4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>481</v>
+      </c>
+      <c r="M4">
+        <v>60000</v>
+      </c>
+      <c r="N4">
+        <f>GETPIVOTDATA("Capacity",$L$2,"Technology","hydrogen OCGT")*0.5</f>
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5">
+        <v>23</v>
+      </c>
+      <c r="B5" t="s">
+        <v>492</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <v>2000</v>
+      </c>
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="M5">
+        <v>39000</v>
+      </c>
+      <c r="N5">
+        <f>GETPIVOTDATA("Capacity",$L$2,"Technology","hydrogen OCGT")*0.1</f>
+        <v>1600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14">
+      <c r="A6">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>492</v>
+      </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>2000</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="M6">
+        <v>12000</v>
+      </c>
+      <c r="N6">
+        <f>GETPIVOTDATA("Capacity",$L$2,"Technology","hydrogen OCGT")*0.13</f>
+        <v>2080</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14">
+      <c r="A7">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>506</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>4000</v>
+      </c>
+      <c r="E7" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0.9</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>506</v>
+      </c>
+      <c r="M7">
+        <v>10000</v>
+      </c>
+      <c r="N7">
+        <f>GETPIVOTDATA("Capacity",$L$2,"Technology","hydrogen OCGT")*0.9</f>
+        <v>14400</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14">
+      <c r="A8">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>481</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8">
+        <v>70000</v>
+      </c>
+      <c r="E8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="M8">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9">
+        <v>27</v>
+      </c>
+      <c r="B9" t="s">
+        <v>482</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>38000</v>
+      </c>
+      <c r="E9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" t="s">
+        <v>39</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>507</v>
+      </c>
+      <c r="M9">
+        <v>2000</v>
+      </c>
+      <c r="N9">
+        <f>SUM(N3:N7)</f>
+        <v>40480</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>486</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>12000</v>
+      </c>
+      <c r="E10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11">
+        <v>29</v>
+      </c>
+      <c r="B11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11">
+        <v>8</v>
+      </c>
+      <c r="D11">
+        <v>400</v>
+      </c>
+      <c r="E11" t="s">
+        <v>38</v>
+      </c>
+      <c r="F11" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="L11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M11">
+        <v>139400</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12">
+        <v>30</v>
+      </c>
+      <c r="B12" t="s">
+        <v>507</v>
+      </c>
+      <c r="C12">
+        <v>8</v>
+      </c>
+      <c r="D12">
+        <v>2000</v>
+      </c>
+      <c r="E12" t="s">
+        <v>38</v>
+      </c>
+      <c r="F12" t="s">
+        <v>39</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13">
+        <v>31</v>
+      </c>
+      <c r="B13" t="s">
+        <v>506</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>6000</v>
+      </c>
+      <c r="E13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" t="s">
+        <v>39</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="N16" s="3"/>
+    </row>
+    <row r="17" spans="12:14">
+      <c r="N17" s="3"/>
+    </row>
+    <row r="18" spans="12:14">
+      <c r="N18" s="3"/>
+    </row>
+    <row r="19" spans="12:14">
+      <c r="N19" s="3"/>
+    </row>
+    <row r="20" spans="12:14">
+      <c r="N20" s="3"/>
+    </row>
+    <row r="21" spans="12:14">
+      <c r="L21" s="3"/>
+      <c r="N21" s="3"/>
+    </row>
+    <row r="22" spans="12:14">
+      <c r="L22" s="3"/>
+      <c r="N22" s="3"/>
+    </row>
+    <row r="23" spans="12:14">
+      <c r="L23" s="3"/>
+      <c r="N23" s="3"/>
+    </row>
+    <row r="24" spans="12:14">
+      <c r="L24" s="3"/>
+      <c r="N24" s="3"/>
+    </row>
+    <row r="25" spans="12:14">
+      <c r="L25" s="3"/>
+      <c r="N25" s="3"/>
+    </row>
+    <row r="26" spans="12:14">
+      <c r="L26" s="3"/>
+    </row>
+    <row r="27" spans="12:14">
+      <c r="L27" s="3"/>
+    </row>
+    <row r="28" spans="12:14">
+      <c r="L28" s="3"/>
+    </row>
+    <row r="29" spans="12:14">
+      <c r="L29" s="3"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:H1" xr:uid="{91B88372-FD70-4A88-9C48-DBF8E6D97E61}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H17">
+      <sortCondition ref="B1"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBE5F2AB-36C9-45F1-BA2B-9CD5F5EA8A3B}">
   <dimension ref="A1:O76"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A42" zoomScale="125" zoomScaleNormal="235" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A33" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -17620,11 +18116,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D14DEAE-C8BB-44BC-945C-749D779BED7E}">
   <dimension ref="A1:N61"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A18" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="L85" sqref="L85"/>
     </sheetView>
   </sheetViews>
@@ -19166,483 +19662,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DED1FE2-7ECD-489A-A2DC-38034E20E145}">
-  <sheetPr>
-    <tabColor rgb="FF0070C0"/>
-  </sheetPr>
-  <dimension ref="A1:N29"/>
-  <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
-    <col min="6" max="6" width="22.42578125" customWidth="1"/>
-    <col min="12" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.140625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" t="s">
-        <v>437</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" s="1"/>
-      <c r="M1" s="5"/>
-    </row>
-    <row r="2" spans="1:14">
-      <c r="A2">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>492</v>
-      </c>
-      <c r="C2">
-        <v>5</v>
-      </c>
-      <c r="D2">
-        <v>4000</v>
-      </c>
-      <c r="E2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G2">
-        <v>0</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14">
-      <c r="A3">
-        <v>21</v>
-      </c>
-      <c r="B3" t="s">
-        <v>492</v>
-      </c>
-      <c r="C3">
-        <v>6</v>
-      </c>
-      <c r="D3">
-        <v>4000</v>
-      </c>
-      <c r="E3" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" t="s">
-        <v>39</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="L3" s="3" t="s">
-        <v>492</v>
-      </c>
-      <c r="M3">
-        <v>16000</v>
-      </c>
-      <c r="N3">
-        <f>GETPIVOTDATA("Capacity",$L$2,"Technology","hydrogen OCGT")*0.9</f>
-        <v>14400</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14">
-      <c r="A4">
-        <v>22</v>
-      </c>
-      <c r="B4" t="s">
-        <v>492</v>
-      </c>
-      <c r="C4">
-        <v>7</v>
-      </c>
-      <c r="D4">
-        <v>4000</v>
-      </c>
-      <c r="E4" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" t="s">
-        <v>39</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>481</v>
-      </c>
-      <c r="M4">
-        <v>60000</v>
-      </c>
-      <c r="N4">
-        <f>GETPIVOTDATA("Capacity",$L$2,"Technology","hydrogen OCGT")*0.5</f>
-        <v>8000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14">
-      <c r="A5">
-        <v>23</v>
-      </c>
-      <c r="B5" t="s">
-        <v>492</v>
-      </c>
-      <c r="C5">
-        <v>8</v>
-      </c>
-      <c r="D5">
-        <v>4000</v>
-      </c>
-      <c r="E5" t="s">
-        <v>38</v>
-      </c>
-      <c r="F5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="L5" s="3" t="s">
-        <v>482</v>
-      </c>
-      <c r="M5">
-        <v>39000</v>
-      </c>
-      <c r="N5">
-        <f>GETPIVOTDATA("Capacity",$L$2,"Technology","hydrogen OCGT")*0.1</f>
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="A6">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>506</v>
-      </c>
-      <c r="C6">
-        <v>6</v>
-      </c>
-      <c r="D6">
-        <v>4000</v>
-      </c>
-      <c r="E6" t="s">
-        <v>38</v>
-      </c>
-      <c r="F6" t="s">
-        <v>39</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>0.9</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>486</v>
-      </c>
-      <c r="M6">
-        <v>12000</v>
-      </c>
-      <c r="N6">
-        <f>GETPIVOTDATA("Capacity",$L$2,"Technology","hydrogen OCGT")*0.13</f>
-        <v>2080</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14">
-      <c r="A7">
-        <v>25</v>
-      </c>
-      <c r="B7" t="s">
-        <v>481</v>
-      </c>
-      <c r="C7">
-        <v>5</v>
-      </c>
-      <c r="D7">
-        <v>70000</v>
-      </c>
-      <c r="E7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F7" t="s">
-        <v>39</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="L7" s="3" t="s">
-        <v>506</v>
-      </c>
-      <c r="M7">
-        <v>10000</v>
-      </c>
-      <c r="N7">
-        <f>GETPIVOTDATA("Capacity",$L$2,"Technology","hydrogen OCGT")*0.9</f>
-        <v>14400</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14">
-      <c r="A8">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>482</v>
-      </c>
-      <c r="C8">
-        <v>5</v>
-      </c>
-      <c r="D8">
-        <v>38000</v>
-      </c>
-      <c r="E8" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="L8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="M8">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14">
-      <c r="A9">
-        <v>27</v>
-      </c>
-      <c r="B9" t="s">
-        <v>486</v>
-      </c>
-      <c r="C9">
-        <v>5</v>
-      </c>
-      <c r="D9">
-        <v>12000</v>
-      </c>
-      <c r="E9" t="s">
-        <v>38</v>
-      </c>
-      <c r="F9" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="L9" s="3" t="s">
-        <v>507</v>
-      </c>
-      <c r="M9">
-        <v>2000</v>
-      </c>
-      <c r="N9">
-        <f>SUM(N3:N7)</f>
-        <v>40480</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14">
-      <c r="A10">
-        <v>28</v>
-      </c>
-      <c r="B10" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10">
-        <v>8</v>
-      </c>
-      <c r="D10">
-        <v>400</v>
-      </c>
-      <c r="E10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="L10" s="3" t="s">
-        <v>487</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14">
-      <c r="A11">
-        <v>29</v>
-      </c>
-      <c r="B11" t="s">
-        <v>507</v>
-      </c>
-      <c r="C11">
-        <v>8</v>
-      </c>
-      <c r="D11">
-        <v>2000</v>
-      </c>
-      <c r="E11" t="s">
-        <v>38</v>
-      </c>
-      <c r="F11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="M11">
-        <v>139400</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14">
-      <c r="A12">
-        <v>30</v>
-      </c>
-      <c r="B12" t="s">
-        <v>506</v>
-      </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12">
-        <v>6000</v>
-      </c>
-      <c r="E12" t="s">
-        <v>38</v>
-      </c>
-      <c r="F12" t="s">
-        <v>39</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="N16" s="3"/>
-    </row>
-    <row r="17" spans="12:14">
-      <c r="N17" s="3"/>
-    </row>
-    <row r="18" spans="12:14">
-      <c r="N18" s="3"/>
-    </row>
-    <row r="19" spans="12:14">
-      <c r="N19" s="3"/>
-    </row>
-    <row r="20" spans="12:14">
-      <c r="N20" s="3"/>
-    </row>
-    <row r="21" spans="12:14">
-      <c r="L21" s="3"/>
-      <c r="N21" s="3"/>
-    </row>
-    <row r="22" spans="12:14">
-      <c r="L22" s="3"/>
-      <c r="N22" s="3"/>
-    </row>
-    <row r="23" spans="12:14">
-      <c r="L23" s="3"/>
-      <c r="N23" s="3"/>
-    </row>
-    <row r="24" spans="12:14">
-      <c r="L24" s="3"/>
-      <c r="N24" s="3"/>
-    </row>
-    <row r="25" spans="12:14">
-      <c r="L25" s="3"/>
-      <c r="N25" s="3"/>
-    </row>
-    <row r="26" spans="12:14">
-      <c r="L26" s="3"/>
-    </row>
-    <row r="27" spans="12:14">
-      <c r="L27" s="3"/>
-    </row>
-    <row r="28" spans="12:14">
-      <c r="L28" s="3"/>
-    </row>
-    <row r="29" spans="12:14">
-      <c r="L29" s="3"/>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:H1" xr:uid="{91B88372-FD70-4A88-9C48-DBF8E6D97E61}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H17">
-      <sortCondition ref="B1"/>
-    </sortState>
-  </autoFilter>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91B88372-FD70-4A88-9C48-DBF8E6D97E61}">
   <dimension ref="A1:M19"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -19814,10 +19839,10 @@
         <v>11</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>483</v>
+        <v>492</v>
       </c>
       <c r="C7">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D7">
         <v>4500</v>
@@ -19840,10 +19865,10 @@
         <v>12</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>483</v>
+        <v>492</v>
       </c>
       <c r="C8">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D8">
         <v>4500</v>
@@ -19866,10 +19891,10 @@
         <v>13</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>483</v>
+        <v>492</v>
       </c>
       <c r="C9">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D9">
         <v>4500</v>
@@ -19892,10 +19917,10 @@
         <v>14</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>483</v>
+        <v>492</v>
       </c>
       <c r="C10">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D10">
         <v>4500</v>
@@ -19918,10 +19943,10 @@
         <v>15</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>483</v>
+        <v>492</v>
       </c>
       <c r="C11">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D11">
         <v>4500</v>
@@ -19944,10 +19969,10 @@
         <v>16</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>483</v>
+        <v>492</v>
       </c>
       <c r="C12">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D12">
         <v>4500</v>
@@ -19970,10 +19995,10 @@
         <v>17</v>
       </c>
       <c r="B13" s="18" t="s">
-        <v>483</v>
+        <v>492</v>
       </c>
       <c r="C13">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D13">
         <v>4500</v>
@@ -19996,10 +20021,10 @@
         <v>18</v>
       </c>
       <c r="B14" s="18" t="s">
-        <v>483</v>
+        <v>492</v>
       </c>
       <c r="C14">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D14">
         <v>4500</v>
@@ -54507,7 +54532,7 @@
   <dimension ref="A1:O51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -73132,7 +73157,7 @@
   </sheetPr>
   <dimension ref="A1:O76"/>
   <sheetViews>
-    <sheetView showRuler="0" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A45" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
adding a bit of batteries for df
</commit_message>
<xml_diff>
--- a/data/Power_plants.xlsx
+++ b/data/Power_plants.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\toolbox-amiris-emlab\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E28EA6C3-91CF-422C-BDA1-736F5873E4B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC114CA5-13FE-4EEF-88CF-1ADB81722D78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-9150" yWindow="-21710" windowWidth="38620" windowHeight="21220" tabRatio="971" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="971" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="groupedNLGAS" sheetId="20" r:id="rId1"/>
@@ -143,7 +143,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6374" uniqueCount="524">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6376" uniqueCount="524">
   <si>
     <t>number</t>
   </si>
@@ -15966,6 +15966,138 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5985B147-C338-4298-BB48-DAAD5DB81760}" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="R6:S17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="10">
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="11">
+        <item x="2"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="1"/>
+        <item x="9"/>
+        <item x="8"/>
+        <item x="5"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="44">
+        <item x="42"/>
+        <item x="41"/>
+        <item x="40"/>
+        <item x="39"/>
+        <item x="38"/>
+        <item x="37"/>
+        <item x="36"/>
+        <item x="35"/>
+        <item x="34"/>
+        <item x="33"/>
+        <item x="32"/>
+        <item x="31"/>
+        <item x="30"/>
+        <item x="29"/>
+        <item x="28"/>
+        <item x="27"/>
+        <item x="26"/>
+        <item x="25"/>
+        <item x="24"/>
+        <item x="23"/>
+        <item x="22"/>
+        <item x="21"/>
+        <item x="20"/>
+        <item x="19"/>
+        <item x="18"/>
+        <item x="17"/>
+        <item x="16"/>
+        <item x="15"/>
+        <item x="14"/>
+        <item x="13"/>
+        <item x="12"/>
+        <item x="11"/>
+        <item x="10"/>
+        <item x="9"/>
+        <item x="8"/>
+        <item x="7"/>
+        <item x="6"/>
+        <item x="5"/>
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="1"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Capacity" fld="3" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{571B6CC6-6461-474A-9FDB-17F5A6DE42F6}" name="PivotTable2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="N8:O21" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="11">
@@ -16141,7 +16273,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{79AD12EE-97D8-411B-9FF6-EFD7D6CF28B9}" name="PivotTable3" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="U6:V17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
@@ -16207,138 +16339,6 @@
   </colItems>
   <dataFields count="1">
     <dataField name="Sum of Capacity" fld="2" baseField="0" baseItem="0"/>
-  </dataFields>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{5985B147-C338-4298-BB48-DAAD5DB81760}" name="PivotTable1" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="R6:S17" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="10">
-    <pivotField showAll="0"/>
-    <pivotField axis="axisRow" showAll="0">
-      <items count="11">
-        <item x="2"/>
-        <item x="4"/>
-        <item x="0"/>
-        <item x="3"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="1"/>
-        <item x="9"/>
-        <item x="8"/>
-        <item x="5"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0">
-      <items count="44">
-        <item x="42"/>
-        <item x="41"/>
-        <item x="40"/>
-        <item x="39"/>
-        <item x="38"/>
-        <item x="37"/>
-        <item x="36"/>
-        <item x="35"/>
-        <item x="34"/>
-        <item x="33"/>
-        <item x="32"/>
-        <item x="31"/>
-        <item x="30"/>
-        <item x="29"/>
-        <item x="28"/>
-        <item x="27"/>
-        <item x="26"/>
-        <item x="25"/>
-        <item x="24"/>
-        <item x="23"/>
-        <item x="22"/>
-        <item x="21"/>
-        <item x="20"/>
-        <item x="19"/>
-        <item x="18"/>
-        <item x="17"/>
-        <item x="16"/>
-        <item x="15"/>
-        <item x="14"/>
-        <item x="13"/>
-        <item x="12"/>
-        <item x="11"/>
-        <item x="10"/>
-        <item x="9"/>
-        <item x="8"/>
-        <item x="7"/>
-        <item x="6"/>
-        <item x="5"/>
-        <item x="4"/>
-        <item x="3"/>
-        <item x="2"/>
-        <item x="1"/>
-        <item x="0"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="1"/>
-  </rowFields>
-  <rowItems count="11">
-    <i>
-      <x/>
-    </i>
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colItems count="1">
-    <i/>
-  </colItems>
-  <dataFields count="1">
-    <dataField name="Sum of Capacity" fld="3" baseField="0" baseItem="0"/>
   </dataFields>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
@@ -19028,7 +19028,7 @@
   </sheetPr>
   <dimension ref="A1:N64"/>
   <sheetViews>
-    <sheetView showRuler="0" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
+    <sheetView showRuler="0" topLeftCell="A43" zoomScale="64" zoomScaleNormal="64" workbookViewId="0">
       <selection activeCell="N55" sqref="N55"/>
     </sheetView>
   </sheetViews>
@@ -68309,10 +68309,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="A1:P67"/>
+  <dimension ref="A1:P68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="I71" sqref="I71"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="H69" sqref="H69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -70264,6 +70264,32 @@
       </c>
       <c r="K67" t="s">
         <v>523</v>
+      </c>
+    </row>
+    <row r="68" spans="1:11">
+      <c r="A68">
+        <v>88</v>
+      </c>
+      <c r="B68" t="s">
+        <v>86</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>10</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+      <c r="F68" t="s">
+        <v>12</v>
+      </c>
+      <c r="G68">
+        <v>0</v>
+      </c>
+      <c r="H68">
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>